<commit_message>
Auto commit - 01091828
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="542">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-08  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="605">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-09  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1555,6 +1555,31 @@
     <t>TM1、2發票機已更新版本</t>
   </si>
   <si>
+    <t>14196115010801</t>
+  </si>
+  <si>
+    <t>2026-01-08 08:31:06</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)螢幕很難觸控點很多下才有反應，協助嘗試執行觸控校正後，門市測試前幾分鐘操作是正常的，但不久又會開始感應遲鈍，店長告知幾乎每一筆都不好按，有時候客人較多也不好錄影，12/26工程師更換主機..請台芝到店協助
+(TM2(TCX800)螢幕很難觸控點很多下才有反應PS.1.昨天已有將門市提供錄影檔給台芝窗口2.20251226台芝有更換主機，無更換硬碟 換下8185000643 換上8185002948)</t>
+  </si>
+  <si>
+    <t>2026-01-08 09:23:44</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 13:23:00</t>
+  </si>
+  <si>
+    <t>換下8185002948.換上8185003706.備份還原.已請客服確認T M版本</t>
+  </si>
+  <si>
     <t>2026-01-08 10:12:04</t>
   </si>
   <si>
@@ -1612,6 +1637,36 @@
     <t>PMQ1+7210002871</t>
   </si>
   <si>
+    <t>E4191115010801</t>
+  </si>
+  <si>
+    <t>三重溪美店</t>
+  </si>
+  <si>
+    <t>2026-01-08 13:20:58</t>
+  </si>
+  <si>
+    <t>門市反應sc螢幕(LCD)不定時閃黑頻，已有重新拔插線路仍異常，ping1有通VNC畫面正常...請台芝到店協助(候場電腦會不停閃退 黑頻)</t>
+  </si>
+  <si>
+    <t>THILF04191</t>
+  </si>
+  <si>
+    <t>2026-01-08 13:27:06</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 17:27:00</t>
+  </si>
+  <si>
+    <t>更換vga線</t>
+  </si>
+  <si>
     <t>林口建安店</t>
   </si>
   <si>
@@ -1682,6 +1737,145 @@
   </si>
   <si>
     <t>2026-01-08 14:45:00</t>
+  </si>
+  <si>
+    <t>L551</t>
+  </si>
+  <si>
+    <t>林口顧家店</t>
+  </si>
+  <si>
+    <t>THILF0L551</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:14:29</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:13:00</t>
+  </si>
+  <si>
+    <t>林口童樂店</t>
+  </si>
+  <si>
+    <t>THILF04538</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:53:04</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-08 15:52:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002877</t>
+  </si>
+  <si>
+    <t>2026-01-08 16:17:56</t>
+  </si>
+  <si>
+    <t>裝潢撤店</t>
+  </si>
+  <si>
+    <t>2026-01-08 18:55:09</t>
+  </si>
+  <si>
+    <t>裝潢撤機</t>
+  </si>
+  <si>
+    <t>北縣泰富店</t>
+  </si>
+  <si>
+    <t>新北市泰山區</t>
+  </si>
+  <si>
+    <t>THILF03606</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:43:55</t>
+  </si>
+  <si>
+    <t>2026-01-09 09:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 10:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002884+L90</t>
+  </si>
+  <si>
+    <t>泰山新民店</t>
+  </si>
+  <si>
+    <t>THILF04656</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:44:52</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:29:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002885</t>
+  </si>
+  <si>
+    <t>14196115010902</t>
+  </si>
+  <si>
+    <t>2026-01-09 12:43:23</t>
+  </si>
+  <si>
+    <t>台芝來電TM1(TCX800)協助更換UPOS，請客服協助派工</t>
+  </si>
+  <si>
+    <t>2026-01-09 12:44:33</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 16:44:00</t>
+  </si>
+  <si>
+    <t>更換tm主機含硬碟有備份還原
+換上8185003712
+換下8185003689
+已請客服確認T M版本
+並告知王小姐更換硬碟注意事項</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:02:25</t>
+  </si>
+  <si>
+    <t>協助開車載貨</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:11:55</t>
+  </si>
+  <si>
+    <t>2026-01-09 14:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002795</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:53:19</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002793</t>
+  </si>
+  <si>
+    <t>2026-01-09 15:54:38</t>
   </si>
 </sst>
 </file>
@@ -2095,10 +2289,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK72"/>
+  <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC69" sqref="AC69"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7681,38 +7875,58 @@
         <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C65" s="7">
-        <v>2026011192</v>
-      </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
+        <v>2026011176</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F65" s="7">
-        <v>5451</v>
+        <v>4196</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>468</v>
+        <v>321</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="7"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="9"/>
+        <v>92</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K65" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N65" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>501</v>
+      </c>
       <c r="Q65" s="7" t="s">
-        <v>472</v>
+        <v>324</v>
       </c>
       <c r="R65" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S65" s="7" t="s">
-        <v>426</v>
+        <v>99</v>
       </c>
       <c r="T65" s="7">
         <v>1</v>
@@ -7721,35 +7935,37 @@
         <v>53</v>
       </c>
       <c r="V65" s="7" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="W65" s="7" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="X65" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="Y65" s="7"/>
+        <v>504</v>
+      </c>
+      <c r="Y65" s="7" t="s">
+        <v>505</v>
+      </c>
       <c r="Z65" s="7">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="AA65" s="7"/>
       <c r="AB65" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC65" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="AD65" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>506</v>
+      </c>
+      <c r="AD65" s="7"/>
       <c r="AE65" s="7"/>
       <c r="AF65" s="7"/>
       <c r="AG65" s="7"/>
       <c r="AH65" s="7"/>
       <c r="AI65" s="7"/>
       <c r="AJ65" s="7"/>
-      <c r="AK65" s="7"/>
+      <c r="AK65" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="66" spans="1:37">
       <c r="A66" s="3">
@@ -7759,15 +7975,15 @@
         <v>118</v>
       </c>
       <c r="C66" s="3">
-        <v>2026011213</v>
+        <v>2026011192</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="3" t="s">
-        <v>489</v>
+      <c r="F66" s="3">
+        <v>5451</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>352</v>
@@ -7781,7 +7997,7 @@
       <c r="O66" s="4"/>
       <c r="P66" s="10"/>
       <c r="Q66" s="3" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="R66" s="3" t="s">
         <v>51</v>
@@ -7796,24 +8012,24 @@
         <v>53</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="W66" s="3" t="s">
-        <v>495</v>
+        <v>508</v>
       </c>
       <c r="X66" s="3" t="s">
-        <v>496</v>
+        <v>509</v>
       </c>
       <c r="Y66" s="3"/>
       <c r="Z66" s="3">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AA66" s="3"/>
       <c r="AB66" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC66" s="10" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="AD66" s="3" t="s">
         <v>60</v>
@@ -7834,18 +8050,18 @@
         <v>118</v>
       </c>
       <c r="C67" s="7">
-        <v>2026011242</v>
+        <v>2026011213</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
-      <c r="F67" s="7">
-        <v>3878</v>
+      <c r="F67" s="7" t="s">
+        <v>489</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>506</v>
+        <v>352</v>
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -7856,13 +8072,13 @@
       <c r="O67" s="8"/>
       <c r="P67" s="9"/>
       <c r="Q67" s="7" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="R67" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S67" s="7" t="s">
-        <v>113</v>
+        <v>426</v>
       </c>
       <c r="T67" s="7">
         <v>1</v>
@@ -7871,24 +8087,24 @@
         <v>53</v>
       </c>
       <c r="V67" s="7" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="W67" s="7" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="X67" s="7" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Y67" s="7"/>
       <c r="Z67" s="7">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="AA67" s="7"/>
       <c r="AB67" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC67" s="9" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="AD67" s="7" t="s">
         <v>60</v>
@@ -7899,9 +8115,7 @@
       <c r="AH67" s="7"/>
       <c r="AI67" s="7"/>
       <c r="AJ67" s="7"/>
-      <c r="AK67" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AK67" s="7"/>
     </row>
     <row r="68" spans="1:37">
       <c r="A68" s="3">
@@ -7911,18 +8125,18 @@
         <v>118</v>
       </c>
       <c r="C68" s="3">
-        <v>2026011257</v>
+        <v>2026011242</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3">
-        <v>4057</v>
+        <v>3878</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
@@ -7933,7 +8147,7 @@
       <c r="O68" s="4"/>
       <c r="P68" s="10"/>
       <c r="Q68" s="3" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>51</v>
@@ -7948,24 +8162,24 @@
         <v>53</v>
       </c>
       <c r="V68" s="3" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="W68" s="3" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="X68" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="Y68" s="3"/>
       <c r="Z68" s="3">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="AA68" s="3"/>
       <c r="AB68" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC68" s="10" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="AD68" s="3" t="s">
         <v>60</v>
@@ -7988,18 +8202,18 @@
         <v>118</v>
       </c>
       <c r="C69" s="7">
-        <v>2026011263</v>
+        <v>2026011257</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7">
-        <v>4326</v>
+        <v>4057</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
@@ -8010,7 +8224,7 @@
       <c r="O69" s="8"/>
       <c r="P69" s="9"/>
       <c r="Q69" s="7" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="R69" s="7" t="s">
         <v>51</v>
@@ -8025,24 +8239,24 @@
         <v>53</v>
       </c>
       <c r="V69" s="7" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="W69" s="7" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="X69" s="7" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="Y69" s="7"/>
       <c r="Z69" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AA69" s="7"/>
       <c r="AB69" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC69" s="9" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="AD69" s="7" t="s">
         <v>60</v>
@@ -8062,38 +8276,58 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C70" s="3">
-        <v>2026011271</v>
-      </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+        <v>2026011262</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F70" s="3">
-        <v>4715</v>
+        <v>4191</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N70" s="3">
+        <v>2501</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>529</v>
+      </c>
       <c r="Q70" s="3" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="R70" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T70" s="3">
         <v>1</v>
@@ -8102,28 +8336,28 @@
         <v>53</v>
       </c>
       <c r="V70" s="3" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="W70" s="3" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="X70" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="Y70" s="3"/>
+        <v>533</v>
+      </c>
+      <c r="Y70" s="3" t="s">
+        <v>534</v>
+      </c>
       <c r="Z70" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA70" s="3"/>
       <c r="AB70" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC70" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="AD70" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>535</v>
+      </c>
+      <c r="AD70" s="3"/>
       <c r="AE70" s="3"/>
       <c r="AF70" s="3"/>
       <c r="AG70" s="3"/>
@@ -8142,18 +8376,18 @@
         <v>118</v>
       </c>
       <c r="C71" s="7">
-        <v>2026011281</v>
+        <v>2026011263</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7">
-        <v>4834</v>
+        <v>4326</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
@@ -8164,7 +8398,7 @@
       <c r="O71" s="8"/>
       <c r="P71" s="9"/>
       <c r="Q71" s="7" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="R71" s="7" t="s">
         <v>51</v>
@@ -8179,24 +8413,24 @@
         <v>53</v>
       </c>
       <c r="V71" s="7" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="W71" s="7" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="X71" s="7" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="Y71" s="7"/>
       <c r="Z71" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA71" s="7"/>
       <c r="AB71" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC71" s="9" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="AD71" s="7" t="s">
         <v>60</v>
@@ -8219,18 +8453,18 @@
         <v>118</v>
       </c>
       <c r="C72" s="3">
-        <v>2026011288</v>
+        <v>2026011271</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="3" t="s">
-        <v>536</v>
+      <c r="F72" s="3">
+        <v>4715</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
@@ -8239,9 +8473,9 @@
       <c r="M72" s="4"/>
       <c r="N72" s="3"/>
       <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
+      <c r="P72" s="10"/>
       <c r="Q72" s="3" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="R72" s="3" t="s">
         <v>51</v>
@@ -8256,24 +8490,24 @@
         <v>53</v>
       </c>
       <c r="V72" s="3" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="W72" s="3" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="X72" s="3" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="Y72" s="3"/>
       <c r="Z72" s="3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AA72" s="3"/>
       <c r="AB72" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC72" s="4" t="s">
-        <v>502</v>
+      <c r="AC72" s="10" t="s">
+        <v>547</v>
       </c>
       <c r="AD72" s="3" t="s">
         <v>60</v>
@@ -8285,6 +8519,1033 @@
       <c r="AI72" s="3"/>
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:37">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="7">
+        <v>2026011281</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7">
+        <v>4834</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="R73" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T73" s="7">
+        <v>1</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V73" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="W73" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="X73" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC73" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="AD73" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="7"/>
+      <c r="AG73" s="7"/>
+      <c r="AH73" s="7"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="7"/>
+      <c r="AK73" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" s="3">
+        <v>2026011288</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T74" s="3">
+        <v>1</v>
+      </c>
+      <c r="U74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V74" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="W74" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="X74" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC74" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD74" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="3"/>
+      <c r="AG74" s="3"/>
+      <c r="AH74" s="3"/>
+      <c r="AI74" s="3"/>
+      <c r="AJ74" s="3"/>
+      <c r="AK74" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" s="7">
+        <v>2026011295</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="R75" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T75" s="7">
+        <v>1</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="W75" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="X75" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC75" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD75" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7"/>
+      <c r="AK75" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2026011311</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3">
+        <v>4538</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T76" s="3">
+        <v>1</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V76" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="X76" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC76" s="10" t="s">
+        <v>571</v>
+      </c>
+      <c r="AD76" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3"/>
+      <c r="AK76" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2026011317</v>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7">
+        <v>2109</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R77" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T77" s="7">
+        <v>1</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V77" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="W77" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="X77" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC77" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="AD77" s="7"/>
+      <c r="AE77" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+      <c r="AK77" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="3">
+        <v>2026011361</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3">
+        <v>2109</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T78" s="3">
+        <v>1</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC78" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="AD78" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE78" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2026011399</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7">
+        <v>3606</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="R79" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T79" s="7">
+        <v>1</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V79" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="W79" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="X79" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC79" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD79" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
+      <c r="AI79" s="7"/>
+      <c r="AJ79" s="7"/>
+      <c r="AK79" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2026011400</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3">
+        <v>4656</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T80" s="3">
+        <v>1</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC80" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="AD80" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3"/>
+      <c r="AK80" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2026011408</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F81" s="7">
+        <v>4196</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I81" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K81" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L81" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M81" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N81" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O81" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="P81" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="Q81" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="R81" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T81" s="7">
+        <v>1</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="Y81" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="Z81" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC81" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="3">
+        <v>2026011437</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3">
+        <v>4196</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T82" s="3">
+        <v>1</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC82" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="AD82" s="3"/>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK82" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2026011438</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7">
+        <v>4196</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T83" s="7">
+        <v>1</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC83" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK83" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2026011459</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <v>4191</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T84" s="3">
+        <v>1</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="3"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="3"/>
+      <c r="AI84" s="3"/>
+      <c r="AJ84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK84" s="3"/>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2026011460</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7">
+        <v>4191</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="R85" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V85" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="X85" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC85" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="AD85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK85" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01121832
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$104</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="605">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-09  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="723">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-12  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1787,6 +1787,30 @@
     <t>裝潢撤機</t>
   </si>
   <si>
+    <t>13017115010901</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:13:17</t>
+  </si>
+  <si>
+    <t>門市反應TM2發票機（BSC10II）常常清帳未出帳條退瓶，僅印出一小截空白，客服查看發票機韌體版本非251118a，請台芝到店更新發票機韌體版本須為251118a，查看TM1發票機型號為BSC10II，韌體版本也非251118a，也請同步更新....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-09 11:15:39</t>
+  </si>
+  <si>
+    <t>2026-01-12 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 10:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 15:15:00</t>
+  </si>
+  <si>
+    <t>兩台發票機進行更新完成</t>
+  </si>
+  <si>
     <t>北縣泰富店</t>
   </si>
   <si>
@@ -1876,6 +1900,348 @@
   </si>
   <si>
     <t>2026-01-09 15:54:38</t>
+  </si>
+  <si>
+    <t>桃縣桃高二店</t>
+  </si>
+  <si>
+    <t>THILF05574</t>
+  </si>
+  <si>
+    <t>2026-01-09 18:27:55</t>
+  </si>
+  <si>
+    <t>2026-01-09 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-09 18:27:00</t>
+  </si>
+  <si>
+    <t>借機三台裝機完成</t>
+  </si>
+  <si>
+    <t>14210115011001</t>
+  </si>
+  <si>
+    <t>三重福華店</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:08:43</t>
+  </si>
+  <si>
+    <t>門市反應TM1發票機（BSC10II）常常發票僅印出一小截空白，客服查看發票機韌體版本非251118a，請台芝到店更新發票機韌體版本須為251118a，查看TM2發票機型號為BSC10II，韌體版本也非251118a，也請同步更新....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04210</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:11:29</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 13:00:00</t>
+  </si>
+  <si>
+    <t>更新發票機韌體版本須為251118a Tm1. Tm2</t>
+  </si>
+  <si>
+    <t>E2375115010901</t>
+  </si>
+  <si>
+    <t>2026-01-09 22:27:25</t>
+  </si>
+  <si>
+    <t>性質轉換-門市告知TM2 CCD掃描器(HC56II-TR)外觀破損，目前有亮燈有嗶聲，但刷讀條碼感應不良，要求協助更換...需請台芝到店協助(掃描器破裂機2/感應不良機1機2/錢盤隔板短少機1機2)</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:11:47</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 16:10:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119006293
+換上8119006499</t>
+  </si>
+  <si>
+    <t>12375115011001</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:12:01</t>
+  </si>
+  <si>
+    <t>性質轉換-門市TM1-CCD掃描器(HC56II-TR)感應不良，有亮燈有嗶聲，但刷讀所有條碼都不好刷，需求更換...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:13:38</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119006292
+換上8119006995</t>
+  </si>
+  <si>
+    <t>12375115011002</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:14:09</t>
+  </si>
+  <si>
+    <t>錢匣損壞</t>
+  </si>
+  <si>
+    <t>性質轉換-門市告知TM1(TCX800)錢盤隔板短少，抽屜顏色米白/鑰匙孔位置中間/無鑰匙孔編號...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:17:05</t>
+  </si>
+  <si>
+    <t>更換錢櫃
+換下81Z1001539
+換上81Z1003420</t>
+  </si>
+  <si>
+    <t>12375115011003</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:17:17</t>
+  </si>
+  <si>
+    <t>性質轉換-門市告知TM2(TCX800)錢盤隔板短少，抽屜顏色米白/鑰匙孔位置中間/無鑰匙孔編號...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-10 09:19:13</t>
+  </si>
+  <si>
+    <t>更換錢櫃
+換下81Z1001540
+換上81Z1003699</t>
+  </si>
+  <si>
+    <t>13770115011001</t>
+  </si>
+  <si>
+    <t>北縣西雲店</t>
+  </si>
+  <si>
+    <t>2026-01-10 13:44:51</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控不靈敏，要點很多次才有反應，已有執行校正仍異常...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03770</t>
+  </si>
+  <si>
+    <t>2026-01-10 13:45:41</t>
+  </si>
+  <si>
+    <t>2026-01-12 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 11:30:00</t>
+  </si>
+  <si>
+    <t>更換TM主機及客顯不含硬碟
+換下8185002290
+換上8185000523</t>
+  </si>
+  <si>
+    <t>13052115011001</t>
+  </si>
+  <si>
+    <t>新莊莊玲店</t>
+  </si>
+  <si>
+    <t>2026-01-10 15:53:17</t>
+  </si>
+  <si>
+    <t>螢幕聲音異常</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD)切換監視器沒聲音，廠商到店表示為SC問題，SC有一條線鬆脫無法旋緊，門市告知因現場線路繁亂無法確定是甚麼線...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03052</t>
+  </si>
+  <si>
+    <t>2026-01-10 15:56:40</t>
+  </si>
+  <si>
+    <t>2026-01-12 09:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重插音源線 </t>
+  </si>
+  <si>
+    <t>12201115011102</t>
+  </si>
+  <si>
+    <t>桃縣內溪店</t>
+  </si>
+  <si>
+    <t>2026-01-11 09:06:16</t>
+  </si>
+  <si>
+    <t>01/11 09:08啟動緊急叫修:門市反應SC(SHUTTLE6S)無法連線，PING1不通無法VNC，門市告知SC有正常開機畫面，已重啟SC仍異常，請門市查看hub 1port有插線有亮燈，重新拔插1port、解MAC後開放2port交叉測試仍ping1不通，...需請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳務做到01/10有印出報表，與通訊小晶確認有收到銷售</t>
+  </si>
+  <si>
+    <t>THILF02201</t>
+  </si>
+  <si>
+    <t>2026-01-11 09:11:19</t>
+  </si>
+  <si>
+    <t>2026-01-11 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-11 15:05:00</t>
+  </si>
+  <si>
+    <t>2026-01-11 15:11:00</t>
+  </si>
+  <si>
+    <t>系統損毀
+更換第一顆及第二顆硬碟不備份還原完成</t>
+  </si>
+  <si>
+    <t>2026-01-11 19:07:24</t>
+  </si>
+  <si>
+    <t>2026-01-11 18:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-11 19:00:00</t>
+  </si>
+  <si>
+    <t>協助撤機</t>
+  </si>
+  <si>
+    <t>2026-01-11 19:07:46</t>
+  </si>
+  <si>
+    <t>2026-01-11 19:06:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">借機三台撤店已完工 </t>
+  </si>
+  <si>
+    <t>1D174115011201</t>
+  </si>
+  <si>
+    <t>D174</t>
+  </si>
+  <si>
+    <t>新莊裕民店</t>
+  </si>
+  <si>
+    <t>2026-01-12 10:23:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市TM1(BSC10II)常常發生未出發票，僅印出一小截空白，查看發票機韌體版本為3.1，還請台芝到店更新發票機韌體，...還請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>THILF0D174</t>
+  </si>
+  <si>
+    <t>2026-01-12 10:24:47</t>
+  </si>
+  <si>
+    <t>2026-01-12 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:24:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 10:46:28</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003052+L90</t>
+  </si>
+  <si>
+    <t>2026-01-12 12:11:01</t>
+  </si>
+  <si>
+    <t>2026-01-12 12:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002831+L90</t>
+  </si>
+  <si>
+    <t>1D649115011201</t>
+  </si>
+  <si>
+    <t>D649</t>
+  </si>
+  <si>
+    <t>三重運動公園</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:29:30</t>
+  </si>
+  <si>
+    <t>門市反應Tm1發票機（BSC10II）常常清帳後帳條或交易發票都僅印出一小截空白，客服查看發票機韌體版本非251118a，請台芝到店更新發票機韌體版本須為251118a，查看TM2發票機型號為BSC10II，韌體版本也非251118a，也請同步更新....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D649</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:30:24</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:05:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 17:30:00</t>
+  </si>
+  <si>
+    <t>更新發票機韌體版本251118a 
+Tm1. Tm2</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:54:21</t>
+  </si>
+  <si>
+    <t>2026-01-12 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002796</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:48:04</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:25:00</t>
+  </si>
+  <si>
+    <t>2026-01-12 14:45:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002825</t>
+  </si>
+  <si>
+    <t>2026-01-12 16:02:10</t>
+  </si>
+  <si>
+    <t>2026-01-12 16:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003072</t>
   </si>
 </sst>
 </file>
@@ -2289,10 +2655,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK85"/>
+  <dimension ref="A1:AK104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="AC101" sqref="AC101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8991,32 +9357,52 @@
         <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C79" s="7">
-        <v>2026011399</v>
-      </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
+        <v>2026011396</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F79" s="7">
-        <v>3606</v>
+        <v>3017</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>576</v>
+        <v>295</v>
       </c>
       <c r="H79" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I79" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="I79" s="7"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="8"/>
-      <c r="N79" s="7"/>
-      <c r="O79" s="8"/>
-      <c r="P79" s="9"/>
+      <c r="J79" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L79" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M79" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N79" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O79" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P79" s="9" t="s">
+        <v>578</v>
+      </c>
       <c r="Q79" s="7" t="s">
-        <v>578</v>
+        <v>301</v>
       </c>
       <c r="R79" s="7" t="s">
         <v>51</v>
@@ -9039,20 +9425,20 @@
       <c r="X79" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="Y79" s="7"/>
+      <c r="Y79" s="7" t="s">
+        <v>582</v>
+      </c>
       <c r="Z79" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AA79" s="7"/>
       <c r="AB79" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC79" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="AD79" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>583</v>
+      </c>
+      <c r="AD79" s="7"/>
       <c r="AE79" s="7"/>
       <c r="AF79" s="7"/>
       <c r="AG79" s="7"/>
@@ -9071,18 +9457,18 @@
         <v>118</v>
       </c>
       <c r="C80" s="3">
-        <v>2026011400</v>
+        <v>2026011399</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3">
-        <v>4656</v>
+        <v>3606</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
@@ -9093,7 +9479,7 @@
       <c r="O80" s="4"/>
       <c r="P80" s="10"/>
       <c r="Q80" s="3" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="R80" s="3" t="s">
         <v>51</v>
@@ -9108,24 +9494,24 @@
         <v>53</v>
       </c>
       <c r="V80" s="3" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="W80" s="3" t="s">
-        <v>503</v>
+        <v>588</v>
       </c>
       <c r="X80" s="3" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="Y80" s="3"/>
       <c r="Z80" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA80" s="3"/>
       <c r="AB80" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC80" s="10" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="AD80" s="3" t="s">
         <v>60</v>
@@ -9145,58 +9531,38 @@
         <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="C81" s="7">
-        <v>2026011408</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>588</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>2026011400</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
       <c r="F81" s="7">
-        <v>4196</v>
+        <v>4656</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>321</v>
+        <v>591</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>589</v>
-      </c>
-      <c r="J81" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="K81" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L81" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="M81" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N81" s="7">
-        <v>2307</v>
-      </c>
-      <c r="O81" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="P81" s="9" t="s">
-        <v>590</v>
-      </c>
+        <v>585</v>
+      </c>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9"/>
       <c r="Q81" s="7" t="s">
-        <v>324</v>
+        <v>592</v>
       </c>
       <c r="R81" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S81" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T81" s="7">
         <v>1</v>
@@ -9205,28 +9571,28 @@
         <v>53</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="W81" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="X81" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="Y81" s="7" t="s">
-        <v>593</v>
-      </c>
+        <v>594</v>
+      </c>
+      <c r="Y81" s="7"/>
       <c r="Z81" s="7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AA81" s="7"/>
       <c r="AB81" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC81" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="AD81" s="7"/>
+        <v>595</v>
+      </c>
+      <c r="AD81" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AE81" s="7"/>
       <c r="AF81" s="7"/>
       <c r="AG81" s="7"/>
@@ -9242,13 +9608,17 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C82" s="3">
-        <v>2026011437</v>
-      </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
+        <v>2026011408</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F82" s="3">
         <v>4196</v>
       </c>
@@ -9258,14 +9628,30 @@
       <c r="H82" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="3"/>
-      <c r="O82" s="4"/>
-      <c r="P82" s="10"/>
+      <c r="I82" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N82" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>598</v>
+      </c>
       <c r="Q82" s="3" t="s">
         <v>324</v>
       </c>
@@ -9273,7 +9659,7 @@
         <v>51</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T82" s="3">
         <v>1</v>
@@ -9282,15 +9668,17 @@
         <v>53</v>
       </c>
       <c r="V82" s="3" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="W82" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="X82" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="Y82" s="3"/>
+        <v>600</v>
+      </c>
+      <c r="Y82" s="3" t="s">
+        <v>601</v>
+      </c>
       <c r="Z82" s="3">
         <v>2</v>
       </c>
@@ -9299,7 +9687,7 @@
         <v>58</v>
       </c>
       <c r="AC82" s="10" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="AD82" s="3"/>
       <c r="AE82" s="3"/>
@@ -9307,9 +9695,7 @@
       <c r="AG82" s="3"/>
       <c r="AH82" s="3"/>
       <c r="AI82" s="3"/>
-      <c r="AJ82" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ82" s="3"/>
       <c r="AK82" s="3" t="s">
         <v>60</v>
       </c>
@@ -9322,7 +9708,7 @@
         <v>118</v>
       </c>
       <c r="C83" s="7">
-        <v>2026011438</v>
+        <v>2026011437</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -9350,7 +9736,7 @@
         <v>51</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="T83" s="7">
         <v>1</v>
@@ -9359,28 +9745,26 @@
         <v>53</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="W83" s="7" t="s">
-        <v>598</v>
+        <v>503</v>
       </c>
       <c r="X83" s="7" t="s">
-        <v>592</v>
+        <v>504</v>
       </c>
       <c r="Y83" s="7"/>
       <c r="Z83" s="7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="AA83" s="7"/>
       <c r="AB83" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC83" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="AD83" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>604</v>
+      </c>
+      <c r="AD83" s="7"/>
       <c r="AE83" s="7"/>
       <c r="AF83" s="7"/>
       <c r="AG83" s="7"/>
@@ -9401,15 +9785,15 @@
         <v>118</v>
       </c>
       <c r="C84" s="3">
-        <v>2026011459</v>
+        <v>2026011438</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3">
-        <v>4191</v>
+        <v>4196</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>527</v>
+        <v>321</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>92</v>
@@ -9423,7 +9807,7 @@
       <c r="O84" s="4"/>
       <c r="P84" s="10"/>
       <c r="Q84" s="3" t="s">
-        <v>530</v>
+        <v>324</v>
       </c>
       <c r="R84" s="3" t="s">
         <v>51</v>
@@ -9438,13 +9822,13 @@
         <v>53</v>
       </c>
       <c r="V84" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="X84" s="3" t="s">
         <v>600</v>
-      </c>
-      <c r="W84" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="X84" s="3" t="s">
-        <v>602</v>
       </c>
       <c r="Y84" s="3"/>
       <c r="Z84" s="3">
@@ -9455,7 +9839,7 @@
         <v>58</v>
       </c>
       <c r="AC84" s="10" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="AD84" s="3" t="s">
         <v>60</v>
@@ -9468,7 +9852,9 @@
       <c r="AJ84" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AK84" s="3"/>
+      <c r="AK84" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="85" spans="1:37">
       <c r="A85" s="7">
@@ -9478,7 +9864,7 @@
         <v>118</v>
       </c>
       <c r="C85" s="7">
-        <v>2026011460</v>
+        <v>2026011459</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -9498,7 +9884,7 @@
       <c r="M85" s="8"/>
       <c r="N85" s="7"/>
       <c r="O85" s="8"/>
-      <c r="P85" s="8"/>
+      <c r="P85" s="9"/>
       <c r="Q85" s="7" t="s">
         <v>530</v>
       </c>
@@ -9515,13 +9901,13 @@
         <v>53</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="W85" s="7" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="X85" s="7" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="Y85" s="7"/>
       <c r="Z85" s="7">
@@ -9531,8 +9917,8 @@
       <c r="AB85" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC85" s="8" t="s">
-        <v>603</v>
+      <c r="AC85" s="9" t="s">
+        <v>611</v>
       </c>
       <c r="AD85" s="7" t="s">
         <v>60</v>
@@ -9545,7 +9931,1676 @@
       <c r="AJ85" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AK85" s="7" t="s">
+      <c r="AK85" s="7"/>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2026011460</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3">
+        <v>4191</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T86" s="3">
+        <v>1</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V86" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC86" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="AD86" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+      <c r="AJ86" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK86" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2026011519</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7">
+        <v>5574</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="9"/>
+      <c r="Q87" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="R87" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T87" s="7">
+        <v>1</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V87" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="W87" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="X87" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC87" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="AD87" s="7"/>
+      <c r="AE87" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" s="3">
+        <v>2026011520</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F88" s="3">
+        <v>4210</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q88" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T88" s="3">
+        <v>1</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="Y88" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z88" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="AD88" s="3"/>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="3"/>
+      <c r="AK88" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2026011521</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F89" s="7">
+        <v>2375</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M89" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="N89" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O89" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="P89" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q89" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y89" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z89" s="7">
+        <v>2.2</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC89" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2026011522</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F90" s="3">
+        <v>2375</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>2.2</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2026011523</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F91" s="7">
+        <v>2375</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L91" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M91" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N91" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O91" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P91" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q91" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y91" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z91" s="7">
+        <v>2.2</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2026011524</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F92" s="3">
+        <v>2375</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N92" s="3">
+        <v>2304</v>
+      </c>
+      <c r="O92" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="P92" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y92" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z92" s="3">
+        <v>2.2</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="AD92" s="3"/>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2026011528</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" s="7">
+        <v>3770</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K93" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L93" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M93" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N93" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O93" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="P93" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q93" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="Y93" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z93" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC93" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="AD93" s="7"/>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2026011530</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F94" s="3">
+        <v>3052</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N94" s="3">
+        <v>2503</v>
+      </c>
+      <c r="O94" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="R94" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T94" s="3">
+        <v>1</v>
+      </c>
+      <c r="U94" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V94" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="X94" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="Y94" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z94" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="AD94" s="3"/>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+      <c r="AJ94" s="3"/>
+      <c r="AK94" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" s="7">
+        <v>2026011531</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="7">
+        <v>2201</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K95" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L95" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="M95" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="N95" s="7">
+        <v>2401</v>
+      </c>
+      <c r="O95" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="P95" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q95" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="R95" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T95" s="7">
+        <v>1</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V95" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="W95" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="X95" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="Y95" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z95" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC95" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="AD95" s="7"/>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="7"/>
+      <c r="AG95" s="7"/>
+      <c r="AH95" s="7"/>
+      <c r="AI95" s="7"/>
+      <c r="AJ95" s="7"/>
+      <c r="AK95" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2026011538</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <v>5574</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S96" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T96" s="3">
+        <v>1</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V96" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="X96" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD96" s="3"/>
+      <c r="AE96" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+      <c r="AJ96" s="3"/>
+      <c r="AK96" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2026011539</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7">
+        <v>5574</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="9"/>
+      <c r="Q97" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7">
+        <v>1.1</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC97" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="AD97" s="7"/>
+      <c r="AE97" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7"/>
+      <c r="AK97" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2026011635</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="N98" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q98" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="Y98" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="Z98" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC98" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD98" s="3"/>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3"/>
+      <c r="AK98" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2026011644</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7">
+        <v>3052</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="Y99" s="7"/>
+      <c r="Z99" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC99" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="AD99" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK99" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2026011672</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3">
+        <v>3770</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK100" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2026011680</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="K101" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L101" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N101" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P101" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="Q101" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="Y101" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="Z101" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>712</v>
+      </c>
+      <c r="AD101" s="7"/>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7"/>
+      <c r="AK101" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2026011685</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3">
+        <v>4210</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="10"/>
+      <c r="Q102" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC102" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="AD102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK102" s="3"/>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2026011700</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC103" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="AD103" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK103" s="7"/>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2026011721</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC104" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="AD104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK104" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01131912
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$104</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$112</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="723">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-12  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="775">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-13  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2235,6 +2235,30 @@
     <t>PMQ1+7210002825</t>
   </si>
   <si>
+    <t>E4191115011201</t>
+  </si>
+  <si>
+    <t>2026-01-12 15:31:12</t>
+  </si>
+  <si>
+    <t>門市性質轉換,TM1 CCD掃描器(HC56II-TR)黑色膠條破損.......還請台芝到店協助(塑膠膠條脫落)</t>
+  </si>
+  <si>
+    <t>2026-01-12 15:46:42</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:15:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:35:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 19:46:00</t>
+  </si>
+  <si>
+    <t>換下8119007307換上8119011531</t>
+  </si>
+  <si>
     <t>2026-01-12 16:02:10</t>
   </si>
   <si>
@@ -2242,6 +2266,141 @@
   </si>
   <si>
     <t>PMQ1+7210003072</t>
+  </si>
+  <si>
+    <t>E4155115011301</t>
+  </si>
+  <si>
+    <t>三重穀保店</t>
+  </si>
+  <si>
+    <t>2026-01-13 08:37:27</t>
+  </si>
+  <si>
+    <t>1/13 09:00 啟動緊急叫修:門市反應SC(SHUTTLE6S)無法正常開機，畫面顯示黑底英文字(Reboot and Select proper boot device or insert boot media in select boot device )的畫面，已請門市將插頭拔掉休息5分鐘後再次開機測試仍異常，PING1不通無法VNC....須請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳關到1/12，與通訊圭連確認有收到銷售，無TM1.2電子存根聯(主機壞掉，螢幕全黑)</t>
+  </si>
+  <si>
+    <t>THILF04155</t>
+  </si>
+  <si>
+    <t>2026-01-13 09:07:21</t>
+  </si>
+  <si>
+    <t>2026-01-13 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 11:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:07:00</t>
+  </si>
+  <si>
+    <t>更換第二顆硬碟不備份還原
+並告知金小姐更換硬碟注意事項
+回報0800</t>
+  </si>
+  <si>
+    <t>淡水屯山店</t>
+  </si>
+  <si>
+    <t>THILF04511</t>
+  </si>
+  <si>
+    <t>2026-01-13 11:12:01</t>
+  </si>
+  <si>
+    <t>2026-01-13 11:11:00</t>
+  </si>
+  <si>
+    <t>閉店撤機已完工</t>
+  </si>
+  <si>
+    <t>E4609115011301</t>
+  </si>
+  <si>
+    <t>蘆洲洲正店</t>
+  </si>
+  <si>
+    <t>2026-01-13 12:20:56</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機無法連線,已有重啟MMK仍無進到網路設定介面,無法連線到正常畫面.....還請台芝到店協助(無法連網路)
+1/13 12:28 請門市初步排除，稍晚去電確認..吳</t>
+  </si>
+  <si>
+    <t>THILF04609</t>
+  </si>
+  <si>
+    <t>2026-01-13 12:45:08</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 16:45:00</t>
+  </si>
+  <si>
+    <t>重設HUB 以再生龍重裝系統</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:24:49</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003084</t>
+  </si>
+  <si>
+    <t>林口老師店</t>
+  </si>
+  <si>
+    <t>THILF04514</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:31:58</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:31:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002876</t>
+  </si>
+  <si>
+    <t>林口舊街店</t>
+  </si>
+  <si>
+    <t>THILF05364</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:57:58</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 16:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002880</t>
+  </si>
+  <si>
+    <t>林口築夢店</t>
+  </si>
+  <si>
+    <t>THILF04483</t>
+  </si>
+  <si>
+    <t>2026-01-13 16:41:40</t>
+  </si>
+  <si>
+    <t>2026-01-13 16:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002875</t>
   </si>
 </sst>
 </file>
@@ -2655,10 +2814,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK104"/>
+  <dimension ref="A1:AK112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC101" sqref="AC101"/>
+      <selection activeCell="AC109" sqref="AC109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11530,38 +11689,58 @@
         <v>102</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C104" s="3">
-        <v>2026011721</v>
-      </c>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3" t="s">
-        <v>688</v>
+        <v>2026011718</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F104" s="3">
+        <v>4191</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>689</v>
+        <v>527</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O104" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>722</v>
+      </c>
       <c r="Q104" s="3" t="s">
-        <v>692</v>
+        <v>530</v>
       </c>
       <c r="R104" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S104" s="3" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T104" s="3">
         <v>1</v>
@@ -11570,37 +11749,695 @@
         <v>53</v>
       </c>
       <c r="V104" s="3" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="W104" s="3" t="s">
-        <v>695</v>
+        <v>724</v>
       </c>
       <c r="X104" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="Y104" s="3"/>
+        <v>725</v>
+      </c>
+      <c r="Y104" s="3" t="s">
+        <v>726</v>
+      </c>
       <c r="Z104" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA104" s="3"/>
       <c r="AB104" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC104" s="4" t="s">
-        <v>722</v>
-      </c>
-      <c r="AD104" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC104" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="AD104" s="3"/>
       <c r="AE104" s="3"/>
       <c r="AF104" s="3"/>
       <c r="AG104" s="3"/>
       <c r="AH104" s="3"/>
       <c r="AI104" s="3"/>
-      <c r="AJ104" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ104" s="3"/>
       <c r="AK104" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:37">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C105" s="7">
+        <v>2026011721</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="8"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="8"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T105" s="7">
+        <v>1</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V105" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="W105" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="X105" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="Y105" s="7"/>
+      <c r="Z105" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC105" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD105" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="7"/>
+      <c r="AG105" s="7"/>
+      <c r="AH105" s="7"/>
+      <c r="AI105" s="7"/>
+      <c r="AJ105" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK105" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:37">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2026011769</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106" s="3">
+        <v>4155</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="N106" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O106" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q106" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T106" s="3">
+        <v>1</v>
+      </c>
+      <c r="U106" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V106" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="X106" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="Y106" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="Z106" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC106" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="AD106" s="3"/>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3"/>
+      <c r="AK106" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:37">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C107" s="7">
+        <v>2026011804</v>
+      </c>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7">
+        <v>4511</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="8"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="8"/>
+      <c r="P107" s="9"/>
+      <c r="Q107" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T107" s="7">
+        <v>1</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="W107" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="X107" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC107" s="9" t="s">
+        <v>745</v>
+      </c>
+      <c r="AD107" s="7"/>
+      <c r="AE107" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF107" s="7"/>
+      <c r="AG107" s="7"/>
+      <c r="AH107" s="7"/>
+      <c r="AI107" s="7"/>
+      <c r="AJ107" s="7"/>
+      <c r="AK107" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:37">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2026011844</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F108" s="3">
+        <v>4609</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="N108" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T108" s="3">
+        <v>1</v>
+      </c>
+      <c r="U108" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="Y108" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="Z108" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC108" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="AD108" s="3"/>
+      <c r="AE108" s="3"/>
+      <c r="AF108" s="3"/>
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:37">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C109" s="7">
+        <v>2026011870</v>
+      </c>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7">
+        <v>4609</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="8"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="8"/>
+      <c r="P109" s="9"/>
+      <c r="Q109" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T109" s="7">
+        <v>1</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V109" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="W109" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="X109" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="Y109" s="7"/>
+      <c r="Z109" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC109" s="9" t="s">
+        <v>757</v>
+      </c>
+      <c r="AD109" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
+      <c r="AG109" s="7"/>
+      <c r="AH109" s="7"/>
+      <c r="AI109" s="7"/>
+      <c r="AJ109" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK109" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2026011887</v>
+      </c>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3">
+        <v>4514</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="Y110" s="3"/>
+      <c r="Z110" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC110" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="AD110" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:37">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C111" s="7">
+        <v>2026011896</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T111" s="7">
+        <v>1</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V111" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="W111" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="Y111" s="7"/>
+      <c r="Z111" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC111" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="AD111" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="7"/>
+      <c r="AH111" s="7"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="7"/>
+      <c r="AK111" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:37">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2026011901</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3">
+        <v>4483</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S112" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T112" s="3">
+        <v>1</v>
+      </c>
+      <c r="U112" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="X112" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="Y112" s="3"/>
+      <c r="Z112" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC112" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="AD112" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE112" s="3"/>
+      <c r="AF112" s="3"/>
+      <c r="AG112" s="3"/>
+      <c r="AH112" s="3"/>
+      <c r="AI112" s="3"/>
+      <c r="AJ112" s="3"/>
+      <c r="AK112" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01161919
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$112</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="775">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-13  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="926">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-16  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2343,6 +2343,36 @@
     <t>重設HUB 以再生龍重裝系統</t>
   </si>
   <si>
+    <t>15428115011302</t>
+  </si>
+  <si>
+    <t>三重野球魂</t>
+  </si>
+  <si>
+    <t>2026-01-13 13:50:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1發票機（BSC10II）常常發生發票未印出情況，客服查看發票機韌體版本非251118a，請台芝到店更新發票機韌體版本須為251118a，查看TM2發票機型號為BSC10II，韌體版本也非251118a，也請同步更新....請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>THILF05428</t>
+  </si>
+  <si>
+    <t>2026-01-13 13:51:11</t>
+  </si>
+  <si>
+    <t>2026-01-13 18:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-13 19:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 17:51:00</t>
+  </si>
+  <si>
+    <t>更新發票機韌體版本251118a.TM1 TM2</t>
+  </si>
+  <si>
     <t>2026-01-13 14:24:49</t>
   </si>
   <si>
@@ -2352,6 +2382,31 @@
     <t>PMQ1+7210003084</t>
   </si>
   <si>
+    <t>15428115011303</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:18:43</t>
+  </si>
+  <si>
+    <t>1/13 14:36 與總公司明翰確認啟動緊急叫修:SC(SHUTTLE7S)-門市原反應操作入帳日1/13的TM轉SC無TM1、2的資料，執行1/13銷售上傳均顯示上傳失敗，查看TM主檔也卡在1/12，經HIPOS查看因帳務卡在TM C槽UPLOAD內故銷售上傳失敗，協助門市版更TM顯示與Sc連線失敗，判斷為此原因導致清帳帳務無法上送至Sc，已手動搬1/13TM帳務檔至SC門市可正常作帳，煩請協助轉派台芝檢查相關設備及線路。經總公司功評檢視SC內無硬碟異常資訊，嘗試重新協助安裝HIPOS資料庫後仍無法作業，請派工到店更換SC第二顆硬碟不備份還原，並攜帶第一顆備用..請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳關到1/13，與通訊圭連確認有收到銷售 ※非24H營業門市，0700~2300營業</t>
+  </si>
+  <si>
+    <t>2026-01-13 14:44:28</t>
+  </si>
+  <si>
+    <t>2026-01-13 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 07:44:00</t>
+  </si>
+  <si>
+    <t>更換SC第二顆硬碟不備份還原
+已跟店家告知宣達請門市回報代收會計.     
+SC_Slave = 20250805
+HiPOS  最新版本=S1223.53.0   
+ARC.DEF = 4.C30u</t>
+  </si>
+  <si>
     <t>林口老師店</t>
   </si>
   <si>
@@ -2370,6 +2425,32 @@
     <t>PMQ1+7210002876</t>
   </si>
   <si>
+    <t>E4514115011301</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:36:10</t>
+  </si>
+  <si>
+    <t>門市反應LIFE ET熱感機(T70II)常常發生卡紙的狀況，門市都需要重裝紙捲重開機才會正常，但仍不定時會發生此狀況...需請台芝到店協助(熱感紙列印時容易卡紙)</t>
+  </si>
+  <si>
+    <t>2026-01-13 15:42:04</t>
+  </si>
+  <si>
+    <t>2026-01-14 13:05:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 13:35:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 19:42:00</t>
+  </si>
+  <si>
+    <t>更換出單機
+換下8138002695
+換上8138001841</t>
+  </si>
+  <si>
     <t>林口舊街店</t>
   </si>
   <si>
@@ -2397,10 +2478,405 @@
     <t>2026-01-13 16:41:40</t>
   </si>
   <si>
-    <t>2026-01-13 16:30:00</t>
-  </si>
-  <si>
     <t>PMQ1+7210002875</t>
+  </si>
+  <si>
+    <t>2026-01-13 19:45:45</t>
+  </si>
+  <si>
+    <t>2026-01-13 16:10:00</t>
+  </si>
+  <si>
+    <t>E3358115011401</t>
+  </si>
+  <si>
+    <t>新莊棒球場</t>
+  </si>
+  <si>
+    <t>2026-01-14 07:49:09</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)抽屜錢匣彈簧斷2個，抽屜外觀米白/鑰匙孔右邊/鑰匙孔編號711....須請台芝到店協助(鈔票夾彈簧斷裂*2)</t>
+  </si>
+  <si>
+    <t>THILF03358</t>
+  </si>
+  <si>
+    <t>2026-01-14 09:05:24</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 13:05:00</t>
+  </si>
+  <si>
+    <t>更換錢箱鈔票夾X2</t>
+  </si>
+  <si>
+    <t>E3358115011402</t>
+  </si>
+  <si>
+    <t>2026-01-14 08:09:17</t>
+  </si>
+  <si>
+    <t>門市反應tm2(TCX800)螢幕觸控異常鼠標閃爍且會自己亂點，門市已有重啟仍異常無法操作觸控校正....須請台芝到店協助(機2觸控不良)</t>
+  </si>
+  <si>
+    <t>2026-01-14 09:06:55</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 13:06:00</t>
+  </si>
+  <si>
+    <t>客顯器端有商品壓著影響觸控 
+移除商品測試正常</t>
+  </si>
+  <si>
+    <t>14312115011401</t>
+  </si>
+  <si>
+    <t>三重文化北</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:00:53</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)抽屜錢匣彈簧1個鬆脫，抽屜外觀白/鑰匙孔中間/無鑰匙孔編號....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04312</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:02:31</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:35:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 14:02:00</t>
+  </si>
+  <si>
+    <t>更換錢箱鐵夾.已裝回彈簧</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:06:04</t>
+  </si>
+  <si>
+    <t>2026-01-14 10:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002799</t>
+  </si>
+  <si>
+    <t>15457115011401</t>
+  </si>
+  <si>
+    <t>三重鑫五華</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:09:04</t>
+  </si>
+  <si>
+    <t>門市反應TM1發票機（BSC10II）常常發生退瓶僅印出一小截空白，客服查看發票機韌體版本為3.1非251118a，請台芝到店更新發票機韌體版本須為251118a，查看TM2發票機型號為BSC10II，韌體版本為3.1也非251118a，也請同步更新....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05457</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:11:14</t>
+  </si>
+  <si>
+    <t>2026-01-14 18:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 19:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 15:11:00</t>
+  </si>
+  <si>
+    <t>更新發票機韌體版本為251118a TM1. TM2</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:51:25</t>
+  </si>
+  <si>
+    <t>2026-01-14 12:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003053</t>
+  </si>
+  <si>
+    <t>E2442115011401</t>
+  </si>
+  <si>
+    <t>2026-01-14 11:59:44</t>
+  </si>
+  <si>
+    <t>門市反應L90停電後無電源反應未亮燈，門市已有重插後方線路仍異常....須請台芝到店協助(停電之後沒有電源顯示，插頭重新插也沒反應)</t>
+  </si>
+  <si>
+    <t>2026-01-14 12:06:53</t>
+  </si>
+  <si>
+    <t>2026-01-14 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 16:38:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 16:06:00</t>
+  </si>
+  <si>
+    <t>變壓器無反應，更換變壓器測試正常</t>
+  </si>
+  <si>
+    <t>林口建林店</t>
+  </si>
+  <si>
+    <t>THILF04282</t>
+  </si>
+  <si>
+    <t>2026-01-14 14:31:53</t>
+  </si>
+  <si>
+    <t>2026-01-14 14:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 14:31:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002873</t>
+  </si>
+  <si>
+    <t>E4316115011401</t>
+  </si>
+  <si>
+    <t>2026-01-14 15:39:44</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD)畫面閃爍頻繁，已嘗試重新拔插後方線路仍異常...需請台芝到店協助(螢幕閃縮)</t>
+  </si>
+  <si>
+    <t>2026-01-14 15:47:19</t>
+  </si>
+  <si>
+    <t>2026-01-15 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 19:47:00</t>
+  </si>
+  <si>
+    <t>重插螢幕背後電源線 訊號線</t>
+  </si>
+  <si>
+    <t>14210115011401</t>
+  </si>
+  <si>
+    <t>2026-01-14 16:01:20</t>
+  </si>
+  <si>
+    <t>門市反應咖啡價目電子看板未更新都顯示舊的資料,水電已到店確認網路無異常，但告知網路線未插在數據機上，已有引導門市插回指定數據機，但價目表仍為舊素材，且內外連線部皆無更新...2026/1/14 (週三) 下午 03:59 總公司娟慧MAIL:請派台芝協助，謝謝您~.....還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-14 16:02:09</t>
+  </si>
+  <si>
+    <t>2026-01-15 15:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 17:06:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 20:02:00</t>
+  </si>
+  <si>
+    <t>到店檢測結果
+1.電視接前場TV線 、商顯數據機接後場TV線
+= 網路無訊號
+2. 筆電接前場TV線 、商顯數據機接後場TV線
+= 網路無訊號
+3. 電視接前場刷卡機A線 、商顯數據機接後場刷卡機A線
+= 網路無訊號
+4. 筆電接前場TV線、SC-HUB接後場TV線
+= 無法PING通HUB</t>
+  </si>
+  <si>
+    <t>2026-01-14 19:24:21</t>
+  </si>
+  <si>
+    <t>2026-01-14 18:55:00</t>
+  </si>
+  <si>
+    <t>2026-01-14 19:20:00</t>
+  </si>
+  <si>
+    <t>三重向日葵</t>
+  </si>
+  <si>
+    <t>THILF05491</t>
+  </si>
+  <si>
+    <t>2026-01-15 15:35:53</t>
+  </si>
+  <si>
+    <t>2026-01-15 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-15 15:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">協助新開門市 </t>
+  </si>
+  <si>
+    <t>2026-01-15 16:49:33</t>
+  </si>
+  <si>
+    <t>新開門市完工 已回報0800確認版本</t>
+  </si>
+  <si>
+    <t>12303115011501</t>
+  </si>
+  <si>
+    <t>三重三和夜市</t>
+  </si>
+  <si>
+    <t>2026-01-15 17:37:36</t>
+  </si>
+  <si>
+    <t>抽屜無法正常開關</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm1收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中間)、鎖頭編號:無)抽屜無法開啟，點選開抽屜也無反應以及無彈開聲音，已有將發票機關機紙捲重裝仍異常...請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>THILF02303</t>
+  </si>
+  <si>
+    <t>2026-01-15 17:39:32</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:35:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 21:39:00</t>
+  </si>
+  <si>
+    <t>線路鬆脫.插回正常</t>
+  </si>
+  <si>
+    <t>E4153115011601</t>
+  </si>
+  <si>
+    <t>淡水莊園店</t>
+  </si>
+  <si>
+    <t>2026-01-16 07:40:26</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)抽屜彈出時都會卡住有彈出聲彈出一點點，抽屜外觀米白/鑰匙孔右邊/鑰匙孔編號k01.....須請台芝到店協助(機依 抽屜卡卡)</t>
+  </si>
+  <si>
+    <t>THILF04153</t>
+  </si>
+  <si>
+    <t>2026-01-16 09:11:21</t>
+  </si>
+  <si>
+    <t>2026-01-16 14:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 13:11:00</t>
+  </si>
+  <si>
+    <t>調整磁簧 清潔上油</t>
+  </si>
+  <si>
+    <t>15428115011601</t>
+  </si>
+  <si>
+    <t>2026-01-16 09:17:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026/1/16 (週五) 上午 08:55 總公司明翰mail 通知:sc(SHUTTLE7S)有關5428三重野球魂門市，請安排到店更換主機。請協助緊急叫修，到店更換SC主機及第一、二顆硬碟，資料不備份，謝謝。...須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳做到01/15，與嘉芳確認都有收到
+</t>
+  </si>
+  <si>
+    <t>2026-01-16 09:27:25</t>
+  </si>
+  <si>
+    <t>2026-01-16 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:27:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">更換sc主機及第一 二 顆硬碟不備份還原
+換下8114004716換上8114004793
+SC = 20250805
+SC_Slave = 20250805
+HiPOS  最新版本=S109.61.0   ARC.DEF = ARC4.c30u
+已跟店家宣達請門市先回報代收會計 </t>
+  </si>
+  <si>
+    <t>D148</t>
+  </si>
+  <si>
+    <t>新莊福營店</t>
+  </si>
+  <si>
+    <t>THILF0D148</t>
+  </si>
+  <si>
+    <t>2026-01-16 11:36:41</t>
+  </si>
+  <si>
+    <t>2026-01-16 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-16 10:30:00</t>
+  </si>
+  <si>
+    <t>閉店撤機</t>
+  </si>
+  <si>
+    <t>2026-01-16 13:36:57</t>
+  </si>
+  <si>
+    <t>閉店</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:57:04</t>
+  </si>
+  <si>
+    <t>2026-01-16 15:55:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002764</t>
   </si>
 </sst>
 </file>
@@ -2814,10 +3290,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK112"/>
+  <dimension ref="A1:AK135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC109" sqref="AC109"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12136,38 +12612,58 @@
         <v>107</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C109" s="7">
-        <v>2026011870</v>
-      </c>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
+        <v>2026011855</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F109" s="7">
-        <v>4609</v>
+        <v>5428</v>
       </c>
       <c r="G109" s="7" t="s">
-        <v>747</v>
+        <v>756</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="I109" s="7"/>
-      <c r="J109" s="7"/>
-      <c r="K109" s="7"/>
-      <c r="L109" s="7"/>
-      <c r="M109" s="8"/>
-      <c r="N109" s="7"/>
-      <c r="O109" s="8"/>
-      <c r="P109" s="9"/>
+        <v>92</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N109" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P109" s="9" t="s">
+        <v>758</v>
+      </c>
       <c r="Q109" s="7" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="R109" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S109" s="7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T109" s="7">
         <v>1</v>
@@ -12176,15 +12672,17 @@
         <v>53</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="W109" s="7" t="s">
-        <v>752</v>
+        <v>761</v>
       </c>
       <c r="X109" s="7" t="s">
-        <v>756</v>
-      </c>
-      <c r="Y109" s="7"/>
+        <v>762</v>
+      </c>
+      <c r="Y109" s="7" t="s">
+        <v>763</v>
+      </c>
       <c r="Z109" s="7">
         <v>0.5</v>
       </c>
@@ -12193,19 +12691,15 @@
         <v>58</v>
       </c>
       <c r="AC109" s="9" t="s">
-        <v>757</v>
-      </c>
-      <c r="AD109" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>764</v>
+      </c>
+      <c r="AD109" s="7"/>
       <c r="AE109" s="7"/>
       <c r="AF109" s="7"/>
       <c r="AG109" s="7"/>
       <c r="AH109" s="7"/>
       <c r="AI109" s="7"/>
-      <c r="AJ109" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ109" s="7"/>
       <c r="AK109" s="7" t="s">
         <v>60</v>
       </c>
@@ -12218,18 +12712,18 @@
         <v>118</v>
       </c>
       <c r="C110" s="3">
-        <v>2026011887</v>
+        <v>2026011870</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3">
-        <v>4514</v>
+        <v>4609</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>758</v>
+        <v>747</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>514</v>
+        <v>250</v>
       </c>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
@@ -12240,13 +12734,13 @@
       <c r="O110" s="4"/>
       <c r="P110" s="10"/>
       <c r="Q110" s="3" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="R110" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="T110" s="3">
         <v>1</v>
@@ -12255,13 +12749,13 @@
         <v>53</v>
       </c>
       <c r="V110" s="3" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
       <c r="X110" s="3" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="Y110" s="3"/>
       <c r="Z110" s="3">
@@ -12272,7 +12766,7 @@
         <v>58</v>
       </c>
       <c r="AC110" s="10" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="AD110" s="3" t="s">
         <v>60</v>
@@ -12282,7 +12776,9 @@
       <c r="AG110" s="3"/>
       <c r="AH110" s="3"/>
       <c r="AI110" s="3"/>
-      <c r="AJ110" s="3"/>
+      <c r="AJ110" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK110" s="3" t="s">
         <v>60</v>
       </c>
@@ -12292,38 +12788,58 @@
         <v>109</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C111" s="7">
-        <v>2026011896</v>
-      </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
+        <v>2026011875</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F111" s="7">
-        <v>5364</v>
+        <v>5428</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="I111" s="7"/>
-      <c r="J111" s="7"/>
-      <c r="K111" s="7"/>
-      <c r="L111" s="7"/>
-      <c r="M111" s="8"/>
-      <c r="N111" s="7"/>
-      <c r="O111" s="8"/>
-      <c r="P111" s="9"/>
+        <v>92</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>769</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="N111" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="P111" s="9" t="s">
+        <v>770</v>
+      </c>
       <c r="Q111" s="7" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="R111" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S111" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T111" s="7">
         <v>1</v>
@@ -12332,28 +12848,28 @@
         <v>53</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="W111" s="7" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="X111" s="7" t="s">
-        <v>768</v>
-      </c>
-      <c r="Y111" s="7"/>
+        <v>761</v>
+      </c>
+      <c r="Y111" s="7" t="s">
+        <v>773</v>
+      </c>
       <c r="Z111" s="7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="AA111" s="7"/>
       <c r="AB111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC111" s="9" t="s">
-        <v>769</v>
-      </c>
-      <c r="AD111" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>774</v>
+      </c>
+      <c r="AD111" s="7"/>
       <c r="AE111" s="7"/>
       <c r="AF111" s="7"/>
       <c r="AG111" s="7"/>
@@ -12372,15 +12888,15 @@
         <v>118</v>
       </c>
       <c r="C112" s="3">
-        <v>2026011901</v>
+        <v>2026011887</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3">
-        <v>4483</v>
+        <v>4514</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>514</v>
@@ -12392,9 +12908,9 @@
       <c r="M112" s="4"/>
       <c r="N112" s="3"/>
       <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
+      <c r="P112" s="10"/>
       <c r="Q112" s="3" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>51</v>
@@ -12409,13 +12925,13 @@
         <v>53</v>
       </c>
       <c r="V112" s="3" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="W112" s="3" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="X112" s="3" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="Y112" s="3"/>
       <c r="Z112" s="3">
@@ -12425,8 +12941,8 @@
       <c r="AB112" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC112" s="4" t="s">
-        <v>774</v>
+      <c r="AC112" s="10" t="s">
+        <v>780</v>
       </c>
       <c r="AD112" s="3" t="s">
         <v>60</v>
@@ -12440,6 +12956,2007 @@
       <c r="AK112" s="3" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="113" spans="1:37">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C113" s="7">
+        <v>2026011892</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F113" s="7">
+        <v>4514</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L113" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="N113" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="P113" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="Q113" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="R113" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T113" s="7">
+        <v>1</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V113" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="W113" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="X113" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="Y113" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="Z113" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC113" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="AD113" s="7"/>
+      <c r="AE113" s="7"/>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="7"/>
+      <c r="AH113" s="7"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="7"/>
+      <c r="AK113" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:37">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2026011896</v>
+      </c>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3">
+        <v>5364</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="10"/>
+      <c r="Q114" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T114" s="3">
+        <v>1</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="Y114" s="3"/>
+      <c r="Z114" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC114" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="AD114" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE114" s="3"/>
+      <c r="AF114" s="3"/>
+      <c r="AG114" s="3"/>
+      <c r="AH114" s="3"/>
+      <c r="AI114" s="3"/>
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2026011901</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7">
+        <v>4483</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="AD115" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2026011919</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>5428</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK116" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2026011921</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F117" s="7">
+        <v>3358</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K117" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="L117" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N117" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P117" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q117" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>808</v>
+      </c>
+      <c r="Y117" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="Z117" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="AD117" s="7"/>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7"/>
+      <c r="AK117" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2026011922</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F118" s="3">
+        <v>3358</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M118" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N118" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O118" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="P118" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="Q118" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="Y118" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="Z118" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="AD118" s="3"/>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3"/>
+      <c r="AK118" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2026011933</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F119" s="7">
+        <v>4312</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K119" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L119" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N119" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P119" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q119" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="Y119" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="Z119" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC119" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="AD119" s="7"/>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7"/>
+      <c r="AK119" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2026011955</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>4312</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK120" s="3"/>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2026011956</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F121" s="7">
+        <v>5457</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I121" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="J121" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K121" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L121" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M121" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N121" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O121" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="P121" s="9" t="s">
+        <v>834</v>
+      </c>
+      <c r="Q121" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="Y121" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="Z121" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC121" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="AD121" s="7"/>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2026011972</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>3358</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC122" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="AD122" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE122" s="3"/>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK122" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2026011974</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>844</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F123" s="7">
+        <v>2442</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="J123" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="N123" s="7">
+        <v>6004</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P123" s="9" t="s">
+        <v>846</v>
+      </c>
+      <c r="Q123" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="Y123" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="Z123" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>851</v>
+      </c>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2026011992</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3">
+        <v>4282</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>857</v>
+      </c>
+      <c r="AD124" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2026012028</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F125" s="7">
+        <v>4316</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N125" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P125" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="Q125" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="Y125" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="Z125" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>865</v>
+      </c>
+      <c r="AD125" s="7"/>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2026012133</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F126" s="3">
+        <v>4210</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L126" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="M126" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="N126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="O126" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="P126" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="Q126" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="Y126" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="Z126" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="AD126" s="3"/>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2026012172</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>5457</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK127" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2026012254</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <v>5491</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="Y128" s="3"/>
+      <c r="Z128" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC128" s="10" t="s">
+        <v>882</v>
+      </c>
+      <c r="AD128" s="3"/>
+      <c r="AE128" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3"/>
+      <c r="AK128" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2026012268</v>
+      </c>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7">
+        <v>5491</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="7"/>
+      <c r="O129" s="8"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="Y129" s="7"/>
+      <c r="Z129" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="AD129" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE129" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2026012290</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F130" s="3">
+        <v>2303</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M130" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N130" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O130" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="P130" s="10" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q130" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="Y130" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="Z130" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC130" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="AD130" s="3"/>
+      <c r="AE130" s="3"/>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3"/>
+      <c r="AK130" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2026012296</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F131" s="7">
+        <v>4153</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K131" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="L131" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N131" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O131" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="P131" s="9" t="s">
+        <v>899</v>
+      </c>
+      <c r="Q131" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="Y131" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="Z131" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="AD131" s="7"/>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2026012303</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F132" s="3">
+        <v>5428</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M132" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="N132" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O132" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P132" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q132" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="Y132" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="Z132" s="3">
+        <v>2.2</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>913</v>
+      </c>
+      <c r="AD132" s="3"/>
+      <c r="AE132" s="3"/>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3"/>
+      <c r="AK132" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2026012338</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC133" s="9" t="s">
+        <v>920</v>
+      </c>
+      <c r="AD133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7"/>
+      <c r="AK133" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2026012356</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="10"/>
+      <c r="Q134" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="Y134" s="3"/>
+      <c r="Z134" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC134" s="10" t="s">
+        <v>922</v>
+      </c>
+      <c r="AD134" s="3"/>
+      <c r="AE134" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C135" s="7">
+        <v>2026012400</v>
+      </c>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7">
+        <v>2303</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I135" s="7"/>
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+      <c r="L135" s="7"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="7"/>
+      <c r="O135" s="8"/>
+      <c r="P135" s="8"/>
+      <c r="Q135" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T135" s="7">
+        <v>1</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>923</v>
+      </c>
+      <c r="W135" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="X135" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="Y135" s="7"/>
+      <c r="Z135" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC135" s="8" t="s">
+        <v>925</v>
+      </c>
+      <c r="AD135" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE135" s="7"/>
+      <c r="AF135" s="7"/>
+      <c r="AG135" s="7"/>
+      <c r="AH135" s="7"/>
+      <c r="AI135" s="7"/>
+      <c r="AJ135" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK135" s="7"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 01201241
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$151</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="926">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-16  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1030">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-20  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2877,6 +2877,323 @@
   </si>
   <si>
     <t>PMQ1+7210002764</t>
+  </si>
+  <si>
+    <t>1D649115011601</t>
+  </si>
+  <si>
+    <t>2026-01-16 16:05:25</t>
+  </si>
+  <si>
+    <t>HL34</t>
+  </si>
+  <si>
+    <t>HL-HUB</t>
+  </si>
+  <si>
+    <t>不能連線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB(DES121028)門市網管主線不通，01/16 16:02遠傳邱先生來電告知中華到店查看設備無異常，客服與門市聯繫，需請門市查看後場相關網路設備，但表示繁忙無法協助，故改派台芝到店協助檢查相關網路設備...需請台芝協助需請台芝協助	</t>
+  </si>
+  <si>
+    <t>2026-01-16 16:09:07</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 20:09:00</t>
+  </si>
+  <si>
+    <t>Pep插錯孔. 中華電信接到pep沒插在wan上差在四線上. 已回報0800</t>
+  </si>
+  <si>
+    <t>E4153115011701</t>
+  </si>
+  <si>
+    <t>2026-01-17 11:11:45</t>
+  </si>
+  <si>
+    <t>門市反應tm1(TCX800)抽屜彈出時都會卡住有彈出聲彈出一點仍需手動拉出，抽屜外觀米白/鑰匙孔右邊/鑰匙孔編號k01，01/16 台芝到店調整磁簧 清潔上油.....須請台芝到店協助(還是很卡)</t>
+  </si>
+  <si>
+    <t>2026-01-17 11:27:47</t>
+  </si>
+  <si>
+    <t>2026-01-19 12:01:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 12:31:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 13:00:00</t>
+  </si>
+  <si>
+    <t>更換錢櫃
+換下81Z1001137
+換上81Z1003538</t>
+  </si>
+  <si>
+    <t>15074115011801</t>
+  </si>
+  <si>
+    <t>2026-01-18 14:53:30</t>
+  </si>
+  <si>
+    <t>門市反應tm1 cc掃描器(HC56II-TR、HC76-TR)無電源反應無亮燈，門市告知查看線路無鬆脫、已有重啟tm....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-18 14:54:34</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:00:00</t>
+  </si>
+  <si>
+    <t>POS重新開機有通電，先更換掃槍測試觀察
+更換掃描槍
+換下8119013215
+換上8119010855</t>
+  </si>
+  <si>
+    <t>中和和大店</t>
+  </si>
+  <si>
+    <t>THILF02911</t>
+  </si>
+  <si>
+    <t>2026-01-19 09:35:09</t>
+  </si>
+  <si>
+    <t>2026-01-19 09:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 09:35:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002965</t>
+  </si>
+  <si>
+    <t>中和景德店</t>
+  </si>
+  <si>
+    <t>THILF04536</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:14:33</t>
+  </si>
+  <si>
+    <t>2026-01-19 09:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:03:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002972</t>
+  </si>
+  <si>
+    <t>中和浪漫店</t>
+  </si>
+  <si>
+    <t>THILF04573</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:55:32</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:15:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:37:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002973</t>
+  </si>
+  <si>
+    <t>12303115011901</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:04:54</t>
+  </si>
+  <si>
+    <t>門市反應tm1收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中間)、鎖頭編號:無)抽屜無法開啟，點選開抽屜也無反應以及無彈開聲音，已有將發票機關機紙捲重裝仍異常，台芝於2026-01-16 15:35:00.000線路鬆脫.插回正常，店長進電告知上次工程師有膠帶黏著線路但常常動到又會發生無反應的狀況，因頻繁發生已造成困擾...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:08:42</t>
+  </si>
+  <si>
+    <t>2026-01-19 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:08:00</t>
+  </si>
+  <si>
+    <t>換下81Z1000819. 換上81Z1003419</t>
+  </si>
+  <si>
+    <t>C216</t>
+  </si>
+  <si>
+    <t>中和南勢店</t>
+  </si>
+  <si>
+    <t>THILF0C216</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:13:23</t>
+  </si>
+  <si>
+    <t>2026-01-19 10:49:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002980</t>
+  </si>
+  <si>
+    <t>中和壽南店</t>
+  </si>
+  <si>
+    <t>THILF05401</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:45:33</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:23:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:41:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002977+L90</t>
+  </si>
+  <si>
+    <t>中和嘉德店</t>
+  </si>
+  <si>
+    <t>THILF04770</t>
+  </si>
+  <si>
+    <t>2026-01-19 12:22:38</t>
+  </si>
+  <si>
+    <t>2026-01-19 11:58:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 12:21:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 13:37:37</t>
+  </si>
+  <si>
+    <t>2026-01-19 12:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 13:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002891</t>
+  </si>
+  <si>
+    <t>淡水灰瑤子</t>
+  </si>
+  <si>
+    <t>THILF02749</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:19:13</t>
+  </si>
+  <si>
+    <t>2026-01-19 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002887</t>
+  </si>
+  <si>
+    <t>三芝芝蘭店</t>
+  </si>
+  <si>
+    <t>新北市三芝區</t>
+  </si>
+  <si>
+    <t>THILF02237</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:50:15</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002754</t>
+  </si>
+  <si>
+    <t>三芝天涯店</t>
+  </si>
+  <si>
+    <t>THILF04844</t>
+  </si>
+  <si>
+    <t>2026-01-19 15:29:30</t>
+  </si>
+  <si>
+    <t>2026-01-19 15:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 15:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002755</t>
+  </si>
+  <si>
+    <t>三芝楓愛林</t>
+  </si>
+  <si>
+    <t>THILF05080</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:19:54</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002756</t>
+  </si>
+  <si>
+    <t>淡水櫻花店</t>
+  </si>
+  <si>
+    <t>THILF04739</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:53:02</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-19 16:52:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003044</t>
   </si>
 </sst>
 </file>
@@ -3290,10 +3607,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK135"/>
+  <dimension ref="A1:AK151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A135" sqref="A135"/>
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14909,7 +15226,7 @@
       <c r="M135" s="8"/>
       <c r="N135" s="7"/>
       <c r="O135" s="8"/>
-      <c r="P135" s="8"/>
+      <c r="P135" s="9"/>
       <c r="Q135" s="7" t="s">
         <v>890</v>
       </c>
@@ -14942,7 +15259,7 @@
       <c r="AB135" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC135" s="8" t="s">
+      <c r="AC135" s="9" t="s">
         <v>925</v>
       </c>
       <c r="AD135" s="7" t="s">
@@ -14957,6 +15274,1330 @@
         <v>60</v>
       </c>
       <c r="AK135" s="7"/>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2026012403</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="M136" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="N136" s="3">
+        <v>3402</v>
+      </c>
+      <c r="O136" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="P136" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="Q136" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T136" s="3">
+        <v>1</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="W136" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="X136" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="Y136" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="Z136" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA136" s="3"/>
+      <c r="AB136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC136" s="10" t="s">
+        <v>936</v>
+      </c>
+      <c r="AD136" s="3"/>
+      <c r="AE136" s="3"/>
+      <c r="AF136" s="3"/>
+      <c r="AG136" s="3"/>
+      <c r="AH136" s="3"/>
+      <c r="AI136" s="3"/>
+      <c r="AJ136" s="3"/>
+      <c r="AK136" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="7">
+        <v>2026012435</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F137" s="7">
+        <v>4153</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I137" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="J137" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K137" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L137" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M137" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N137" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O137" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="P137" s="9" t="s">
+        <v>939</v>
+      </c>
+      <c r="Q137" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="R137" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S137" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T137" s="7">
+        <v>1</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V137" s="7" t="s">
+        <v>940</v>
+      </c>
+      <c r="W137" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="X137" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="Y137" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="Z137" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC137" s="9" t="s">
+        <v>944</v>
+      </c>
+      <c r="AD137" s="7"/>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+      <c r="AG137" s="7"/>
+      <c r="AH137" s="7"/>
+      <c r="AI137" s="7"/>
+      <c r="AJ137" s="7"/>
+      <c r="AK137" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:37">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C138" s="3">
+        <v>2026012447</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F138" s="3">
+        <v>5074</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M138" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O138" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P138" s="10" t="s">
+        <v>947</v>
+      </c>
+      <c r="Q138" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S138" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T138" s="3">
+        <v>1</v>
+      </c>
+      <c r="U138" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V138" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="W138" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="X138" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="Y138" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="Z138" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA138" s="3"/>
+      <c r="AB138" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC138" s="10" t="s">
+        <v>951</v>
+      </c>
+      <c r="AD138" s="3"/>
+      <c r="AE138" s="3"/>
+      <c r="AF138" s="3"/>
+      <c r="AG138" s="3"/>
+      <c r="AH138" s="3"/>
+      <c r="AI138" s="3"/>
+      <c r="AJ138" s="3"/>
+      <c r="AK138" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:37">
+      <c r="A139" s="7">
+        <v>137</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C139" s="7">
+        <v>2026012468</v>
+      </c>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7">
+        <v>2911</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I139" s="7"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="8"/>
+      <c r="N139" s="7"/>
+      <c r="O139" s="8"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="R139" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S139" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T139" s="7">
+        <v>1</v>
+      </c>
+      <c r="U139" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V139" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="W139" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="X139" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="Y139" s="7"/>
+      <c r="Z139" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA139" s="7"/>
+      <c r="AB139" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC139" s="9" t="s">
+        <v>957</v>
+      </c>
+      <c r="AD139" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE139" s="7"/>
+      <c r="AF139" s="7"/>
+      <c r="AG139" s="7"/>
+      <c r="AH139" s="7"/>
+      <c r="AI139" s="7"/>
+      <c r="AJ139" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK139" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:37">
+      <c r="A140" s="3">
+        <v>138</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C140" s="3">
+        <v>2026012487</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3">
+        <v>4536</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="R140" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S140" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T140" s="3">
+        <v>1</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V140" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="X140" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="Y140" s="3"/>
+      <c r="Z140" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA140" s="3"/>
+      <c r="AB140" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC140" s="10" t="s">
+        <v>963</v>
+      </c>
+      <c r="AD140" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE140" s="3"/>
+      <c r="AF140" s="3"/>
+      <c r="AG140" s="3"/>
+      <c r="AH140" s="3"/>
+      <c r="AI140" s="3"/>
+      <c r="AJ140" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK140" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2026012502</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7">
+        <v>4573</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="7"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="R141" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S141" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T141" s="7">
+        <v>1</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V141" s="7" t="s">
+        <v>966</v>
+      </c>
+      <c r="W141" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="X141" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC141" s="9" t="s">
+        <v>969</v>
+      </c>
+      <c r="AD141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+      <c r="AG141" s="7"/>
+      <c r="AH141" s="7"/>
+      <c r="AI141" s="7"/>
+      <c r="AJ141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK141" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2026012505</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F142" s="3">
+        <v>2303</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M142" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N142" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O142" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="P142" s="10" t="s">
+        <v>972</v>
+      </c>
+      <c r="Q142" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T142" s="3">
+        <v>1</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="X142" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="Y142" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="Z142" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA142" s="3"/>
+      <c r="AB142" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC142" s="10" t="s">
+        <v>977</v>
+      </c>
+      <c r="AD142" s="3"/>
+      <c r="AE142" s="3"/>
+      <c r="AF142" s="3"/>
+      <c r="AG142" s="3"/>
+      <c r="AH142" s="3"/>
+      <c r="AI142" s="3"/>
+      <c r="AJ142" s="3"/>
+      <c r="AK142" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C143" s="7">
+        <v>2026012506</v>
+      </c>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>979</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="7"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="R143" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S143" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T143" s="7">
+        <v>1</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V143" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="W143" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="X143" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC143" s="9" t="s">
+        <v>984</v>
+      </c>
+      <c r="AD143" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+      <c r="AG143" s="7"/>
+      <c r="AH143" s="7"/>
+      <c r="AI143" s="7"/>
+      <c r="AJ143" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK143" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2026012512</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3">
+        <v>5401</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T144" s="3">
+        <v>1</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="X144" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="Y144" s="3"/>
+      <c r="Z144" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC144" s="10" t="s">
+        <v>990</v>
+      </c>
+      <c r="AD144" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE144" s="3"/>
+      <c r="AF144" s="3"/>
+      <c r="AG144" s="3"/>
+      <c r="AH144" s="3"/>
+      <c r="AI144" s="3"/>
+      <c r="AJ144" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK144" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="1:37">
+      <c r="A145" s="7">
+        <v>143</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C145" s="7">
+        <v>2026012518</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7">
+        <v>4770</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I145" s="7"/>
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="7"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="R145" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S145" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T145" s="7">
+        <v>1</v>
+      </c>
+      <c r="U145" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V145" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="W145" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="X145" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="Y145" s="7"/>
+      <c r="Z145" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA145" s="7"/>
+      <c r="AB145" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC145" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD145" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE145" s="7"/>
+      <c r="AF145" s="7"/>
+      <c r="AG145" s="7"/>
+      <c r="AH145" s="7"/>
+      <c r="AI145" s="7"/>
+      <c r="AJ145" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK145" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:37">
+      <c r="A146" s="3">
+        <v>144</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2026012527</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3">
+        <v>4153</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T146" s="3">
+        <v>1</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="W146" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="X146" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="Y146" s="3"/>
+      <c r="Z146" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA146" s="3"/>
+      <c r="AB146" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC146" s="10" t="s">
+        <v>999</v>
+      </c>
+      <c r="AD146" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE146" s="3"/>
+      <c r="AF146" s="3"/>
+      <c r="AG146" s="3"/>
+      <c r="AH146" s="3"/>
+      <c r="AI146" s="3"/>
+      <c r="AJ146" s="3"/>
+      <c r="AK146" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:37">
+      <c r="A147" s="7">
+        <v>145</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2026012538</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7">
+        <v>2749</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I147" s="7"/>
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="7"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="R147" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S147" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T147" s="7">
+        <v>1</v>
+      </c>
+      <c r="U147" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V147" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="W147" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="X147" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y147" s="7"/>
+      <c r="Z147" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA147" s="7"/>
+      <c r="AB147" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC147" s="9" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AD147" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE147" s="7"/>
+      <c r="AF147" s="7"/>
+      <c r="AG147" s="7"/>
+      <c r="AH147" s="7"/>
+      <c r="AI147" s="7"/>
+      <c r="AJ147" s="7"/>
+      <c r="AK147" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:37">
+      <c r="A148" s="3">
+        <v>146</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2026012547</v>
+      </c>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3">
+        <v>2237</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S148" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T148" s="3">
+        <v>1</v>
+      </c>
+      <c r="U148" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V148" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="W148" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="X148" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Y148" s="3"/>
+      <c r="Z148" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA148" s="3"/>
+      <c r="AB148" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC148" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AD148" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE148" s="3"/>
+      <c r="AF148" s="3"/>
+      <c r="AG148" s="3"/>
+      <c r="AH148" s="3"/>
+      <c r="AI148" s="3"/>
+      <c r="AJ148" s="3"/>
+      <c r="AK148" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="149" spans="1:37">
+      <c r="A149" s="7">
+        <v>147</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C149" s="7">
+        <v>2026012557</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7">
+        <v>4844</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I149" s="7"/>
+      <c r="J149" s="7"/>
+      <c r="K149" s="7"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="8"/>
+      <c r="N149" s="7"/>
+      <c r="O149" s="8"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="R149" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S149" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T149" s="7">
+        <v>1</v>
+      </c>
+      <c r="U149" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V149" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="W149" s="7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="X149" s="7" t="s">
+        <v>1017</v>
+      </c>
+      <c r="Y149" s="7"/>
+      <c r="Z149" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA149" s="7"/>
+      <c r="AB149" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC149" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="AD149" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE149" s="7"/>
+      <c r="AF149" s="7"/>
+      <c r="AG149" s="7"/>
+      <c r="AH149" s="7"/>
+      <c r="AI149" s="7"/>
+      <c r="AJ149" s="7"/>
+      <c r="AK149" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:37">
+      <c r="A150" s="3">
+        <v>148</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2026012570</v>
+      </c>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3">
+        <v>5080</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="10"/>
+      <c r="Q150" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="R150" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S150" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T150" s="3">
+        <v>1</v>
+      </c>
+      <c r="U150" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V150" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="W150" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="X150" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Y150" s="3"/>
+      <c r="Z150" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA150" s="3"/>
+      <c r="AB150" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC150" s="10" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AD150" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE150" s="3"/>
+      <c r="AF150" s="3"/>
+      <c r="AG150" s="3"/>
+      <c r="AH150" s="3"/>
+      <c r="AI150" s="3"/>
+      <c r="AJ150" s="3"/>
+      <c r="AK150" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="151" spans="1:37">
+      <c r="A151" s="7">
+        <v>149</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C151" s="7">
+        <v>2026012586</v>
+      </c>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7">
+        <v>4739</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I151" s="7"/>
+      <c r="J151" s="7"/>
+      <c r="K151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="8"/>
+      <c r="N151" s="7"/>
+      <c r="O151" s="8"/>
+      <c r="P151" s="8"/>
+      <c r="Q151" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="R151" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S151" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T151" s="7">
+        <v>1</v>
+      </c>
+      <c r="U151" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V151" s="7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="W151" s="7" t="s">
+        <v>1027</v>
+      </c>
+      <c r="X151" s="7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="Y151" s="7"/>
+      <c r="Z151" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC151" s="8" t="s">
+        <v>1029</v>
+      </c>
+      <c r="AD151" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE151" s="7"/>
+      <c r="AF151" s="7"/>
+      <c r="AG151" s="7"/>
+      <c r="AH151" s="7"/>
+      <c r="AI151" s="7"/>
+      <c r="AJ151" s="7"/>
+      <c r="AK151" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Auto commit - 01201730
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$151</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$162</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1103">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-20  )</t>
   </si>
@@ -3124,6 +3124,42 @@
     <t>PMQ1+7210002887</t>
   </si>
   <si>
+    <t>ED057115011901</t>
+  </si>
+  <si>
+    <t>D057</t>
+  </si>
+  <si>
+    <t>北縣溪尾二店</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:34:25</t>
+  </si>
+  <si>
+    <t>切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應mmk熱感機(t70ii)無法正常切紙切不斷，門市已有重裝紙捲重開機測試仍異常....須請台芝到店協助(不正常)</t>
+  </si>
+  <si>
+    <t>THILF0D057</t>
+  </si>
+  <si>
+    <t>2026-01-19 14:43:18</t>
+  </si>
+  <si>
+    <t>2026-01-20 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 14:15:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 18:43:00</t>
+  </si>
+  <si>
+    <t>換下8138001797換上8138003161</t>
+  </si>
+  <si>
     <t>三芝芝蘭店</t>
   </si>
   <si>
@@ -3194,6 +3230,195 @@
   </si>
   <si>
     <t>PMQ1+7210003044</t>
+  </si>
+  <si>
+    <t>E2209115012001</t>
+  </si>
+  <si>
+    <t>2026-01-20 08:09:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm2 ccd掃描器(HC76TR)近期常發生刷讀不到條碼有亮燈有逼聲但未讀進tm，門市已有操作校正仍異常且查看輸入顯示有鼠標....須請台芝到店協助(機2 指標已在輸入顯示處掃描商品無反應.)
+01/20 09:05  請門市操作掃描器校正，稍晚聯繫...廖
+</t>
+  </si>
+  <si>
+    <t>2026-01-20 09:22:55</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:15:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 13:22:00</t>
+  </si>
+  <si>
+    <t>重新校正掃槍</t>
+  </si>
+  <si>
+    <t>12014115012002</t>
+  </si>
+  <si>
+    <t>三重果菜市場</t>
+  </si>
+  <si>
+    <t>2026-01-20 11:24:25</t>
+  </si>
+  <si>
+    <t>01/20 11:26 啟動緊急叫修:門市反應SC(SHUTTLE6S)突然自己關機無法開機，PING1不通無法VNC，按開機鍵無反應未亮燈，門市找不到電源插頭可拔插....須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到01/19，與通訊功評確認都有收到</t>
+  </si>
+  <si>
+    <t>THILF02014</t>
+  </si>
+  <si>
+    <t>2026-01-20 11:32:15</t>
+  </si>
+  <si>
+    <t>2026-01-20 12:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 12:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 17:32:00</t>
+  </si>
+  <si>
+    <t>更換電源插座.重新差拔sc主機.變壓器</t>
+  </si>
+  <si>
+    <t>2026-01-20 12:40:28</t>
+  </si>
+  <si>
+    <t>2026-01-20 12:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 12:36:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002757</t>
+  </si>
+  <si>
+    <t>15457115012002</t>
+  </si>
+  <si>
+    <t>2026-01-20 13:11:01</t>
+  </si>
+  <si>
+    <t>01/20 13:11 啟動緊急叫修:門市反應sc(SHUTTLE6S)無法正常開機畫面黑屏，請門市查看電源燈有亮但無畫面ping1不通無法vnc。請門市更換插座、拔插休息開機仍異常電源燈有亮但未正常開機，....須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到01/20，待與通訊確認</t>
+  </si>
+  <si>
+    <t>2026-01-20 13:14:24</t>
+  </si>
+  <si>
+    <t>2026-01-20 13:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 13:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 19:14:00</t>
+  </si>
+  <si>
+    <t>SC散熱口物品堵住，重新擺放後開機正常</t>
+  </si>
+  <si>
+    <t>2026-01-20 14:35:17</t>
+  </si>
+  <si>
+    <t>2026-01-20 14:35:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002816</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:14:05</t>
+  </si>
+  <si>
+    <t>2026-01-20 14:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:05:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002759</t>
+  </si>
+  <si>
+    <t>永和頂溪站</t>
+  </si>
+  <si>
+    <t>THILF02941</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:51:32</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002986</t>
+  </si>
+  <si>
+    <t>永和永霖店</t>
+  </si>
+  <si>
+    <t>THILF04019</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:12:02</t>
+  </si>
+  <si>
+    <t>2026-01-20 15:54:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:12:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002990</t>
+  </si>
+  <si>
+    <t>永和福和花園</t>
+  </si>
+  <si>
+    <t>THILF03082</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:41:08</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:21:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002987</t>
+  </si>
+  <si>
+    <t>永和貞寧店</t>
+  </si>
+  <si>
+    <t>THILF03968</t>
+  </si>
+  <si>
+    <t>2026-01-20 17:09:29</t>
+  </si>
+  <si>
+    <t>2026-01-20 16:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 17:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002989</t>
   </si>
 </sst>
 </file>
@@ -3607,10 +3832,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK151"/>
+  <dimension ref="A1:AK162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A151" sqref="A151"/>
+      <selection activeCell="AC159" sqref="AC159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16296,38 +16521,58 @@
         <v>146</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C148" s="3">
-        <v>2026012547</v>
-      </c>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3">
-        <v>2237</v>
+        <v>2026012544</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>1007</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I148" s="3"/>
-      <c r="J148" s="3"/>
-      <c r="K148" s="3"/>
-      <c r="L148" s="3"/>
-      <c r="M148" s="4"/>
-      <c r="N148" s="3"/>
-      <c r="O148" s="4"/>
-      <c r="P148" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M148" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="N148" s="3">
+        <v>5901</v>
+      </c>
+      <c r="O148" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P148" s="10" t="s">
+        <v>1011</v>
+      </c>
       <c r="Q148" s="3" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="R148" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S148" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T148" s="3">
         <v>1</v>
@@ -16336,15 +16581,17 @@
         <v>53</v>
       </c>
       <c r="V148" s="3" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="W148" s="3" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="X148" s="3" t="s">
-        <v>1011</v>
-      </c>
-      <c r="Y148" s="3"/>
+        <v>1015</v>
+      </c>
+      <c r="Y148" s="3" t="s">
+        <v>1016</v>
+      </c>
       <c r="Z148" s="3">
         <v>0.3</v>
       </c>
@@ -16353,11 +16600,9 @@
         <v>58</v>
       </c>
       <c r="AC148" s="10" t="s">
-        <v>1012</v>
-      </c>
-      <c r="AD148" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>1017</v>
+      </c>
+      <c r="AD148" s="3"/>
       <c r="AE148" s="3"/>
       <c r="AF148" s="3"/>
       <c r="AG148" s="3"/>
@@ -16376,18 +16621,18 @@
         <v>118</v>
       </c>
       <c r="C149" s="7">
-        <v>2026012557</v>
+        <v>2026012547</v>
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
       <c r="F149" s="7">
-        <v>4844</v>
+        <v>2237</v>
       </c>
       <c r="G149" s="7" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>1007</v>
+        <v>1019</v>
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -16398,7 +16643,7 @@
       <c r="O149" s="8"/>
       <c r="P149" s="9"/>
       <c r="Q149" s="7" t="s">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="R149" s="7" t="s">
         <v>51</v>
@@ -16413,13 +16658,13 @@
         <v>53</v>
       </c>
       <c r="V149" s="7" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="W149" s="7" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="X149" s="7" t="s">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="Y149" s="7"/>
       <c r="Z149" s="7">
@@ -16430,7 +16675,7 @@
         <v>58</v>
       </c>
       <c r="AC149" s="9" t="s">
-        <v>1018</v>
+        <v>1024</v>
       </c>
       <c r="AD149" s="7" t="s">
         <v>60</v>
@@ -16453,18 +16698,18 @@
         <v>118</v>
       </c>
       <c r="C150" s="3">
-        <v>2026012570</v>
+        <v>2026012557</v>
       </c>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3">
-        <v>5080</v>
+        <v>4844</v>
       </c>
       <c r="G150" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H150" s="3" t="s">
         <v>1019</v>
-      </c>
-      <c r="H150" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -16475,7 +16720,7 @@
       <c r="O150" s="4"/>
       <c r="P150" s="10"/>
       <c r="Q150" s="3" t="s">
-        <v>1020</v>
+        <v>1026</v>
       </c>
       <c r="R150" s="3" t="s">
         <v>51</v>
@@ -16490,13 +16735,13 @@
         <v>53</v>
       </c>
       <c r="V150" s="3" t="s">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="W150" s="3" t="s">
-        <v>933</v>
+        <v>1028</v>
       </c>
       <c r="X150" s="3" t="s">
-        <v>1022</v>
+        <v>1029</v>
       </c>
       <c r="Y150" s="3"/>
       <c r="Z150" s="3">
@@ -16507,7 +16752,7 @@
         <v>58</v>
       </c>
       <c r="AC150" s="10" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
       <c r="AD150" s="3" t="s">
         <v>60</v>
@@ -16530,18 +16775,18 @@
         <v>118</v>
       </c>
       <c r="C151" s="7">
-        <v>2026012586</v>
+        <v>2026012570</v>
       </c>
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
       <c r="F151" s="7">
-        <v>4739</v>
+        <v>5080</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>1024</v>
+        <v>1031</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>154</v>
+        <v>1019</v>
       </c>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
@@ -16550,9 +16795,9 @@
       <c r="M151" s="8"/>
       <c r="N151" s="7"/>
       <c r="O151" s="8"/>
-      <c r="P151" s="8"/>
+      <c r="P151" s="9"/>
       <c r="Q151" s="7" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="R151" s="7" t="s">
         <v>51</v>
@@ -16567,24 +16812,24 @@
         <v>53</v>
       </c>
       <c r="V151" s="7" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
       <c r="W151" s="7" t="s">
-        <v>1027</v>
+        <v>933</v>
       </c>
       <c r="X151" s="7" t="s">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="Y151" s="7"/>
       <c r="Z151" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA151" s="7"/>
       <c r="AB151" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC151" s="8" t="s">
-        <v>1029</v>
+      <c r="AC151" s="9" t="s">
+        <v>1035</v>
       </c>
       <c r="AD151" s="7" t="s">
         <v>60</v>
@@ -16596,6 +16841,921 @@
       <c r="AI151" s="7"/>
       <c r="AJ151" s="7"/>
       <c r="AK151" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:37">
+      <c r="A152" s="3">
+        <v>150</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2026012586</v>
+      </c>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3">
+        <v>4739</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="3"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="10"/>
+      <c r="Q152" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S152" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T152" s="3">
+        <v>1</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V152" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="X152" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Y152" s="3"/>
+      <c r="Z152" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA152" s="3"/>
+      <c r="AB152" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC152" s="10" t="s">
+        <v>1041</v>
+      </c>
+      <c r="AD152" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE152" s="3"/>
+      <c r="AF152" s="3"/>
+      <c r="AG152" s="3"/>
+      <c r="AH152" s="3"/>
+      <c r="AI152" s="3"/>
+      <c r="AJ152" s="3"/>
+      <c r="AK152" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:37">
+      <c r="A153" s="7">
+        <v>151</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C153" s="7">
+        <v>2026012616</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F153" s="7">
+        <v>2209</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I153" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="J153" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K153" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L153" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M153" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="N153" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O153" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="P153" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="Q153" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="R153" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S153" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T153" s="7">
+        <v>1</v>
+      </c>
+      <c r="U153" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V153" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="W153" s="7" t="s">
+        <v>1046</v>
+      </c>
+      <c r="X153" s="7" t="s">
+        <v>1047</v>
+      </c>
+      <c r="Y153" s="7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Z153" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AA153" s="7"/>
+      <c r="AB153" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC153" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AD153" s="7"/>
+      <c r="AE153" s="7"/>
+      <c r="AF153" s="7"/>
+      <c r="AG153" s="7"/>
+      <c r="AH153" s="7"/>
+      <c r="AI153" s="7"/>
+      <c r="AJ153" s="7"/>
+      <c r="AK153" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:37">
+      <c r="A154" s="3">
+        <v>152</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2026012672</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F154" s="3">
+        <v>2014</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M154" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="N154" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O154" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P154" s="10" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Q154" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="R154" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S154" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T154" s="3">
+        <v>1</v>
+      </c>
+      <c r="U154" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V154" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="W154" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="X154" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Y154" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Z154" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA154" s="3"/>
+      <c r="AB154" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC154" s="10" t="s">
+        <v>1059</v>
+      </c>
+      <c r="AD154" s="3"/>
+      <c r="AE154" s="3"/>
+      <c r="AF154" s="3"/>
+      <c r="AG154" s="3"/>
+      <c r="AH154" s="3"/>
+      <c r="AI154" s="3"/>
+      <c r="AJ154" s="3"/>
+      <c r="AK154" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:37">
+      <c r="A155" s="7">
+        <v>153</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C155" s="7">
+        <v>2026012694</v>
+      </c>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7">
+        <v>2014</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I155" s="7"/>
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="8"/>
+      <c r="N155" s="7"/>
+      <c r="O155" s="8"/>
+      <c r="P155" s="9"/>
+      <c r="Q155" s="7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="R155" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S155" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T155" s="7">
+        <v>1</v>
+      </c>
+      <c r="U155" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V155" s="7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="W155" s="7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="X155" s="7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="Y155" s="7"/>
+      <c r="Z155" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC155" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AD155" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE155" s="7"/>
+      <c r="AF155" s="7"/>
+      <c r="AG155" s="7"/>
+      <c r="AH155" s="7"/>
+      <c r="AI155" s="7"/>
+      <c r="AJ155" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK155" s="7"/>
+    </row>
+    <row r="156" spans="1:37">
+      <c r="A156" s="3">
+        <v>154</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" s="3">
+        <v>2026012703</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F156" s="3">
+        <v>5457</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L156" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M156" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="N156" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O156" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="P156" s="10" t="s">
+        <v>1066</v>
+      </c>
+      <c r="Q156" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="R156" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S156" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T156" s="3">
+        <v>1</v>
+      </c>
+      <c r="U156" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V156" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="W156" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="X156" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Y156" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Z156" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA156" s="3"/>
+      <c r="AB156" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC156" s="10" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AD156" s="3"/>
+      <c r="AE156" s="3"/>
+      <c r="AF156" s="3"/>
+      <c r="AG156" s="3"/>
+      <c r="AH156" s="3"/>
+      <c r="AI156" s="3"/>
+      <c r="AJ156" s="3"/>
+      <c r="AK156" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:37">
+      <c r="A157" s="7">
+        <v>155</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C157" s="7">
+        <v>2026012747</v>
+      </c>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I157" s="7"/>
+      <c r="J157" s="7"/>
+      <c r="K157" s="7"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="8"/>
+      <c r="N157" s="7"/>
+      <c r="O157" s="8"/>
+      <c r="P157" s="9"/>
+      <c r="Q157" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R157" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S157" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T157" s="7">
+        <v>1</v>
+      </c>
+      <c r="U157" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V157" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="W157" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="X157" s="7" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Y157" s="7"/>
+      <c r="Z157" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA157" s="7"/>
+      <c r="AB157" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC157" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="AD157" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE157" s="7"/>
+      <c r="AF157" s="7"/>
+      <c r="AG157" s="7"/>
+      <c r="AH157" s="7"/>
+      <c r="AI157" s="7"/>
+      <c r="AJ157" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK157" s="7"/>
+    </row>
+    <row r="158" spans="1:37">
+      <c r="A158" s="3">
+        <v>156</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C158" s="3">
+        <v>2026012767</v>
+      </c>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3">
+        <v>2209</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I158" s="3"/>
+      <c r="J158" s="3"/>
+      <c r="K158" s="3"/>
+      <c r="L158" s="3"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="3"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="10"/>
+      <c r="Q158" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="R158" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S158" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T158" s="3">
+        <v>1</v>
+      </c>
+      <c r="U158" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V158" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="W158" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="X158" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Y158" s="3"/>
+      <c r="Z158" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA158" s="3"/>
+      <c r="AB158" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC158" s="10" t="s">
+        <v>1078</v>
+      </c>
+      <c r="AD158" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE158" s="3"/>
+      <c r="AF158" s="3"/>
+      <c r="AG158" s="3"/>
+      <c r="AH158" s="3"/>
+      <c r="AI158" s="3"/>
+      <c r="AJ158" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK158" s="3"/>
+    </row>
+    <row r="159" spans="1:37">
+      <c r="A159" s="7">
+        <v>157</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C159" s="7">
+        <v>2026012773</v>
+      </c>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7">
+        <v>2941</v>
+      </c>
+      <c r="G159" s="7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H159" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="I159" s="7"/>
+      <c r="J159" s="7"/>
+      <c r="K159" s="7"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="8"/>
+      <c r="N159" s="7"/>
+      <c r="O159" s="8"/>
+      <c r="P159" s="9"/>
+      <c r="Q159" s="7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="R159" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S159" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T159" s="7">
+        <v>1</v>
+      </c>
+      <c r="U159" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V159" s="7" t="s">
+        <v>1081</v>
+      </c>
+      <c r="W159" s="7" t="s">
+        <v>1082</v>
+      </c>
+      <c r="X159" s="7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Y159" s="7"/>
+      <c r="Z159" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA159" s="7"/>
+      <c r="AB159" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC159" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AD159" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE159" s="7"/>
+      <c r="AF159" s="7"/>
+      <c r="AG159" s="7"/>
+      <c r="AH159" s="7"/>
+      <c r="AI159" s="7"/>
+      <c r="AJ159" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK159" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:37">
+      <c r="A160" s="3">
+        <v>158</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C160" s="3">
+        <v>2026012796</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3">
+        <v>4019</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="H160" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I160" s="3"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="4"/>
+      <c r="P160" s="10"/>
+      <c r="Q160" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="R160" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S160" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T160" s="3">
+        <v>1</v>
+      </c>
+      <c r="U160" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V160" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="W160" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="X160" s="3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Y160" s="3"/>
+      <c r="Z160" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA160" s="3"/>
+      <c r="AB160" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC160" s="10" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AD160" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE160" s="3"/>
+      <c r="AF160" s="3"/>
+      <c r="AG160" s="3"/>
+      <c r="AH160" s="3"/>
+      <c r="AI160" s="3"/>
+      <c r="AJ160" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK160" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:37">
+      <c r="A161" s="7">
+        <v>159</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C161" s="7">
+        <v>2026012804</v>
+      </c>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7">
+        <v>3082</v>
+      </c>
+      <c r="G161" s="7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="H161" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="I161" s="7"/>
+      <c r="J161" s="7"/>
+      <c r="K161" s="7"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="8"/>
+      <c r="N161" s="7"/>
+      <c r="O161" s="8"/>
+      <c r="P161" s="9"/>
+      <c r="Q161" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="R161" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S161" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T161" s="7">
+        <v>1</v>
+      </c>
+      <c r="U161" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V161" s="7" t="s">
+        <v>1093</v>
+      </c>
+      <c r="W161" s="7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="X161" s="7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Y161" s="7"/>
+      <c r="Z161" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA161" s="7"/>
+      <c r="AB161" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC161" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AD161" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE161" s="7"/>
+      <c r="AF161" s="7"/>
+      <c r="AG161" s="7"/>
+      <c r="AH161" s="7"/>
+      <c r="AI161" s="7"/>
+      <c r="AJ161" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK161" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:37">
+      <c r="A162" s="3">
+        <v>160</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C162" s="3">
+        <v>2026012817</v>
+      </c>
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3">
+        <v>3968</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I162" s="3"/>
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="3"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="3"/>
+      <c r="O162" s="4"/>
+      <c r="P162" s="4"/>
+      <c r="Q162" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="R162" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S162" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T162" s="3">
+        <v>1</v>
+      </c>
+      <c r="U162" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V162" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="W162" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="X162" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="Y162" s="3"/>
+      <c r="Z162" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA162" s="3"/>
+      <c r="AB162" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC162" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="AD162" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE162" s="3"/>
+      <c r="AF162" s="3"/>
+      <c r="AG162" s="3"/>
+      <c r="AH162" s="3"/>
+      <c r="AI162" s="3"/>
+      <c r="AJ162" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK162" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01211447
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$162</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$164</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1103">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-20  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1115">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-21  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3419,6 +3419,42 @@
   </si>
   <si>
     <t>PMQ1+7210002989</t>
+  </si>
+  <si>
+    <t>中和一品苑</t>
+  </si>
+  <si>
+    <t>THILF04970</t>
+  </si>
+  <si>
+    <t>2026-01-20 18:24:40</t>
+  </si>
+  <si>
+    <t>2026-01-20 17:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-20 17:45:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002975</t>
+  </si>
+  <si>
+    <t>蘆竹坑口店</t>
+  </si>
+  <si>
+    <t>THILF02315</t>
+  </si>
+  <si>
+    <t>2026-01-21 13:54:51</t>
+  </si>
+  <si>
+    <t>2026-01-21 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002723+L90</t>
   </si>
 </sst>
 </file>
@@ -3832,10 +3868,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK162"/>
+  <dimension ref="A1:AK164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC159" sqref="AC159"/>
+      <selection activeCell="AC161" sqref="AC161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17708,7 +17744,7 @@
       <c r="M162" s="4"/>
       <c r="N162" s="3"/>
       <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
+      <c r="P162" s="10"/>
       <c r="Q162" s="3" t="s">
         <v>1098</v>
       </c>
@@ -17741,7 +17777,7 @@
       <c r="AB162" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC162" s="4" t="s">
+      <c r="AC162" s="10" t="s">
         <v>1102</v>
       </c>
       <c r="AD162" s="3" t="s">
@@ -17756,6 +17792,162 @@
         <v>60</v>
       </c>
       <c r="AK162" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="163" spans="1:37">
+      <c r="A163" s="7">
+        <v>161</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C163" s="7">
+        <v>2026012830</v>
+      </c>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7">
+        <v>4970</v>
+      </c>
+      <c r="G163" s="7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="H163" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I163" s="7"/>
+      <c r="J163" s="7"/>
+      <c r="K163" s="7"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="8"/>
+      <c r="N163" s="7"/>
+      <c r="O163" s="8"/>
+      <c r="P163" s="9"/>
+      <c r="Q163" s="7" t="s">
+        <v>1104</v>
+      </c>
+      <c r="R163" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S163" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T163" s="7">
+        <v>1</v>
+      </c>
+      <c r="U163" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V163" s="7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="W163" s="7" t="s">
+        <v>1106</v>
+      </c>
+      <c r="X163" s="7" t="s">
+        <v>1107</v>
+      </c>
+      <c r="Y163" s="7"/>
+      <c r="Z163" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA163" s="7"/>
+      <c r="AB163" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC163" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AD163" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE163" s="7"/>
+      <c r="AF163" s="7"/>
+      <c r="AG163" s="7"/>
+      <c r="AH163" s="7"/>
+      <c r="AI163" s="7"/>
+      <c r="AJ163" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK163" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="164" spans="1:37">
+      <c r="A164" s="3">
+        <v>162</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C164" s="3">
+        <v>2026012895</v>
+      </c>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3">
+        <v>2315</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I164" s="3"/>
+      <c r="J164" s="3"/>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="3"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="R164" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S164" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T164" s="3">
+        <v>1</v>
+      </c>
+      <c r="U164" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V164" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="W164" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="X164" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="Y164" s="3"/>
+      <c r="Z164" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA164" s="3"/>
+      <c r="AB164" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC164" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AD164" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE164" s="3"/>
+      <c r="AF164" s="3"/>
+      <c r="AG164" s="3"/>
+      <c r="AH164" s="3"/>
+      <c r="AI164" s="3"/>
+      <c r="AJ164" s="3"/>
+      <c r="AK164" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01211737
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$164</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$171</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1157">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-21  )</t>
   </si>
@@ -3439,6 +3439,60 @@
     <t>PMQ1+7210002975</t>
   </si>
   <si>
+    <t>E4191115012001</t>
+  </si>
+  <si>
+    <t>2026-01-20 19:23:53</t>
+  </si>
+  <si>
+    <t>HL29</t>
+  </si>
+  <si>
+    <t>HL-CCD掃描器(SC)</t>
+  </si>
+  <si>
+    <t>性質轉換:門市反應SC掃描器(AT20B)按鈕卡住...需請台芝到店協助(感應不良)</t>
+  </si>
+  <si>
+    <t>2026-01-20 19:31:26</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:55:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 23:31:00</t>
+  </si>
+  <si>
+    <t>換下8119012116 換上8119013590</t>
+  </si>
+  <si>
+    <t>14191115012001</t>
+  </si>
+  <si>
+    <t>2026-01-20 19:31:42</t>
+  </si>
+  <si>
+    <t>鍵盤按鍵不良或無反應</t>
+  </si>
+  <si>
+    <t>性質轉換:門市反應SC(SHUTTLE6S)鍵盤的上下鍵有時按了都沒反應，已有重新拔插線路仍異常...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-20 19:34:39</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:16:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 23:34:00</t>
+  </si>
+  <si>
+    <t>更換鍵盤</t>
+  </si>
+  <si>
     <t>蘆竹坑口店</t>
   </si>
   <si>
@@ -3455,6 +3509,78 @@
   </si>
   <si>
     <t>PMQ1+7210002723+L90</t>
+  </si>
+  <si>
+    <t>L565</t>
+  </si>
+  <si>
+    <t>匯躍蘆竹店</t>
+  </si>
+  <si>
+    <t>THILF0L565</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:20:20</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:10:00</t>
+  </si>
+  <si>
+    <t>三重義天店</t>
+  </si>
+  <si>
+    <t>THILF02222</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:48:27</t>
+  </si>
+  <si>
+    <t>2026-01-21 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:30:00</t>
+  </si>
+  <si>
+    <t>回裝門市已完工 已請0800確認版本</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:54:25</t>
+  </si>
+  <si>
+    <t>協助回裝</t>
+  </si>
+  <si>
+    <t>蘆竹海湖店</t>
+  </si>
+  <si>
+    <t>THILF04572</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:54:49</t>
+  </si>
+  <si>
+    <t>2026-01-21 15:50:00</t>
+  </si>
+  <si>
+    <t>L556</t>
+  </si>
+  <si>
+    <t>蘆竹揚耀店</t>
+  </si>
+  <si>
+    <t>THILF0L556</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:20:46</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:20:00</t>
   </si>
 </sst>
 </file>
@@ -3868,10 +3994,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK164"/>
+  <dimension ref="A1:AK171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC161" sqref="AC161"/>
+      <selection activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17879,38 +18005,58 @@
         <v>162</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C164" s="3">
-        <v>2026012895</v>
-      </c>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
+        <v>2026012831</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F164" s="3">
-        <v>2315</v>
+        <v>4191</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>1109</v>
+        <v>527</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I164" s="3"/>
-      <c r="J164" s="3"/>
-      <c r="K164" s="3"/>
-      <c r="L164" s="3"/>
-      <c r="M164" s="4"/>
-      <c r="N164" s="3"/>
-      <c r="O164" s="4"/>
-      <c r="P164" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="L164" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="M164" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="N164" s="3">
+        <v>2901</v>
+      </c>
+      <c r="O164" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P164" s="10" t="s">
+        <v>1113</v>
+      </c>
       <c r="Q164" s="3" t="s">
-        <v>1110</v>
+        <v>530</v>
       </c>
       <c r="R164" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S164" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T164" s="3">
         <v>1</v>
@@ -17919,15 +18065,17 @@
         <v>53</v>
       </c>
       <c r="V164" s="3" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="W164" s="3" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="X164" s="3" t="s">
-        <v>1113</v>
-      </c>
-      <c r="Y164" s="3"/>
+        <v>1116</v>
+      </c>
+      <c r="Y164" s="3" t="s">
+        <v>1117</v>
+      </c>
       <c r="Z164" s="3">
         <v>0.3</v>
       </c>
@@ -17935,12 +18083,10 @@
       <c r="AB164" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC164" s="4" t="s">
-        <v>1114</v>
-      </c>
-      <c r="AD164" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC164" s="10" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AD164" s="3"/>
       <c r="AE164" s="3"/>
       <c r="AF164" s="3"/>
       <c r="AG164" s="3"/>
@@ -17948,6 +18094,565 @@
       <c r="AI164" s="3"/>
       <c r="AJ164" s="3"/>
       <c r="AK164" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="165" spans="1:37">
+      <c r="A165" s="7">
+        <v>163</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C165" s="7">
+        <v>2026012832</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F165" s="7">
+        <v>4191</v>
+      </c>
+      <c r="G165" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H165" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I165" s="7" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J165" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K165" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="L165" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="M165" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="N165" s="7">
+        <v>2402</v>
+      </c>
+      <c r="O165" s="8" t="s">
+        <v>1121</v>
+      </c>
+      <c r="P165" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="Q165" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="R165" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S165" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T165" s="7">
+        <v>1</v>
+      </c>
+      <c r="U165" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V165" s="7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="W165" s="7" t="s">
+        <v>1116</v>
+      </c>
+      <c r="X165" s="7" t="s">
+        <v>1124</v>
+      </c>
+      <c r="Y165" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="Z165" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA165" s="7"/>
+      <c r="AB165" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC165" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AD165" s="7"/>
+      <c r="AE165" s="7"/>
+      <c r="AF165" s="7"/>
+      <c r="AG165" s="7"/>
+      <c r="AH165" s="7"/>
+      <c r="AI165" s="7"/>
+      <c r="AJ165" s="7"/>
+      <c r="AK165" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="166" spans="1:37">
+      <c r="A166" s="3">
+        <v>164</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C166" s="3">
+        <v>2026012895</v>
+      </c>
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3">
+        <v>2315</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+      <c r="L166" s="3"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="3"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="10"/>
+      <c r="Q166" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="R166" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S166" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T166" s="3">
+        <v>1</v>
+      </c>
+      <c r="U166" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V166" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="W166" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="X166" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="Y166" s="3"/>
+      <c r="Z166" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA166" s="3"/>
+      <c r="AB166" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC166" s="10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AD166" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE166" s="3"/>
+      <c r="AF166" s="3"/>
+      <c r="AG166" s="3"/>
+      <c r="AH166" s="3"/>
+      <c r="AI166" s="3"/>
+      <c r="AJ166" s="3"/>
+      <c r="AK166" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="167" spans="1:37">
+      <c r="A167" s="7">
+        <v>165</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C167" s="7">
+        <v>2026012907</v>
+      </c>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7"/>
+      <c r="F167" s="7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G167" s="7" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H167" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I167" s="7"/>
+      <c r="J167" s="7"/>
+      <c r="K167" s="7"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="8"/>
+      <c r="N167" s="7"/>
+      <c r="O167" s="8"/>
+      <c r="P167" s="9"/>
+      <c r="Q167" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="R167" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S167" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T167" s="7">
+        <v>1</v>
+      </c>
+      <c r="U167" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V167" s="7" t="s">
+        <v>1136</v>
+      </c>
+      <c r="W167" s="7" t="s">
+        <v>1137</v>
+      </c>
+      <c r="X167" s="7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="Y167" s="7"/>
+      <c r="Z167" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA167" s="7"/>
+      <c r="AB167" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC167" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD167" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE167" s="7"/>
+      <c r="AF167" s="7"/>
+      <c r="AG167" s="7"/>
+      <c r="AH167" s="7"/>
+      <c r="AI167" s="7"/>
+      <c r="AJ167" s="7"/>
+      <c r="AK167" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="168" spans="1:37">
+      <c r="A168" s="3">
+        <v>166</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C168" s="3">
+        <v>2026012913</v>
+      </c>
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3">
+        <v>2222</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I168" s="3"/>
+      <c r="J168" s="3"/>
+      <c r="K168" s="3"/>
+      <c r="L168" s="3"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="3"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="10"/>
+      <c r="Q168" s="3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="R168" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S168" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T168" s="3">
+        <v>1</v>
+      </c>
+      <c r="U168" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V168" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="W168" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="X168" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Y168" s="3"/>
+      <c r="Z168" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="AA168" s="3"/>
+      <c r="AB168" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC168" s="10" t="s">
+        <v>1144</v>
+      </c>
+      <c r="AD168" s="3"/>
+      <c r="AE168" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF168" s="3"/>
+      <c r="AG168" s="3"/>
+      <c r="AH168" s="3"/>
+      <c r="AI168" s="3"/>
+      <c r="AJ168" s="3"/>
+      <c r="AK168" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="1:37">
+      <c r="A169" s="7">
+        <v>167</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C169" s="7">
+        <v>2026012916</v>
+      </c>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
+      <c r="F169" s="7">
+        <v>2222</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H169" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I169" s="7"/>
+      <c r="J169" s="7"/>
+      <c r="K169" s="7"/>
+      <c r="L169" s="7"/>
+      <c r="M169" s="8"/>
+      <c r="N169" s="7"/>
+      <c r="O169" s="8"/>
+      <c r="P169" s="9"/>
+      <c r="Q169" s="7" t="s">
+        <v>1140</v>
+      </c>
+      <c r="R169" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S169" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T169" s="7">
+        <v>1</v>
+      </c>
+      <c r="U169" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V169" s="7" t="s">
+        <v>1145</v>
+      </c>
+      <c r="W169" s="7" t="s">
+        <v>1142</v>
+      </c>
+      <c r="X169" s="7" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Y169" s="7"/>
+      <c r="Z169" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="AA169" s="7"/>
+      <c r="AB169" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC169" s="9" t="s">
+        <v>1146</v>
+      </c>
+      <c r="AD169" s="7"/>
+      <c r="AE169" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF169" s="7"/>
+      <c r="AG169" s="7"/>
+      <c r="AH169" s="7"/>
+      <c r="AI169" s="7"/>
+      <c r="AJ169" s="7"/>
+      <c r="AK169" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="170" spans="1:37">
+      <c r="A170" s="3">
+        <v>168</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C170" s="3">
+        <v>2026012917</v>
+      </c>
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3">
+        <v>4572</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I170" s="3"/>
+      <c r="J170" s="3"/>
+      <c r="K170" s="3"/>
+      <c r="L170" s="3"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="3"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="10"/>
+      <c r="Q170" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="R170" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S170" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T170" s="3">
+        <v>1</v>
+      </c>
+      <c r="U170" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V170" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="W170" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="X170" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="Y170" s="3"/>
+      <c r="Z170" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA170" s="3"/>
+      <c r="AB170" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC170" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD170" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE170" s="3"/>
+      <c r="AF170" s="3"/>
+      <c r="AG170" s="3"/>
+      <c r="AH170" s="3"/>
+      <c r="AI170" s="3"/>
+      <c r="AJ170" s="3"/>
+      <c r="AK170" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="171" spans="1:37">
+      <c r="A171" s="7">
+        <v>169</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C171" s="7">
+        <v>2026012930</v>
+      </c>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
+      <c r="F171" s="7" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G171" s="7" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H171" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I171" s="7"/>
+      <c r="J171" s="7"/>
+      <c r="K171" s="7"/>
+      <c r="L171" s="7"/>
+      <c r="M171" s="8"/>
+      <c r="N171" s="7"/>
+      <c r="O171" s="8"/>
+      <c r="P171" s="8"/>
+      <c r="Q171" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="R171" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S171" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T171" s="7">
+        <v>1</v>
+      </c>
+      <c r="U171" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V171" s="7" t="s">
+        <v>1154</v>
+      </c>
+      <c r="W171" s="7" t="s">
+        <v>1155</v>
+      </c>
+      <c r="X171" s="7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Y171" s="7"/>
+      <c r="Z171" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA171" s="7"/>
+      <c r="AB171" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC171" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD171" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE171" s="7"/>
+      <c r="AF171" s="7"/>
+      <c r="AG171" s="7"/>
+      <c r="AH171" s="7"/>
+      <c r="AI171" s="7"/>
+      <c r="AJ171" s="7"/>
+      <c r="AK171" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01231149
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$171</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$191</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1157">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-22  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1278">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-23  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3581,6 +3581,372 @@
   </si>
   <si>
     <t>2026-01-21 16:20:00</t>
+  </si>
+  <si>
+    <t>1D070115012101</t>
+  </si>
+  <si>
+    <t>D070</t>
+  </si>
+  <si>
+    <t>三重重新店</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:24:31</t>
+  </si>
+  <si>
+    <t>執行發票機韌體更新發現TM1(TCX800)的D槽連線不到，請到店更換TM第二顆硬碟，並協助併更新到251118A版本，TM2如果是BSC10II需同步更新到251118A版本。</t>
+  </si>
+  <si>
+    <t>THILF0D070</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:29:11</t>
+  </si>
+  <si>
+    <t>2026-01-22 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 10:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 20:29:00</t>
+  </si>
+  <si>
+    <t>重插清潔.更新發票機251118A版本tm1. Tm2</t>
+  </si>
+  <si>
+    <t>1D057115012101</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:24:05</t>
+  </si>
+  <si>
+    <t>2026-01-21 16:31:55</t>
+  </si>
+  <si>
+    <t>2026-01-22 11:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 12:24:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 20:31:00</t>
+  </si>
+  <si>
+    <t>重新差拔清潔tm1第二顆硬碟. 更新發票機到251118A版本TM1. TM2</t>
+  </si>
+  <si>
+    <t>14352115012201</t>
+  </si>
+  <si>
+    <t>三重公園店</t>
+  </si>
+  <si>
+    <t>2026-01-22 08:43:44</t>
+  </si>
+  <si>
+    <t>TM1(TCX800)執行發票機韌體更新發現TM1的D槽連線不到，請到店更換TM第二顆硬碟，並協助併更新到251118A版本，TM2如果是BSC10II需同步更新到251118A版本。</t>
+  </si>
+  <si>
+    <t>THILF04352</t>
+  </si>
+  <si>
+    <t>2026-01-22 08:59:30</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:39:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 12:59:00</t>
+  </si>
+  <si>
+    <t>Tm1硬碟重新差拔清潔. 更新發票機到251118A版本Tm1. Tm2</t>
+  </si>
+  <si>
+    <t>E4241115012201</t>
+  </si>
+  <si>
+    <t>三重仁義店</t>
+  </si>
+  <si>
+    <t>2026-01-22 07:15:58</t>
+  </si>
+  <si>
+    <t>店長交接 門市反應tm1 CCD掃描器(HC56II-TR)前端膠條脫落導致刷讀也受影響....須請台芝到店協助(櫃台2台的掃描器 刷商品 會很慢 .掃描器最前端的黑色橡膠皮 有點剝落)</t>
+  </si>
+  <si>
+    <t>THILF04241</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:15:11</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 13:15:00</t>
+  </si>
+  <si>
+    <t>換下8119008752.換上8119011800</t>
+  </si>
+  <si>
+    <t>14241115012201</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:15:24</t>
+  </si>
+  <si>
+    <t>店長交接 門市反應tm2 CCD掃描器(HC56II-TR)前端膠條脫落導致刷讀也受影響....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:15:47</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:40:00</t>
+  </si>
+  <si>
+    <t>換下8119008493.換上8119008544</t>
+  </si>
+  <si>
+    <t>E5245115012201</t>
+  </si>
+  <si>
+    <t>三重護山店</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:29:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應sc螢幕(LCD22)會突然黑畫面或閃爍，當下無做任何排除會突然恢復正常，門市告知已有重新拔插螢幕後方線路仍頻繁發生...請台芝到店協助(螢幕會有閃爍頻繁或無畫面，變成全黑)
+</t>
+  </si>
+  <si>
+    <t>THILF05245</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:45:20</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:38:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:55:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 13:45:00</t>
+  </si>
+  <si>
+    <t>更換vgA線</t>
+  </si>
+  <si>
+    <t>12390115012201</t>
+  </si>
+  <si>
+    <t>五股產業園區</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:56:33</t>
+  </si>
+  <si>
+    <t>門市反應sc螢幕(LCD)會不斷閃爍一下變亮一下變暗，門市已有重新拔插後方線路仍異常.....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02390</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:57:47</t>
+  </si>
+  <si>
+    <t>2026-01-22 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 11:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 13:57:00</t>
+  </si>
+  <si>
+    <t>更換螢幕
+換上8133003738
+換下8133000752</t>
+  </si>
+  <si>
+    <t>2026-01-22 11:06:12</t>
+  </si>
+  <si>
+    <t>2026-01-22 09:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002817</t>
+  </si>
+  <si>
+    <t>2026-01-22 11:55:47</t>
+  </si>
+  <si>
+    <t>2026-01-22 12:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002827</t>
+  </si>
+  <si>
+    <t>龜山樂學店</t>
+  </si>
+  <si>
+    <t>THILF04981</t>
+  </si>
+  <si>
+    <t>2026-01-22 12:42:53</t>
+  </si>
+  <si>
+    <t>2026-01-22 12:42:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002713+L90</t>
+  </si>
+  <si>
+    <t>桃縣桃高店</t>
+  </si>
+  <si>
+    <t>THILF02596</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:02:08</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002699+L90</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:14:25</t>
+  </si>
+  <si>
+    <t>2026-01-22 12:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002797</t>
+  </si>
+  <si>
+    <t>龜山復恆店</t>
+  </si>
+  <si>
+    <t>THILF04503</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:40:16</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002707+L90</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:06:29</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:01:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002801</t>
+  </si>
+  <si>
+    <t>龜山樂善店</t>
+  </si>
+  <si>
+    <t>THILF05016</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:51:46</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:51:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002714+L90</t>
+  </si>
+  <si>
+    <t>龜山文化二</t>
+  </si>
+  <si>
+    <t>THILF02428</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:53:28</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:54:59</t>
+  </si>
+  <si>
+    <t>2026-01-22 15:18:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002810</t>
+  </si>
+  <si>
+    <t>龜山玄武店</t>
+  </si>
+  <si>
+    <t>THILF04902</t>
+  </si>
+  <si>
+    <t>2026-01-22 16:18:44</t>
+  </si>
+  <si>
+    <t>2026-01-22 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-22 16:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002711+L90</t>
+  </si>
+  <si>
+    <t>2026-01-22 17:18:04</t>
+  </si>
+  <si>
+    <t>2026-01-22 16:15:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002760</t>
+  </si>
+  <si>
+    <t>新莊頭前公園</t>
+  </si>
+  <si>
+    <t>THILF04228</t>
+  </si>
+  <si>
+    <t>2026-01-23 11:45:47</t>
+  </si>
+  <si>
+    <t>2026-01-23 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 11:30:00</t>
   </si>
 </sst>
 </file>
@@ -3994,10 +4360,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK171"/>
+  <dimension ref="A1:AK191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A171" sqref="A171"/>
+      <selection activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18607,7 +18973,7 @@
       <c r="M171" s="8"/>
       <c r="N171" s="7"/>
       <c r="O171" s="8"/>
-      <c r="P171" s="8"/>
+      <c r="P171" s="9"/>
       <c r="Q171" s="7" t="s">
         <v>1153</v>
       </c>
@@ -18640,7 +19006,7 @@
       <c r="AB171" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC171" s="8" t="s">
+      <c r="AC171" s="9" t="s">
         <v>510</v>
       </c>
       <c r="AD171" s="7" t="s">
@@ -18653,6 +19019,1698 @@
       <c r="AI171" s="7"/>
       <c r="AJ171" s="7"/>
       <c r="AK171" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="172" spans="1:37">
+      <c r="A172" s="3">
+        <v>170</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C172" s="3">
+        <v>2026012931</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L172" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M172" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N172" s="3">
+        <v>2308</v>
+      </c>
+      <c r="O172" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P172" s="10" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Q172" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="R172" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S172" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T172" s="3">
+        <v>1</v>
+      </c>
+      <c r="U172" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V172" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="W172" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="X172" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="Y172" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="Z172" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA172" s="3"/>
+      <c r="AB172" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC172" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="AD172" s="3"/>
+      <c r="AE172" s="3"/>
+      <c r="AF172" s="3"/>
+      <c r="AG172" s="3"/>
+      <c r="AH172" s="3"/>
+      <c r="AI172" s="3"/>
+      <c r="AJ172" s="3"/>
+      <c r="AK172" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="173" spans="1:37">
+      <c r="A173" s="7">
+        <v>171</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C173" s="7">
+        <v>2026012933</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E173" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F173" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G173" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H173" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I173" s="7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J173" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K173" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L173" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M173" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N173" s="7">
+        <v>2308</v>
+      </c>
+      <c r="O173" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="P173" s="9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Q173" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R173" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S173" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T173" s="7">
+        <v>1</v>
+      </c>
+      <c r="U173" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V173" s="7" t="s">
+        <v>1170</v>
+      </c>
+      <c r="W173" s="7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="X173" s="7" t="s">
+        <v>1172</v>
+      </c>
+      <c r="Y173" s="7" t="s">
+        <v>1173</v>
+      </c>
+      <c r="Z173" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA173" s="7"/>
+      <c r="AB173" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC173" s="9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="AD173" s="7"/>
+      <c r="AE173" s="7"/>
+      <c r="AF173" s="7"/>
+      <c r="AG173" s="7"/>
+      <c r="AH173" s="7"/>
+      <c r="AI173" s="7"/>
+      <c r="AJ173" s="7"/>
+      <c r="AK173" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="174" spans="1:37">
+      <c r="A174" s="3">
+        <v>172</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C174" s="3">
+        <v>2026012963</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F174" s="3">
+        <v>4352</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="J174" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K174" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L174" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M174" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N174" s="3">
+        <v>2308</v>
+      </c>
+      <c r="O174" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P174" s="10" t="s">
+        <v>1178</v>
+      </c>
+      <c r="Q174" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="R174" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S174" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T174" s="3">
+        <v>1</v>
+      </c>
+      <c r="U174" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V174" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="W174" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="X174" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="Y174" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="Z174" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA174" s="3"/>
+      <c r="AB174" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC174" s="10" t="s">
+        <v>1184</v>
+      </c>
+      <c r="AD174" s="3"/>
+      <c r="AE174" s="3"/>
+      <c r="AF174" s="3"/>
+      <c r="AG174" s="3"/>
+      <c r="AH174" s="3"/>
+      <c r="AI174" s="3"/>
+      <c r="AJ174" s="3"/>
+      <c r="AK174" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="175" spans="1:37">
+      <c r="A175" s="7">
+        <v>173</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C175" s="7">
+        <v>2026012966</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F175" s="7">
+        <v>4241</v>
+      </c>
+      <c r="G175" s="7" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H175" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I175" s="7" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J175" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K175" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="L175" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M175" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="N175" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O175" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="P175" s="9" t="s">
+        <v>1188</v>
+      </c>
+      <c r="Q175" s="7" t="s">
+        <v>1189</v>
+      </c>
+      <c r="R175" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S175" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T175" s="7">
+        <v>1</v>
+      </c>
+      <c r="U175" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V175" s="7" t="s">
+        <v>1190</v>
+      </c>
+      <c r="W175" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="X175" s="7" t="s">
+        <v>1192</v>
+      </c>
+      <c r="Y175" s="7" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Z175" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA175" s="7"/>
+      <c r="AB175" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC175" s="9" t="s">
+        <v>1194</v>
+      </c>
+      <c r="AD175" s="7"/>
+      <c r="AE175" s="7"/>
+      <c r="AF175" s="7"/>
+      <c r="AG175" s="7"/>
+      <c r="AH175" s="7"/>
+      <c r="AI175" s="7"/>
+      <c r="AJ175" s="7"/>
+      <c r="AK175" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="176" spans="1:37">
+      <c r="A176" s="3">
+        <v>174</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C176" s="3">
+        <v>2026012967</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F176" s="3">
+        <v>4241</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="J176" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L176" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M176" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N176" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O176" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P176" s="10" t="s">
+        <v>1197</v>
+      </c>
+      <c r="Q176" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="R176" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S176" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T176" s="3">
+        <v>1</v>
+      </c>
+      <c r="U176" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V176" s="3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="W176" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="X176" s="3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="Y176" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Z176" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA176" s="3"/>
+      <c r="AB176" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC176" s="10" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AD176" s="3"/>
+      <c r="AE176" s="3"/>
+      <c r="AF176" s="3"/>
+      <c r="AG176" s="3"/>
+      <c r="AH176" s="3"/>
+      <c r="AI176" s="3"/>
+      <c r="AJ176" s="3"/>
+      <c r="AK176" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="177" spans="1:37">
+      <c r="A177" s="7">
+        <v>175</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C177" s="7">
+        <v>2026012973</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F177" s="7">
+        <v>5245</v>
+      </c>
+      <c r="G177" s="7" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H177" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I177" s="7" t="s">
+        <v>1204</v>
+      </c>
+      <c r="J177" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K177" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L177" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M177" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N177" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O177" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P177" s="9" t="s">
+        <v>1205</v>
+      </c>
+      <c r="Q177" s="7" t="s">
+        <v>1206</v>
+      </c>
+      <c r="R177" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S177" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T177" s="7">
+        <v>1</v>
+      </c>
+      <c r="U177" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V177" s="7" t="s">
+        <v>1207</v>
+      </c>
+      <c r="W177" s="7" t="s">
+        <v>1208</v>
+      </c>
+      <c r="X177" s="7" t="s">
+        <v>1209</v>
+      </c>
+      <c r="Y177" s="7" t="s">
+        <v>1210</v>
+      </c>
+      <c r="Z177" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA177" s="7"/>
+      <c r="AB177" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC177" s="9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="AD177" s="7"/>
+      <c r="AE177" s="7"/>
+      <c r="AF177" s="7"/>
+      <c r="AG177" s="7"/>
+      <c r="AH177" s="7"/>
+      <c r="AI177" s="7"/>
+      <c r="AJ177" s="7"/>
+      <c r="AK177" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:37">
+      <c r="A178" s="3">
+        <v>176</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C178" s="3">
+        <v>2026012978</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F178" s="3">
+        <v>2390</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="J178" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K178" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L178" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M178" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N178" s="3">
+        <v>2501</v>
+      </c>
+      <c r="O178" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P178" s="10" t="s">
+        <v>1215</v>
+      </c>
+      <c r="Q178" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="R178" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S178" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T178" s="3">
+        <v>1</v>
+      </c>
+      <c r="U178" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V178" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="W178" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="X178" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="Y178" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="Z178" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA178" s="3"/>
+      <c r="AB178" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC178" s="10" t="s">
+        <v>1221</v>
+      </c>
+      <c r="AD178" s="3"/>
+      <c r="AE178" s="3"/>
+      <c r="AF178" s="3"/>
+      <c r="AG178" s="3"/>
+      <c r="AH178" s="3"/>
+      <c r="AI178" s="3"/>
+      <c r="AJ178" s="3"/>
+      <c r="AK178" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="179" spans="1:37">
+      <c r="A179" s="7">
+        <v>177</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C179" s="7">
+        <v>2026012997</v>
+      </c>
+      <c r="D179" s="7"/>
+      <c r="E179" s="7"/>
+      <c r="F179" s="7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H179" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I179" s="7"/>
+      <c r="J179" s="7"/>
+      <c r="K179" s="7"/>
+      <c r="L179" s="7"/>
+      <c r="M179" s="8"/>
+      <c r="N179" s="7"/>
+      <c r="O179" s="8"/>
+      <c r="P179" s="9"/>
+      <c r="Q179" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="R179" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S179" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T179" s="7">
+        <v>1</v>
+      </c>
+      <c r="U179" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V179" s="7" t="s">
+        <v>1222</v>
+      </c>
+      <c r="W179" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="X179" s="7" t="s">
+        <v>1164</v>
+      </c>
+      <c r="Y179" s="7"/>
+      <c r="Z179" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA179" s="7"/>
+      <c r="AB179" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC179" s="9" t="s">
+        <v>1224</v>
+      </c>
+      <c r="AD179" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE179" s="7"/>
+      <c r="AF179" s="7"/>
+      <c r="AG179" s="7"/>
+      <c r="AH179" s="7"/>
+      <c r="AI179" s="7"/>
+      <c r="AJ179" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK179" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="180" spans="1:37">
+      <c r="A180" s="3">
+        <v>178</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C180" s="3">
+        <v>2026013011</v>
+      </c>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3">
+        <v>2390</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="3"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="3"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="10"/>
+      <c r="Q180" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="R180" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S180" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T180" s="3">
+        <v>1</v>
+      </c>
+      <c r="U180" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V180" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="W180" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="X180" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="Y180" s="3"/>
+      <c r="Z180" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA180" s="3"/>
+      <c r="AB180" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC180" s="10" t="s">
+        <v>1227</v>
+      </c>
+      <c r="AD180" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE180" s="3"/>
+      <c r="AF180" s="3"/>
+      <c r="AG180" s="3"/>
+      <c r="AH180" s="3"/>
+      <c r="AI180" s="3"/>
+      <c r="AJ180" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK180" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="181" spans="1:37">
+      <c r="A181" s="7">
+        <v>179</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C181" s="7">
+        <v>2026013012</v>
+      </c>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7">
+        <v>4981</v>
+      </c>
+      <c r="G181" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H181" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I181" s="7"/>
+      <c r="J181" s="7"/>
+      <c r="K181" s="7"/>
+      <c r="L181" s="7"/>
+      <c r="M181" s="8"/>
+      <c r="N181" s="7"/>
+      <c r="O181" s="8"/>
+      <c r="P181" s="9"/>
+      <c r="Q181" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="R181" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S181" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T181" s="7">
+        <v>1</v>
+      </c>
+      <c r="U181" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V181" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="W181" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="X181" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="Y181" s="7"/>
+      <c r="Z181" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA181" s="7"/>
+      <c r="AB181" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC181" s="9" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AD181" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE181" s="7"/>
+      <c r="AF181" s="7"/>
+      <c r="AG181" s="7"/>
+      <c r="AH181" s="7"/>
+      <c r="AI181" s="7"/>
+      <c r="AJ181" s="7"/>
+      <c r="AK181" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="182" spans="1:37">
+      <c r="A182" s="3">
+        <v>180</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C182" s="3">
+        <v>2026013024</v>
+      </c>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3">
+        <v>2596</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H182" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I182" s="3"/>
+      <c r="J182" s="3"/>
+      <c r="K182" s="3"/>
+      <c r="L182" s="3"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="3"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="10"/>
+      <c r="Q182" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="R182" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S182" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T182" s="3">
+        <v>1</v>
+      </c>
+      <c r="U182" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V182" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="W182" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="X182" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="Y182" s="3"/>
+      <c r="Z182" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA182" s="3"/>
+      <c r="AB182" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC182" s="10" t="s">
+        <v>1237</v>
+      </c>
+      <c r="AD182" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE182" s="3"/>
+      <c r="AF182" s="3"/>
+      <c r="AG182" s="3"/>
+      <c r="AH182" s="3"/>
+      <c r="AI182" s="3"/>
+      <c r="AJ182" s="3"/>
+      <c r="AK182" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="183" spans="1:37">
+      <c r="A183" s="7">
+        <v>181</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C183" s="7">
+        <v>2026013030</v>
+      </c>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7">
+        <v>4241</v>
+      </c>
+      <c r="G183" s="7" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H183" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I183" s="7"/>
+      <c r="J183" s="7"/>
+      <c r="K183" s="7"/>
+      <c r="L183" s="7"/>
+      <c r="M183" s="8"/>
+      <c r="N183" s="7"/>
+      <c r="O183" s="8"/>
+      <c r="P183" s="9"/>
+      <c r="Q183" s="7" t="s">
+        <v>1189</v>
+      </c>
+      <c r="R183" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S183" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T183" s="7">
+        <v>1</v>
+      </c>
+      <c r="U183" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V183" s="7" t="s">
+        <v>1238</v>
+      </c>
+      <c r="W183" s="7" t="s">
+        <v>1239</v>
+      </c>
+      <c r="X183" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Y183" s="7"/>
+      <c r="Z183" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA183" s="7"/>
+      <c r="AB183" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC183" s="9" t="s">
+        <v>1240</v>
+      </c>
+      <c r="AD183" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE183" s="7"/>
+      <c r="AF183" s="7"/>
+      <c r="AG183" s="7"/>
+      <c r="AH183" s="7"/>
+      <c r="AI183" s="7"/>
+      <c r="AJ183" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK183" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="184" spans="1:37">
+      <c r="A184" s="3">
+        <v>182</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C184" s="3">
+        <v>2026013047</v>
+      </c>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3">
+        <v>4503</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H184" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I184" s="3"/>
+      <c r="J184" s="3"/>
+      <c r="K184" s="3"/>
+      <c r="L184" s="3"/>
+      <c r="M184" s="4"/>
+      <c r="N184" s="3"/>
+      <c r="O184" s="4"/>
+      <c r="P184" s="10"/>
+      <c r="Q184" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="R184" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S184" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T184" s="3">
+        <v>1</v>
+      </c>
+      <c r="U184" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V184" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="W184" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="X184" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Y184" s="3"/>
+      <c r="Z184" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA184" s="3"/>
+      <c r="AB184" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC184" s="10" t="s">
+        <v>1246</v>
+      </c>
+      <c r="AD184" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE184" s="3"/>
+      <c r="AF184" s="3"/>
+      <c r="AG184" s="3"/>
+      <c r="AH184" s="3"/>
+      <c r="AI184" s="3"/>
+      <c r="AJ184" s="3"/>
+      <c r="AK184" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="185" spans="1:37">
+      <c r="A185" s="7">
+        <v>183</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C185" s="7">
+        <v>2026013057</v>
+      </c>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7"/>
+      <c r="F185" s="7">
+        <v>4352</v>
+      </c>
+      <c r="G185" s="7" t="s">
+        <v>1176</v>
+      </c>
+      <c r="H185" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I185" s="7"/>
+      <c r="J185" s="7"/>
+      <c r="K185" s="7"/>
+      <c r="L185" s="7"/>
+      <c r="M185" s="8"/>
+      <c r="N185" s="7"/>
+      <c r="O185" s="8"/>
+      <c r="P185" s="9"/>
+      <c r="Q185" s="7" t="s">
+        <v>1179</v>
+      </c>
+      <c r="R185" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S185" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T185" s="7">
+        <v>1</v>
+      </c>
+      <c r="U185" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V185" s="7" t="s">
+        <v>1247</v>
+      </c>
+      <c r="W185" s="7" t="s">
+        <v>1248</v>
+      </c>
+      <c r="X185" s="7" t="s">
+        <v>1249</v>
+      </c>
+      <c r="Y185" s="7"/>
+      <c r="Z185" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA185" s="7"/>
+      <c r="AB185" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC185" s="9" t="s">
+        <v>1250</v>
+      </c>
+      <c r="AD185" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE185" s="7"/>
+      <c r="AF185" s="7"/>
+      <c r="AG185" s="7"/>
+      <c r="AH185" s="7"/>
+      <c r="AI185" s="7"/>
+      <c r="AJ185" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK185" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="186" spans="1:37">
+      <c r="A186" s="3">
+        <v>184</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C186" s="3">
+        <v>2026013075</v>
+      </c>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3">
+        <v>5016</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3"/>
+      <c r="M186" s="4"/>
+      <c r="N186" s="3"/>
+      <c r="O186" s="4"/>
+      <c r="P186" s="10"/>
+      <c r="Q186" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="R186" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S186" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T186" s="3">
+        <v>1</v>
+      </c>
+      <c r="U186" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V186" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="W186" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="X186" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="Y186" s="3"/>
+      <c r="Z186" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA186" s="3"/>
+      <c r="AB186" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC186" s="10" t="s">
+        <v>1256</v>
+      </c>
+      <c r="AD186" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE186" s="3"/>
+      <c r="AF186" s="3"/>
+      <c r="AG186" s="3"/>
+      <c r="AH186" s="3"/>
+      <c r="AI186" s="3"/>
+      <c r="AJ186" s="3"/>
+      <c r="AK186" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="187" spans="1:37">
+      <c r="A187" s="7">
+        <v>185</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C187" s="7">
+        <v>2026013076</v>
+      </c>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7">
+        <v>2428</v>
+      </c>
+      <c r="G187" s="7" t="s">
+        <v>1257</v>
+      </c>
+      <c r="H187" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I187" s="7"/>
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="8"/>
+      <c r="N187" s="7"/>
+      <c r="O187" s="8"/>
+      <c r="P187" s="9"/>
+      <c r="Q187" s="7" t="s">
+        <v>1258</v>
+      </c>
+      <c r="R187" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S187" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T187" s="7">
+        <v>1</v>
+      </c>
+      <c r="U187" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V187" s="7" t="s">
+        <v>1259</v>
+      </c>
+      <c r="W187" s="7" t="s">
+        <v>1248</v>
+      </c>
+      <c r="X187" s="7" t="s">
+        <v>1260</v>
+      </c>
+      <c r="Y187" s="7"/>
+      <c r="Z187" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA187" s="7"/>
+      <c r="AB187" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC187" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD187" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE187" s="7"/>
+      <c r="AF187" s="7"/>
+      <c r="AG187" s="7"/>
+      <c r="AH187" s="7"/>
+      <c r="AI187" s="7"/>
+      <c r="AJ187" s="7"/>
+      <c r="AK187" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="188" spans="1:37">
+      <c r="A188" s="3">
+        <v>186</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C188" s="3">
+        <v>2026013077</v>
+      </c>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3">
+        <v>5245</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H188" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I188" s="3"/>
+      <c r="J188" s="3"/>
+      <c r="K188" s="3"/>
+      <c r="L188" s="3"/>
+      <c r="M188" s="4"/>
+      <c r="N188" s="3"/>
+      <c r="O188" s="4"/>
+      <c r="P188" s="10"/>
+      <c r="Q188" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="R188" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S188" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T188" s="3">
+        <v>1</v>
+      </c>
+      <c r="U188" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V188" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="W188" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="X188" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="Y188" s="3"/>
+      <c r="Z188" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA188" s="3"/>
+      <c r="AB188" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC188" s="10" t="s">
+        <v>1263</v>
+      </c>
+      <c r="AD188" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE188" s="3"/>
+      <c r="AF188" s="3"/>
+      <c r="AG188" s="3"/>
+      <c r="AH188" s="3"/>
+      <c r="AI188" s="3"/>
+      <c r="AJ188" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK188" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="189" spans="1:37">
+      <c r="A189" s="7">
+        <v>187</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C189" s="7">
+        <v>2026013083</v>
+      </c>
+      <c r="D189" s="7"/>
+      <c r="E189" s="7"/>
+      <c r="F189" s="7">
+        <v>4902</v>
+      </c>
+      <c r="G189" s="7" t="s">
+        <v>1264</v>
+      </c>
+      <c r="H189" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I189" s="7"/>
+      <c r="J189" s="7"/>
+      <c r="K189" s="7"/>
+      <c r="L189" s="7"/>
+      <c r="M189" s="8"/>
+      <c r="N189" s="7"/>
+      <c r="O189" s="8"/>
+      <c r="P189" s="9"/>
+      <c r="Q189" s="7" t="s">
+        <v>1265</v>
+      </c>
+      <c r="R189" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S189" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T189" s="7">
+        <v>1</v>
+      </c>
+      <c r="U189" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V189" s="7" t="s">
+        <v>1266</v>
+      </c>
+      <c r="W189" s="7" t="s">
+        <v>1267</v>
+      </c>
+      <c r="X189" s="7" t="s">
+        <v>1268</v>
+      </c>
+      <c r="Y189" s="7"/>
+      <c r="Z189" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA189" s="7"/>
+      <c r="AB189" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC189" s="9" t="s">
+        <v>1269</v>
+      </c>
+      <c r="AD189" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE189" s="7"/>
+      <c r="AF189" s="7"/>
+      <c r="AG189" s="7"/>
+      <c r="AH189" s="7"/>
+      <c r="AI189" s="7"/>
+      <c r="AJ189" s="7"/>
+      <c r="AK189" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="190" spans="1:37">
+      <c r="A190" s="3">
+        <v>188</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C190" s="3">
+        <v>2026013180</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3">
+        <v>2222</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H190" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I190" s="3"/>
+      <c r="J190" s="3"/>
+      <c r="K190" s="3"/>
+      <c r="L190" s="3"/>
+      <c r="M190" s="4"/>
+      <c r="N190" s="3"/>
+      <c r="O190" s="4"/>
+      <c r="P190" s="10"/>
+      <c r="Q190" s="3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="R190" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S190" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T190" s="3">
+        <v>1</v>
+      </c>
+      <c r="U190" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V190" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="W190" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="X190" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="Y190" s="3"/>
+      <c r="Z190" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA190" s="3"/>
+      <c r="AB190" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC190" s="10" t="s">
+        <v>1272</v>
+      </c>
+      <c r="AD190" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE190" s="3"/>
+      <c r="AF190" s="3"/>
+      <c r="AG190" s="3"/>
+      <c r="AH190" s="3"/>
+      <c r="AI190" s="3"/>
+      <c r="AJ190" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK190" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="191" spans="1:37">
+      <c r="A191" s="7">
+        <v>189</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C191" s="7">
+        <v>2026013254</v>
+      </c>
+      <c r="D191" s="7"/>
+      <c r="E191" s="7"/>
+      <c r="F191" s="7">
+        <v>4228</v>
+      </c>
+      <c r="G191" s="7" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H191" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I191" s="7"/>
+      <c r="J191" s="7"/>
+      <c r="K191" s="7"/>
+      <c r="L191" s="7"/>
+      <c r="M191" s="8"/>
+      <c r="N191" s="7"/>
+      <c r="O191" s="8"/>
+      <c r="P191" s="8"/>
+      <c r="Q191" s="7" t="s">
+        <v>1274</v>
+      </c>
+      <c r="R191" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S191" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T191" s="7">
+        <v>1</v>
+      </c>
+      <c r="U191" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V191" s="7" t="s">
+        <v>1275</v>
+      </c>
+      <c r="W191" s="7" t="s">
+        <v>1276</v>
+      </c>
+      <c r="X191" s="7" t="s">
+        <v>1277</v>
+      </c>
+      <c r="Y191" s="7"/>
+      <c r="Z191" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA191" s="7"/>
+      <c r="AB191" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC191" s="8" t="s">
+        <v>922</v>
+      </c>
+      <c r="AD191" s="7"/>
+      <c r="AE191" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF191" s="7"/>
+      <c r="AG191" s="7"/>
+      <c r="AH191" s="7"/>
+      <c r="AI191" s="7"/>
+      <c r="AJ191" s="7"/>
+      <c r="AK191" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01231724
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$191</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$197</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1318">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-23  )</t>
   </si>
@@ -3829,6 +3829,44 @@
     <t>PMQ1+7210002699+L90</t>
   </si>
   <si>
+    <t>E2062115012201</t>
+  </si>
+  <si>
+    <t>中和員山店</t>
+  </si>
+  <si>
+    <t>2026-01-22 13:08:27</t>
+  </si>
+  <si>
+    <t>D302</t>
+  </si>
+  <si>
+    <t>發票印字不清</t>
+  </si>
+  <si>
+    <t>門市反應tm3熱感發票機(BSC-10)列印出的兌換券於tm1.2.3都無法刷讀，tm1.2列印出的兌換券於tm1.2.3刷讀則正常，已有將發票機關機紙捲重裝仍異常...請台芝到店協助(機3列印條碼不清楚.無法直接刷條碼兌換商品.只能手動入條碼)
+01/22 13:35 區經理告知會請門市進線客服...欣
+01/22 13:13 13:30 13:35 門市電話未接...欣</t>
+  </si>
+  <si>
+    <t>THILF02062</t>
+  </si>
+  <si>
+    <t>2026-01-22 14:09:19</t>
+  </si>
+  <si>
+    <t>2026-01-23 15:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 18:09:00</t>
+  </si>
+  <si>
+    <t>換下8155003473換上8155005376</t>
+  </si>
+  <si>
     <t>2026-01-22 14:14:25</t>
   </si>
   <si>
@@ -3947,6 +3985,91 @@
   </si>
   <si>
     <t>2026-01-23 11:30:00</t>
+  </si>
+  <si>
+    <t>14125115012302</t>
+  </si>
+  <si>
+    <t>蘆洲長樂店</t>
+  </si>
+  <si>
+    <t>2026-01-23 15:10:56</t>
+  </si>
+  <si>
+    <t>門市反應無法操作TM1(TCX800)發票韌體更新，查看門市為1/21就要更新韌體，VNC查看仍為3.1，點選其他&gt;發票機韌體更新&gt;顯示找不到更新檔，總公司健誌副理協助查看 :查詢門市收銀機1似乎無法連線D磁碟機，請派工到店檢查狀況。
+2026/1/23 (週五) 下午 03:13總公司明翰MAILL:請協助一般派工，請到店更換TM第二顆硬碟，並協助併更新到251118A版本，TM2如果是BSC10II需同步更新到251118A版本</t>
+  </si>
+  <si>
+    <t>THILF04125</t>
+  </si>
+  <si>
+    <t>2026-01-23 15:16:18</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 19:16:00</t>
+  </si>
+  <si>
+    <t>重裝硬碟 更新韌體</t>
+  </si>
+  <si>
+    <t>14701115012301</t>
+  </si>
+  <si>
+    <t>新莊昌平店</t>
+  </si>
+  <si>
+    <t>2026-01-23 15:26:37</t>
+  </si>
+  <si>
+    <t>門市反應L90無法正常裁紙，門市已有重裝紙捲重開機仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04701</t>
+  </si>
+  <si>
+    <t>2026-01-23 15:27:34</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 19:27:00</t>
+  </si>
+  <si>
+    <t>更新韌體</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:30:32</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:05:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:25:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002960</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:32:24</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:48:04</t>
+  </si>
+  <si>
+    <t>2026-01-23 16:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003081</t>
   </si>
 </sst>
 </file>
@@ -4360,10 +4483,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK191"/>
+  <dimension ref="A1:AK197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A191" sqref="A191"/>
+      <selection activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20018,32 +20141,52 @@
         <v>181</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C183" s="7">
-        <v>2026013030</v>
-      </c>
-      <c r="D183" s="7"/>
-      <c r="E183" s="7"/>
+        <v>2026013025</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E183" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F183" s="7">
-        <v>4241</v>
+        <v>2062</v>
       </c>
       <c r="G183" s="7" t="s">
-        <v>1186</v>
+        <v>1239</v>
       </c>
       <c r="H183" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I183" s="7"/>
-      <c r="J183" s="7"/>
-      <c r="K183" s="7"/>
-      <c r="L183" s="7"/>
-      <c r="M183" s="8"/>
-      <c r="N183" s="7"/>
-      <c r="O183" s="8"/>
-      <c r="P183" s="9"/>
+        <v>127</v>
+      </c>
+      <c r="I183" s="7" t="s">
+        <v>1240</v>
+      </c>
+      <c r="J183" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K183" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L183" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M183" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N183" s="7" t="s">
+        <v>1241</v>
+      </c>
+      <c r="O183" s="8" t="s">
+        <v>1242</v>
+      </c>
+      <c r="P183" s="9" t="s">
+        <v>1243</v>
+      </c>
       <c r="Q183" s="7" t="s">
-        <v>1189</v>
+        <v>1244</v>
       </c>
       <c r="R183" s="7" t="s">
         <v>51</v>
@@ -20058,15 +20201,17 @@
         <v>53</v>
       </c>
       <c r="V183" s="7" t="s">
-        <v>1238</v>
+        <v>1245</v>
       </c>
       <c r="W183" s="7" t="s">
-        <v>1239</v>
+        <v>1246</v>
       </c>
       <c r="X183" s="7" t="s">
-        <v>1191</v>
-      </c>
-      <c r="Y183" s="7"/>
+        <v>1247</v>
+      </c>
+      <c r="Y183" s="7" t="s">
+        <v>1248</v>
+      </c>
       <c r="Z183" s="7">
         <v>0.3</v>
       </c>
@@ -20075,19 +20220,15 @@
         <v>58</v>
       </c>
       <c r="AC183" s="9" t="s">
-        <v>1240</v>
-      </c>
-      <c r="AD183" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>1249</v>
+      </c>
+      <c r="AD183" s="7"/>
       <c r="AE183" s="7"/>
       <c r="AF183" s="7"/>
       <c r="AG183" s="7"/>
       <c r="AH183" s="7"/>
       <c r="AI183" s="7"/>
-      <c r="AJ183" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ183" s="7"/>
       <c r="AK183" s="7" t="s">
         <v>60</v>
       </c>
@@ -20100,18 +20241,18 @@
         <v>118</v>
       </c>
       <c r="C184" s="3">
-        <v>2026013047</v>
+        <v>2026013030</v>
       </c>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
       <c r="F184" s="3">
-        <v>4503</v>
+        <v>4241</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>1241</v>
+        <v>1186</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>296</v>
+        <v>92</v>
       </c>
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
@@ -20122,13 +20263,13 @@
       <c r="O184" s="4"/>
       <c r="P184" s="10"/>
       <c r="Q184" s="3" t="s">
-        <v>1242</v>
+        <v>1189</v>
       </c>
       <c r="R184" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S184" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T184" s="3">
         <v>1</v>
@@ -20137,13 +20278,13 @@
         <v>53</v>
       </c>
       <c r="V184" s="3" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
       <c r="W184" s="3" t="s">
-        <v>1244</v>
+        <v>1251</v>
       </c>
       <c r="X184" s="3" t="s">
-        <v>1245</v>
+        <v>1191</v>
       </c>
       <c r="Y184" s="3"/>
       <c r="Z184" s="3">
@@ -20154,7 +20295,7 @@
         <v>58</v>
       </c>
       <c r="AC184" s="10" t="s">
-        <v>1246</v>
+        <v>1252</v>
       </c>
       <c r="AD184" s="3" t="s">
         <v>60</v>
@@ -20164,7 +20305,9 @@
       <c r="AG184" s="3"/>
       <c r="AH184" s="3"/>
       <c r="AI184" s="3"/>
-      <c r="AJ184" s="3"/>
+      <c r="AJ184" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK184" s="3" t="s">
         <v>60</v>
       </c>
@@ -20177,18 +20320,18 @@
         <v>118</v>
       </c>
       <c r="C185" s="7">
-        <v>2026013057</v>
+        <v>2026013047</v>
       </c>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
       <c r="F185" s="7">
-        <v>4352</v>
+        <v>4503</v>
       </c>
       <c r="G185" s="7" t="s">
-        <v>1176</v>
+        <v>1253</v>
       </c>
       <c r="H185" s="7" t="s">
-        <v>92</v>
+        <v>296</v>
       </c>
       <c r="I185" s="7"/>
       <c r="J185" s="7"/>
@@ -20199,13 +20342,13 @@
       <c r="O185" s="8"/>
       <c r="P185" s="9"/>
       <c r="Q185" s="7" t="s">
-        <v>1179</v>
+        <v>1254</v>
       </c>
       <c r="R185" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S185" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T185" s="7">
         <v>1</v>
@@ -20214,24 +20357,24 @@
         <v>53</v>
       </c>
       <c r="V185" s="7" t="s">
-        <v>1247</v>
+        <v>1255</v>
       </c>
       <c r="W185" s="7" t="s">
-        <v>1248</v>
+        <v>1256</v>
       </c>
       <c r="X185" s="7" t="s">
-        <v>1249</v>
+        <v>1257</v>
       </c>
       <c r="Y185" s="7"/>
       <c r="Z185" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA185" s="7"/>
       <c r="AB185" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC185" s="9" t="s">
-        <v>1250</v>
+        <v>1258</v>
       </c>
       <c r="AD185" s="7" t="s">
         <v>60</v>
@@ -20241,9 +20384,7 @@
       <c r="AG185" s="7"/>
       <c r="AH185" s="7"/>
       <c r="AI185" s="7"/>
-      <c r="AJ185" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ185" s="7"/>
       <c r="AK185" s="7" t="s">
         <v>60</v>
       </c>
@@ -20256,18 +20397,18 @@
         <v>118</v>
       </c>
       <c r="C186" s="3">
-        <v>2026013075</v>
+        <v>2026013057</v>
       </c>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
       <c r="F186" s="3">
-        <v>5016</v>
+        <v>4352</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>1251</v>
+        <v>1176</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>296</v>
+        <v>92</v>
       </c>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
@@ -20278,13 +20419,13 @@
       <c r="O186" s="4"/>
       <c r="P186" s="10"/>
       <c r="Q186" s="3" t="s">
-        <v>1252</v>
+        <v>1179</v>
       </c>
       <c r="R186" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S186" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T186" s="3">
         <v>1</v>
@@ -20293,13 +20434,13 @@
         <v>53</v>
       </c>
       <c r="V186" s="3" t="s">
-        <v>1253</v>
+        <v>1259</v>
       </c>
       <c r="W186" s="3" t="s">
-        <v>1254</v>
+        <v>1260</v>
       </c>
       <c r="X186" s="3" t="s">
-        <v>1255</v>
+        <v>1261</v>
       </c>
       <c r="Y186" s="3"/>
       <c r="Z186" s="3">
@@ -20310,7 +20451,7 @@
         <v>58</v>
       </c>
       <c r="AC186" s="10" t="s">
-        <v>1256</v>
+        <v>1262</v>
       </c>
       <c r="AD186" s="3" t="s">
         <v>60</v>
@@ -20320,7 +20461,9 @@
       <c r="AG186" s="3"/>
       <c r="AH186" s="3"/>
       <c r="AI186" s="3"/>
-      <c r="AJ186" s="3"/>
+      <c r="AJ186" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK186" s="3" t="s">
         <v>60</v>
       </c>
@@ -20333,15 +20476,15 @@
         <v>118</v>
       </c>
       <c r="C187" s="7">
-        <v>2026013076</v>
+        <v>2026013075</v>
       </c>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
       <c r="F187" s="7">
-        <v>2428</v>
+        <v>5016</v>
       </c>
       <c r="G187" s="7" t="s">
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="H187" s="7" t="s">
         <v>296</v>
@@ -20355,7 +20498,7 @@
       <c r="O187" s="8"/>
       <c r="P187" s="9"/>
       <c r="Q187" s="7" t="s">
-        <v>1258</v>
+        <v>1264</v>
       </c>
       <c r="R187" s="7" t="s">
         <v>51</v>
@@ -20370,24 +20513,24 @@
         <v>53</v>
       </c>
       <c r="V187" s="7" t="s">
-        <v>1259</v>
+        <v>1265</v>
       </c>
       <c r="W187" s="7" t="s">
-        <v>1248</v>
+        <v>1266</v>
       </c>
       <c r="X187" s="7" t="s">
-        <v>1260</v>
+        <v>1267</v>
       </c>
       <c r="Y187" s="7"/>
       <c r="Z187" s="7">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="AA187" s="7"/>
       <c r="AB187" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC187" s="9" t="s">
-        <v>121</v>
+        <v>1268</v>
       </c>
       <c r="AD187" s="7" t="s">
         <v>60</v>
@@ -20410,18 +20553,18 @@
         <v>118</v>
       </c>
       <c r="C188" s="3">
-        <v>2026013077</v>
+        <v>2026013076</v>
       </c>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
       <c r="F188" s="3">
-        <v>5245</v>
+        <v>2428</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>1203</v>
+        <v>1269</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>92</v>
+        <v>296</v>
       </c>
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
@@ -20432,13 +20575,13 @@
       <c r="O188" s="4"/>
       <c r="P188" s="10"/>
       <c r="Q188" s="3" t="s">
-        <v>1206</v>
+        <v>1270</v>
       </c>
       <c r="R188" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S188" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T188" s="3">
         <v>1</v>
@@ -20447,13 +20590,13 @@
         <v>53</v>
       </c>
       <c r="V188" s="3" t="s">
-        <v>1261</v>
+        <v>1271</v>
       </c>
       <c r="W188" s="3" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="X188" s="3" t="s">
-        <v>1208</v>
+        <v>1272</v>
       </c>
       <c r="Y188" s="3"/>
       <c r="Z188" s="3">
@@ -20464,7 +20607,7 @@
         <v>58</v>
       </c>
       <c r="AC188" s="10" t="s">
-        <v>1263</v>
+        <v>121</v>
       </c>
       <c r="AD188" s="3" t="s">
         <v>60</v>
@@ -20474,9 +20617,7 @@
       <c r="AG188" s="3"/>
       <c r="AH188" s="3"/>
       <c r="AI188" s="3"/>
-      <c r="AJ188" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ188" s="3"/>
       <c r="AK188" s="3" t="s">
         <v>60</v>
       </c>
@@ -20489,18 +20630,18 @@
         <v>118</v>
       </c>
       <c r="C189" s="7">
-        <v>2026013083</v>
+        <v>2026013077</v>
       </c>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
       <c r="F189" s="7">
-        <v>4902</v>
+        <v>5245</v>
       </c>
       <c r="G189" s="7" t="s">
-        <v>1264</v>
+        <v>1203</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>296</v>
+        <v>92</v>
       </c>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
@@ -20511,13 +20652,13 @@
       <c r="O189" s="8"/>
       <c r="P189" s="9"/>
       <c r="Q189" s="7" t="s">
-        <v>1265</v>
+        <v>1206</v>
       </c>
       <c r="R189" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S189" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T189" s="7">
         <v>1</v>
@@ -20526,13 +20667,13 @@
         <v>53</v>
       </c>
       <c r="V189" s="7" t="s">
-        <v>1266</v>
+        <v>1273</v>
       </c>
       <c r="W189" s="7" t="s">
-        <v>1267</v>
+        <v>1274</v>
       </c>
       <c r="X189" s="7" t="s">
-        <v>1268</v>
+        <v>1208</v>
       </c>
       <c r="Y189" s="7"/>
       <c r="Z189" s="7">
@@ -20543,7 +20684,7 @@
         <v>58</v>
       </c>
       <c r="AC189" s="9" t="s">
-        <v>1269</v>
+        <v>1275</v>
       </c>
       <c r="AD189" s="7" t="s">
         <v>60</v>
@@ -20553,7 +20694,9 @@
       <c r="AG189" s="7"/>
       <c r="AH189" s="7"/>
       <c r="AI189" s="7"/>
-      <c r="AJ189" s="7"/>
+      <c r="AJ189" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AK189" s="7" t="s">
         <v>60</v>
       </c>
@@ -20566,18 +20709,18 @@
         <v>118</v>
       </c>
       <c r="C190" s="3">
-        <v>2026013180</v>
+        <v>2026013083</v>
       </c>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
       <c r="F190" s="3">
-        <v>2222</v>
+        <v>4902</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>1139</v>
+        <v>1276</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>92</v>
+        <v>296</v>
       </c>
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
@@ -20588,13 +20731,13 @@
       <c r="O190" s="4"/>
       <c r="P190" s="10"/>
       <c r="Q190" s="3" t="s">
-        <v>1140</v>
+        <v>1277</v>
       </c>
       <c r="R190" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S190" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T190" s="3">
         <v>1</v>
@@ -20603,13 +20746,13 @@
         <v>53</v>
       </c>
       <c r="V190" s="3" t="s">
-        <v>1270</v>
+        <v>1278</v>
       </c>
       <c r="W190" s="3" t="s">
-        <v>1267</v>
+        <v>1279</v>
       </c>
       <c r="X190" s="3" t="s">
-        <v>1271</v>
+        <v>1280</v>
       </c>
       <c r="Y190" s="3"/>
       <c r="Z190" s="3">
@@ -20620,7 +20763,7 @@
         <v>58</v>
       </c>
       <c r="AC190" s="10" t="s">
-        <v>1272</v>
+        <v>1281</v>
       </c>
       <c r="AD190" s="3" t="s">
         <v>60</v>
@@ -20630,9 +20773,7 @@
       <c r="AG190" s="3"/>
       <c r="AH190" s="3"/>
       <c r="AI190" s="3"/>
-      <c r="AJ190" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ190" s="3"/>
       <c r="AK190" s="3" t="s">
         <v>60</v>
       </c>
@@ -20645,18 +20786,18 @@
         <v>118</v>
       </c>
       <c r="C191" s="7">
-        <v>2026013254</v>
+        <v>2026013180</v>
       </c>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
       <c r="F191" s="7">
-        <v>4228</v>
+        <v>2222</v>
       </c>
       <c r="G191" s="7" t="s">
-        <v>1273</v>
+        <v>1139</v>
       </c>
       <c r="H191" s="7" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
@@ -20665,15 +20806,15 @@
       <c r="M191" s="8"/>
       <c r="N191" s="7"/>
       <c r="O191" s="8"/>
-      <c r="P191" s="8"/>
+      <c r="P191" s="9"/>
       <c r="Q191" s="7" t="s">
-        <v>1274</v>
+        <v>1140</v>
       </c>
       <c r="R191" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S191" s="7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T191" s="7">
         <v>1</v>
@@ -20682,35 +20823,543 @@
         <v>53</v>
       </c>
       <c r="V191" s="7" t="s">
-        <v>1275</v>
+        <v>1282</v>
       </c>
       <c r="W191" s="7" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="X191" s="7" t="s">
-        <v>1277</v>
+        <v>1283</v>
       </c>
       <c r="Y191" s="7"/>
       <c r="Z191" s="7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA191" s="7"/>
       <c r="AB191" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC191" s="8" t="s">
-        <v>922</v>
-      </c>
-      <c r="AD191" s="7"/>
-      <c r="AE191" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC191" s="9" t="s">
+        <v>1284</v>
+      </c>
+      <c r="AD191" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE191" s="7"/>
       <c r="AF191" s="7"/>
       <c r="AG191" s="7"/>
       <c r="AH191" s="7"/>
       <c r="AI191" s="7"/>
-      <c r="AJ191" s="7"/>
+      <c r="AJ191" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AK191" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="192" spans="1:37">
+      <c r="A192" s="3">
+        <v>190</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C192" s="3">
+        <v>2026013254</v>
+      </c>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3">
+        <v>4228</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="H192" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I192" s="3"/>
+      <c r="J192" s="3"/>
+      <c r="K192" s="3"/>
+      <c r="L192" s="3"/>
+      <c r="M192" s="4"/>
+      <c r="N192" s="3"/>
+      <c r="O192" s="4"/>
+      <c r="P192" s="10"/>
+      <c r="Q192" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="R192" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S192" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T192" s="3">
+        <v>1</v>
+      </c>
+      <c r="U192" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V192" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="W192" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="X192" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="Y192" s="3"/>
+      <c r="Z192" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA192" s="3"/>
+      <c r="AB192" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC192" s="10" t="s">
+        <v>922</v>
+      </c>
+      <c r="AD192" s="3"/>
+      <c r="AE192" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF192" s="3"/>
+      <c r="AG192" s="3"/>
+      <c r="AH192" s="3"/>
+      <c r="AI192" s="3"/>
+      <c r="AJ192" s="3"/>
+      <c r="AK192" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="193" spans="1:37">
+      <c r="A193" s="7">
+        <v>191</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C193" s="7">
+        <v>2026013340</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F193" s="7">
+        <v>4125</v>
+      </c>
+      <c r="G193" s="7" t="s">
+        <v>1291</v>
+      </c>
+      <c r="H193" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I193" s="7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="J193" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K193" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L193" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M193" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N193" s="7">
+        <v>2308</v>
+      </c>
+      <c r="O193" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="P193" s="9" t="s">
+        <v>1293</v>
+      </c>
+      <c r="Q193" s="7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="R193" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S193" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T193" s="7">
+        <v>1</v>
+      </c>
+      <c r="U193" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V193" s="7" t="s">
+        <v>1295</v>
+      </c>
+      <c r="W193" s="7" t="s">
+        <v>1296</v>
+      </c>
+      <c r="X193" s="7" t="s">
+        <v>1297</v>
+      </c>
+      <c r="Y193" s="7" t="s">
+        <v>1298</v>
+      </c>
+      <c r="Z193" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA193" s="7"/>
+      <c r="AB193" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC193" s="9" t="s">
+        <v>1299</v>
+      </c>
+      <c r="AD193" s="7"/>
+      <c r="AE193" s="7"/>
+      <c r="AF193" s="7"/>
+      <c r="AG193" s="7"/>
+      <c r="AH193" s="7"/>
+      <c r="AI193" s="7"/>
+      <c r="AJ193" s="7"/>
+      <c r="AK193" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="194" spans="1:37">
+      <c r="A194" s="3">
+        <v>192</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C194" s="3">
+        <v>2026013345</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F194" s="3">
+        <v>4701</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="H194" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I194" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J194" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K194" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L194" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="M194" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="N194" s="3">
+        <v>6001</v>
+      </c>
+      <c r="O194" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P194" s="10" t="s">
+        <v>1303</v>
+      </c>
+      <c r="Q194" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="R194" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S194" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T194" s="3">
+        <v>1</v>
+      </c>
+      <c r="U194" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V194" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="W194" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="X194" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="Y194" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="Z194" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA194" s="3"/>
+      <c r="AB194" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC194" s="10" t="s">
+        <v>1309</v>
+      </c>
+      <c r="AD194" s="3"/>
+      <c r="AE194" s="3"/>
+      <c r="AF194" s="3"/>
+      <c r="AG194" s="3"/>
+      <c r="AH194" s="3"/>
+      <c r="AI194" s="3"/>
+      <c r="AJ194" s="3"/>
+      <c r="AK194" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="195" spans="1:37">
+      <c r="A195" s="7">
+        <v>193</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C195" s="7">
+        <v>2026013384</v>
+      </c>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7"/>
+      <c r="F195" s="7">
+        <v>2062</v>
+      </c>
+      <c r="G195" s="7" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H195" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I195" s="7"/>
+      <c r="J195" s="7"/>
+      <c r="K195" s="7"/>
+      <c r="L195" s="7"/>
+      <c r="M195" s="8"/>
+      <c r="N195" s="7"/>
+      <c r="O195" s="8"/>
+      <c r="P195" s="9"/>
+      <c r="Q195" s="7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="R195" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S195" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T195" s="7">
+        <v>1</v>
+      </c>
+      <c r="U195" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V195" s="7" t="s">
+        <v>1310</v>
+      </c>
+      <c r="W195" s="7" t="s">
+        <v>1311</v>
+      </c>
+      <c r="X195" s="7" t="s">
+        <v>1312</v>
+      </c>
+      <c r="Y195" s="7"/>
+      <c r="Z195" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA195" s="7"/>
+      <c r="AB195" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC195" s="9" t="s">
+        <v>1313</v>
+      </c>
+      <c r="AD195" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE195" s="7"/>
+      <c r="AF195" s="7"/>
+      <c r="AG195" s="7"/>
+      <c r="AH195" s="7"/>
+      <c r="AI195" s="7"/>
+      <c r="AJ195" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK195" s="7"/>
+    </row>
+    <row r="196" spans="1:37">
+      <c r="A196" s="3">
+        <v>194</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C196" s="3">
+        <v>2026013385</v>
+      </c>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3">
+        <v>2062</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H196" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I196" s="3"/>
+      <c r="J196" s="3"/>
+      <c r="K196" s="3"/>
+      <c r="L196" s="3"/>
+      <c r="M196" s="4"/>
+      <c r="N196" s="3"/>
+      <c r="O196" s="4"/>
+      <c r="P196" s="10"/>
+      <c r="Q196" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="R196" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S196" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T196" s="3">
+        <v>1</v>
+      </c>
+      <c r="U196" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V196" s="3" t="s">
+        <v>1314</v>
+      </c>
+      <c r="W196" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="X196" s="3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="Y196" s="3"/>
+      <c r="Z196" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA196" s="3"/>
+      <c r="AB196" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC196" s="10" t="s">
+        <v>1313</v>
+      </c>
+      <c r="AD196" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE196" s="3"/>
+      <c r="AF196" s="3"/>
+      <c r="AG196" s="3"/>
+      <c r="AH196" s="3"/>
+      <c r="AI196" s="3"/>
+      <c r="AJ196" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK196" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="197" spans="1:37">
+      <c r="A197" s="7">
+        <v>195</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C197" s="7">
+        <v>2026013390</v>
+      </c>
+      <c r="D197" s="7"/>
+      <c r="E197" s="7"/>
+      <c r="F197" s="7">
+        <v>4125</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>1291</v>
+      </c>
+      <c r="H197" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I197" s="7"/>
+      <c r="J197" s="7"/>
+      <c r="K197" s="7"/>
+      <c r="L197" s="7"/>
+      <c r="M197" s="8"/>
+      <c r="N197" s="7"/>
+      <c r="O197" s="8"/>
+      <c r="P197" s="8"/>
+      <c r="Q197" s="7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="R197" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S197" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T197" s="7">
+        <v>1</v>
+      </c>
+      <c r="U197" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V197" s="7" t="s">
+        <v>1315</v>
+      </c>
+      <c r="W197" s="7" t="s">
+        <v>1297</v>
+      </c>
+      <c r="X197" s="7" t="s">
+        <v>1316</v>
+      </c>
+      <c r="Y197" s="7"/>
+      <c r="Z197" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA197" s="7"/>
+      <c r="AB197" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC197" s="8" t="s">
+        <v>1317</v>
+      </c>
+      <c r="AD197" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE197" s="7"/>
+      <c r="AF197" s="7"/>
+      <c r="AG197" s="7"/>
+      <c r="AH197" s="7"/>
+      <c r="AI197" s="7"/>
+      <c r="AJ197" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK197" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01231845
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$197</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$200</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1334">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-23  )</t>
   </si>
@@ -3987,6 +3987,42 @@
     <t>2026-01-23 11:30:00</t>
   </si>
   <si>
+    <t>EC672115012301</t>
+  </si>
+  <si>
+    <t>C672</t>
+  </si>
+  <si>
+    <t>中和橋安店</t>
+  </si>
+  <si>
+    <t>2026-01-23 12:59:11</t>
+  </si>
+  <si>
+    <t>印字不清</t>
+  </si>
+  <si>
+    <t>門市反應LIFE ET熱感機(T70II)印出的小白單條碼模糊，門市已嘗試重裝紙捲、重啟熱感機電源，清潔出票口仍異常...需請台芝到店協助(熱感紙列印出來模糊.無法刷繳)</t>
+  </si>
+  <si>
+    <t>THILF0C672</t>
+  </si>
+  <si>
+    <t>2026-01-23 13:06:55</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:33:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 17:06:00</t>
+  </si>
+  <si>
+    <t>清潔感熱頭測試正常</t>
+  </si>
+  <si>
     <t>14125115012302</t>
   </si>
   <si>
@@ -4039,9 +4075,6 @@
     <t>2026-01-23 17:00:00</t>
   </si>
   <si>
-    <t>2026-01-23 17:20:00</t>
-  </si>
-  <si>
     <t>2026-01-26 19:27:00</t>
   </si>
   <si>
@@ -4070,6 +4103,21 @@
   </si>
   <si>
     <t>PMQ1+7210003081</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:32:11</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003066</t>
+  </si>
+  <si>
+    <t>2026-01-23 17:36:47</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002982</t>
   </si>
 </sst>
 </file>
@@ -4483,10 +4531,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK197"/>
+  <dimension ref="A1:AK200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A197" sqref="A197"/>
+      <selection activeCell="AC197" sqref="AC197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20942,7 +20990,7 @@
         <v>38</v>
       </c>
       <c r="C193" s="7">
-        <v>2026013340</v>
+        <v>2026013278</v>
       </c>
       <c r="D193" s="7" t="s">
         <v>1290</v>
@@ -20950,17 +20998,17 @@
       <c r="E193" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F193" s="7">
-        <v>4125</v>
+      <c r="F193" s="7" t="s">
+        <v>1291</v>
       </c>
       <c r="G193" s="7" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>250</v>
+        <v>127</v>
       </c>
       <c r="I193" s="7" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="J193" s="7" t="s">
         <v>129</v>
@@ -20969,28 +21017,28 @@
         <v>79</v>
       </c>
       <c r="L193" s="7" t="s">
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="M193" s="8" t="s">
-        <v>47</v>
+        <v>195</v>
       </c>
       <c r="N193" s="7">
-        <v>2308</v>
+        <v>5902</v>
       </c>
       <c r="O193" s="8" t="s">
-        <v>287</v>
+        <v>1294</v>
       </c>
       <c r="P193" s="9" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="Q193" s="7" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="R193" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S193" s="7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T193" s="7">
         <v>1</v>
@@ -20999,26 +21047,26 @@
         <v>53</v>
       </c>
       <c r="V193" s="7" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="W193" s="7" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="X193" s="7" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="Y193" s="7" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="Z193" s="7">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AA193" s="7"/>
       <c r="AB193" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC193" s="9" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="AD193" s="7"/>
       <c r="AE193" s="7"/>
@@ -21039,25 +21087,25 @@
         <v>38</v>
       </c>
       <c r="C194" s="3">
-        <v>2026013345</v>
+        <v>2026013340</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F194" s="3">
-        <v>4701</v>
+        <v>4125</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>77</v>
+        <v>250</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="J194" s="3" t="s">
         <v>129</v>
@@ -21066,22 +21114,22 @@
         <v>79</v>
       </c>
       <c r="L194" s="3" t="s">
-        <v>253</v>
+        <v>46</v>
       </c>
       <c r="M194" s="4" t="s">
-        <v>254</v>
+        <v>47</v>
       </c>
       <c r="N194" s="3">
-        <v>6001</v>
+        <v>2308</v>
       </c>
       <c r="O194" s="4" t="s">
-        <v>1010</v>
+        <v>287</v>
       </c>
       <c r="P194" s="10" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="Q194" s="3" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="R194" s="3" t="s">
         <v>51</v>
@@ -21096,26 +21144,26 @@
         <v>53</v>
       </c>
       <c r="V194" s="3" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="W194" s="3" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="X194" s="3" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="Y194" s="3" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="Z194" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA194" s="3"/>
       <c r="AB194" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC194" s="10" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="AD194" s="3"/>
       <c r="AE194" s="3"/>
@@ -21133,38 +21181,58 @@
         <v>193</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C195" s="7">
-        <v>2026013384</v>
-      </c>
-      <c r="D195" s="7"/>
-      <c r="E195" s="7"/>
+        <v>2026013345</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F195" s="7">
-        <v>2062</v>
+        <v>4701</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>1239</v>
+        <v>1313</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I195" s="7"/>
-      <c r="J195" s="7"/>
-      <c r="K195" s="7"/>
-      <c r="L195" s="7"/>
-      <c r="M195" s="8"/>
-      <c r="N195" s="7"/>
-      <c r="O195" s="8"/>
-      <c r="P195" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="I195" s="7" t="s">
+        <v>1314</v>
+      </c>
+      <c r="J195" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K195" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L195" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="M195" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="N195" s="7">
+        <v>6001</v>
+      </c>
+      <c r="O195" s="8" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P195" s="9" t="s">
+        <v>1315</v>
+      </c>
       <c r="Q195" s="7" t="s">
-        <v>1244</v>
+        <v>1316</v>
       </c>
       <c r="R195" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S195" s="7" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="T195" s="7">
         <v>1</v>
@@ -21173,15 +21241,17 @@
         <v>53</v>
       </c>
       <c r="V195" s="7" t="s">
-        <v>1310</v>
+        <v>1317</v>
       </c>
       <c r="W195" s="7" t="s">
-        <v>1311</v>
+        <v>1318</v>
       </c>
       <c r="X195" s="7" t="s">
-        <v>1312</v>
-      </c>
-      <c r="Y195" s="7"/>
+        <v>1298</v>
+      </c>
+      <c r="Y195" s="7" t="s">
+        <v>1319</v>
+      </c>
       <c r="Z195" s="7">
         <v>0.3</v>
       </c>
@@ -21190,20 +21260,18 @@
         <v>58</v>
       </c>
       <c r="AC195" s="9" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AD195" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>1320</v>
+      </c>
+      <c r="AD195" s="7"/>
       <c r="AE195" s="7"/>
       <c r="AF195" s="7"/>
       <c r="AG195" s="7"/>
       <c r="AH195" s="7"/>
       <c r="AI195" s="7"/>
-      <c r="AJ195" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK195" s="7"/>
+      <c r="AJ195" s="7"/>
+      <c r="AK195" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="196" spans="1:37">
       <c r="A196" s="3">
@@ -21213,7 +21281,7 @@
         <v>118</v>
       </c>
       <c r="C196" s="3">
-        <v>2026013385</v>
+        <v>2026013384</v>
       </c>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
@@ -21250,13 +21318,13 @@
         <v>53</v>
       </c>
       <c r="V196" s="3" t="s">
-        <v>1314</v>
+        <v>1321</v>
       </c>
       <c r="W196" s="3" t="s">
-        <v>1311</v>
+        <v>1322</v>
       </c>
       <c r="X196" s="3" t="s">
-        <v>1312</v>
+        <v>1323</v>
       </c>
       <c r="Y196" s="3"/>
       <c r="Z196" s="3">
@@ -21267,7 +21335,7 @@
         <v>58</v>
       </c>
       <c r="AC196" s="10" t="s">
-        <v>1313</v>
+        <v>1324</v>
       </c>
       <c r="AD196" s="3" t="s">
         <v>60</v>
@@ -21280,9 +21348,7 @@
       <c r="AJ196" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AK196" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AK196" s="3"/>
     </row>
     <row r="197" spans="1:37">
       <c r="A197" s="7">
@@ -21292,18 +21358,18 @@
         <v>118</v>
       </c>
       <c r="C197" s="7">
-        <v>2026013390</v>
+        <v>2026013385</v>
       </c>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
       <c r="F197" s="7">
-        <v>4125</v>
+        <v>2062</v>
       </c>
       <c r="G197" s="7" t="s">
-        <v>1291</v>
+        <v>1239</v>
       </c>
       <c r="H197" s="7" t="s">
-        <v>250</v>
+        <v>127</v>
       </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
@@ -21312,15 +21378,15 @@
       <c r="M197" s="8"/>
       <c r="N197" s="7"/>
       <c r="O197" s="8"/>
-      <c r="P197" s="8"/>
+      <c r="P197" s="9"/>
       <c r="Q197" s="7" t="s">
-        <v>1294</v>
+        <v>1244</v>
       </c>
       <c r="R197" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S197" s="7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T197" s="7">
         <v>1</v>
@@ -21329,13 +21395,13 @@
         <v>53</v>
       </c>
       <c r="V197" s="7" t="s">
-        <v>1315</v>
+        <v>1325</v>
       </c>
       <c r="W197" s="7" t="s">
-        <v>1297</v>
+        <v>1322</v>
       </c>
       <c r="X197" s="7" t="s">
-        <v>1316</v>
+        <v>1323</v>
       </c>
       <c r="Y197" s="7"/>
       <c r="Z197" s="7">
@@ -21345,8 +21411,8 @@
       <c r="AB197" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC197" s="8" t="s">
-        <v>1317</v>
+      <c r="AC197" s="9" t="s">
+        <v>1324</v>
       </c>
       <c r="AD197" s="7" t="s">
         <v>60</v>
@@ -21360,6 +21426,243 @@
         <v>60</v>
       </c>
       <c r="AK197" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="198" spans="1:37">
+      <c r="A198" s="3">
+        <v>196</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C198" s="3">
+        <v>2026013390</v>
+      </c>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3">
+        <v>4125</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>1303</v>
+      </c>
+      <c r="H198" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I198" s="3"/>
+      <c r="J198" s="3"/>
+      <c r="K198" s="3"/>
+      <c r="L198" s="3"/>
+      <c r="M198" s="4"/>
+      <c r="N198" s="3"/>
+      <c r="O198" s="4"/>
+      <c r="P198" s="10"/>
+      <c r="Q198" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="R198" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S198" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T198" s="3">
+        <v>1</v>
+      </c>
+      <c r="U198" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V198" s="3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="W198" s="3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="X198" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="Y198" s="3"/>
+      <c r="Z198" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA198" s="3"/>
+      <c r="AB198" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC198" s="10" t="s">
+        <v>1328</v>
+      </c>
+      <c r="AD198" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE198" s="3"/>
+      <c r="AF198" s="3"/>
+      <c r="AG198" s="3"/>
+      <c r="AH198" s="3"/>
+      <c r="AI198" s="3"/>
+      <c r="AJ198" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK198" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="199" spans="1:37">
+      <c r="A199" s="7">
+        <v>197</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C199" s="7">
+        <v>2026013392</v>
+      </c>
+      <c r="D199" s="7"/>
+      <c r="E199" s="7"/>
+      <c r="F199" s="7">
+        <v>4701</v>
+      </c>
+      <c r="G199" s="7" t="s">
+        <v>1313</v>
+      </c>
+      <c r="H199" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I199" s="7"/>
+      <c r="J199" s="7"/>
+      <c r="K199" s="7"/>
+      <c r="L199" s="7"/>
+      <c r="M199" s="8"/>
+      <c r="N199" s="7"/>
+      <c r="O199" s="8"/>
+      <c r="P199" s="9"/>
+      <c r="Q199" s="7" t="s">
+        <v>1316</v>
+      </c>
+      <c r="R199" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S199" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T199" s="7">
+        <v>1</v>
+      </c>
+      <c r="U199" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V199" s="7" t="s">
+        <v>1329</v>
+      </c>
+      <c r="W199" s="7" t="s">
+        <v>1298</v>
+      </c>
+      <c r="X199" s="7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="Y199" s="7"/>
+      <c r="Z199" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA199" s="7"/>
+      <c r="AB199" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC199" s="9" t="s">
+        <v>1331</v>
+      </c>
+      <c r="AD199" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE199" s="7"/>
+      <c r="AF199" s="7"/>
+      <c r="AG199" s="7"/>
+      <c r="AH199" s="7"/>
+      <c r="AI199" s="7"/>
+      <c r="AJ199" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK199" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="200" spans="1:37">
+      <c r="A200" s="3">
+        <v>198</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C200" s="3">
+        <v>2026013393</v>
+      </c>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="H200" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I200" s="3"/>
+      <c r="J200" s="3"/>
+      <c r="K200" s="3"/>
+      <c r="L200" s="3"/>
+      <c r="M200" s="4"/>
+      <c r="N200" s="3"/>
+      <c r="O200" s="4"/>
+      <c r="P200" s="4"/>
+      <c r="Q200" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="R200" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S200" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T200" s="3">
+        <v>1</v>
+      </c>
+      <c r="U200" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V200" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="W200" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="X200" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="Y200" s="3"/>
+      <c r="Z200" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA200" s="3"/>
+      <c r="AB200" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC200" s="4" t="s">
+        <v>1333</v>
+      </c>
+      <c r="AD200" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE200" s="3"/>
+      <c r="AF200" s="3"/>
+      <c r="AG200" s="3"/>
+      <c r="AH200" s="3"/>
+      <c r="AI200" s="3"/>
+      <c r="AJ200" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK200" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01261725
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$200</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$207</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1334">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-23  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1381">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-26  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -4118,6 +4118,149 @@
   </si>
   <si>
     <t>PMQ1+7210002982</t>
+  </si>
+  <si>
+    <t>13569115012401</t>
+  </si>
+  <si>
+    <t>中和中板店</t>
+  </si>
+  <si>
+    <t>2026-01-24 09:47:11</t>
+  </si>
+  <si>
+    <t>D308</t>
+  </si>
+  <si>
+    <t>上蓋打不開</t>
+  </si>
+  <si>
+    <t>01/24 09:51百大門市啟動緊急叫修:門市反應TM1發票機(BSC-10、BSC10II)更換紙捲後上蓋打開後無法合起來，門市告知無法自行排除...台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03569</t>
+  </si>
+  <si>
+    <t>2026-01-24 09:52:37</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:28:00</t>
+  </si>
+  <si>
+    <t>2026-01-24 15:52:00</t>
+  </si>
+  <si>
+    <t>裁刀為定位. 清潔後即可</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:33:26</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:05:00</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:25:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002967</t>
+  </si>
+  <si>
+    <t>14208115012402</t>
+  </si>
+  <si>
+    <t>新莊瓊泰店</t>
+  </si>
+  <si>
+    <t>2026-01-24 11:53:29</t>
+  </si>
+  <si>
+    <t>1/24 11:50 與總公司明翰確認啟動緊急叫修:SC(SHUTTLE6S)-門市反應TM1.2主檔未更新，顯示01/23，應為01/24，查看SC主檔01/24，執行SC轉TM&gt;手動TM版更&gt;10分鐘後TM執行版更仍異常，客服嘗試至最高權限執行手動排除主檔無法更新&gt;查詢SC主檔為當日&gt;SC轉TM&gt;手動TM版本更新&gt;10分鐘後TM執行版本更新仍異常，經HIPOS執行NewOpen-&gt;手動主檔轉入-&gt;Sc轉tm後，查看sc e檔 trans_in 未丟任何檔案，經總公司圭連告知疑似SC第二硬碟區塊毀損，需到店更換硬碟，並攜帶第一顆硬碟備著...請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳關到01/23，與通訊圭連確認都有收到</t>
+  </si>
+  <si>
+    <t>THILF04208</t>
+  </si>
+  <si>
+    <t>2026-01-24 12:01:58</t>
+  </si>
+  <si>
+    <t>2026-01-24 12:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-24 15:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-24 18:01:00</t>
+  </si>
+  <si>
+    <t>更換第一二顆硬碟不備份還原
+並告知李先生更換硬碟注意事項
+回報0800</t>
+  </si>
+  <si>
+    <t>E4155115012401</t>
+  </si>
+  <si>
+    <t>2026-01-24 17:46:54</t>
+  </si>
+  <si>
+    <t>L90門市反應昨天停電復電後票卷機無法開機無電源反應，門市已有重新拔插按電源健仍異常無反應...須請台芝到店協助(昨晚台電停電 票卷機故障 無法開機)</t>
+  </si>
+  <si>
+    <t>2026-01-24 17:53:36</t>
+  </si>
+  <si>
+    <t>2026-01-26 16:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 16:56:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 13:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重新插拔電源. </t>
+  </si>
+  <si>
+    <t>三重重新橋</t>
+  </si>
+  <si>
+    <t>THILF03627</t>
+  </si>
+  <si>
+    <t>2026-01-26 14:14:40</t>
+  </si>
+  <si>
+    <t>2026-01-26 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 14:13:00</t>
+  </si>
+  <si>
+    <t>裝潢回裝完成</t>
+  </si>
+  <si>
+    <t>2026-01-26 14:23:46</t>
+  </si>
+  <si>
+    <t>2026-01-26 14:00:00</t>
+  </si>
+  <si>
+    <t>回裝已完工已請0800確認版本</t>
+  </si>
+  <si>
+    <t>2026-01-26 16:59:22</t>
+  </si>
+  <si>
+    <t>2026-01-26 16:38:00</t>
+  </si>
+  <si>
+    <t>2026-01-26 16:55:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002791</t>
   </si>
 </sst>
 </file>
@@ -4531,10 +4674,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK200"/>
+  <dimension ref="A1:AK207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC197" sqref="AC197"/>
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21615,7 +21758,7 @@
       <c r="M200" s="4"/>
       <c r="N200" s="3"/>
       <c r="O200" s="4"/>
-      <c r="P200" s="4"/>
+      <c r="P200" s="10"/>
       <c r="Q200" s="3" t="s">
         <v>1296</v>
       </c>
@@ -21648,7 +21791,7 @@
       <c r="AB200" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC200" s="4" t="s">
+      <c r="AC200" s="10" t="s">
         <v>1333</v>
       </c>
       <c r="AD200" s="3" t="s">
@@ -21663,6 +21806,607 @@
         <v>60</v>
       </c>
       <c r="AK200" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="201" spans="1:37">
+      <c r="A201" s="7">
+        <v>199</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C201" s="7">
+        <v>2026013396</v>
+      </c>
+      <c r="D201" s="7" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E201" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F201" s="7">
+        <v>3569</v>
+      </c>
+      <c r="G201" s="7" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H201" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I201" s="7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="J201" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K201" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L201" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="M201" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N201" s="7" t="s">
+        <v>1337</v>
+      </c>
+      <c r="O201" s="8" t="s">
+        <v>1338</v>
+      </c>
+      <c r="P201" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="Q201" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="R201" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S201" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T201" s="7">
+        <v>1</v>
+      </c>
+      <c r="U201" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V201" s="7" t="s">
+        <v>1341</v>
+      </c>
+      <c r="W201" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="X201" s="7" t="s">
+        <v>1343</v>
+      </c>
+      <c r="Y201" s="7" t="s">
+        <v>1344</v>
+      </c>
+      <c r="Z201" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA201" s="7"/>
+      <c r="AB201" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC201" s="9" t="s">
+        <v>1345</v>
+      </c>
+      <c r="AD201" s="7"/>
+      <c r="AE201" s="7"/>
+      <c r="AF201" s="7"/>
+      <c r="AG201" s="7"/>
+      <c r="AH201" s="7"/>
+      <c r="AI201" s="7"/>
+      <c r="AJ201" s="7"/>
+      <c r="AK201" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="202" spans="1:37">
+      <c r="A202" s="3">
+        <v>200</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C202" s="3">
+        <v>2026013401</v>
+      </c>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="3">
+        <v>3569</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H202" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I202" s="3"/>
+      <c r="J202" s="3"/>
+      <c r="K202" s="3"/>
+      <c r="L202" s="3"/>
+      <c r="M202" s="4"/>
+      <c r="N202" s="3"/>
+      <c r="O202" s="4"/>
+      <c r="P202" s="10"/>
+      <c r="Q202" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="R202" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S202" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T202" s="3">
+        <v>1</v>
+      </c>
+      <c r="U202" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V202" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="W202" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="X202" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="Y202" s="3"/>
+      <c r="Z202" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA202" s="3"/>
+      <c r="AB202" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC202" s="10" t="s">
+        <v>1349</v>
+      </c>
+      <c r="AD202" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE202" s="3"/>
+      <c r="AF202" s="3"/>
+      <c r="AG202" s="3"/>
+      <c r="AH202" s="3"/>
+      <c r="AI202" s="3"/>
+      <c r="AJ202" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK202" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="203" spans="1:37">
+      <c r="A203" s="7">
+        <v>201</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C203" s="7">
+        <v>2026013402</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E203" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F203" s="7">
+        <v>4208</v>
+      </c>
+      <c r="G203" s="7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="H203" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I203" s="7" t="s">
+        <v>1352</v>
+      </c>
+      <c r="J203" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K203" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L203" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="M203" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="N203" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O203" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="P203" s="9" t="s">
+        <v>1353</v>
+      </c>
+      <c r="Q203" s="7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="R203" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S203" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T203" s="7">
+        <v>1</v>
+      </c>
+      <c r="U203" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V203" s="7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="W203" s="7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="X203" s="7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="Y203" s="7" t="s">
+        <v>1358</v>
+      </c>
+      <c r="Z203" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="AA203" s="7"/>
+      <c r="AB203" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC203" s="9" t="s">
+        <v>1359</v>
+      </c>
+      <c r="AD203" s="7"/>
+      <c r="AE203" s="7"/>
+      <c r="AF203" s="7"/>
+      <c r="AG203" s="7"/>
+      <c r="AH203" s="7"/>
+      <c r="AI203" s="7"/>
+      <c r="AJ203" s="7"/>
+      <c r="AK203" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="204" spans="1:37">
+      <c r="A204" s="3">
+        <v>202</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C204" s="3">
+        <v>2026013406</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F204" s="3">
+        <v>4155</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="H204" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I204" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="J204" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K204" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L204" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="M204" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="N204" s="3">
+        <v>6004</v>
+      </c>
+      <c r="O204" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P204" s="10" t="s">
+        <v>1362</v>
+      </c>
+      <c r="Q204" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="R204" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S204" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T204" s="3">
+        <v>1</v>
+      </c>
+      <c r="U204" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V204" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="W204" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="X204" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="Y204" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="Z204" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA204" s="3"/>
+      <c r="AB204" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC204" s="10" t="s">
+        <v>1367</v>
+      </c>
+      <c r="AD204" s="3"/>
+      <c r="AE204" s="3"/>
+      <c r="AF204" s="3"/>
+      <c r="AG204" s="3"/>
+      <c r="AH204" s="3"/>
+      <c r="AI204" s="3"/>
+      <c r="AJ204" s="3"/>
+      <c r="AK204" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="205" spans="1:37">
+      <c r="A205" s="7">
+        <v>203</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C205" s="7">
+        <v>2026013468</v>
+      </c>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7">
+        <v>3627</v>
+      </c>
+      <c r="G205" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="H205" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I205" s="7"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="8"/>
+      <c r="N205" s="7"/>
+      <c r="O205" s="8"/>
+      <c r="P205" s="9"/>
+      <c r="Q205" s="7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="R205" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S205" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T205" s="7">
+        <v>1</v>
+      </c>
+      <c r="U205" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V205" s="7" t="s">
+        <v>1370</v>
+      </c>
+      <c r="W205" s="7" t="s">
+        <v>1371</v>
+      </c>
+      <c r="X205" s="7" t="s">
+        <v>1372</v>
+      </c>
+      <c r="Y205" s="7"/>
+      <c r="Z205" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="AA205" s="7"/>
+      <c r="AB205" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC205" s="9" t="s">
+        <v>1373</v>
+      </c>
+      <c r="AD205" s="7"/>
+      <c r="AE205" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF205" s="7"/>
+      <c r="AG205" s="7"/>
+      <c r="AH205" s="7"/>
+      <c r="AI205" s="7"/>
+      <c r="AJ205" s="7"/>
+      <c r="AK205" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="206" spans="1:37">
+      <c r="A206" s="3">
+        <v>204</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C206" s="3">
+        <v>2026013473</v>
+      </c>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="3">
+        <v>3627</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="H206" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I206" s="3"/>
+      <c r="J206" s="3"/>
+      <c r="K206" s="3"/>
+      <c r="L206" s="3"/>
+      <c r="M206" s="4"/>
+      <c r="N206" s="3"/>
+      <c r="O206" s="4"/>
+      <c r="P206" s="10"/>
+      <c r="Q206" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="R206" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S206" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T206" s="3">
+        <v>1</v>
+      </c>
+      <c r="U206" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V206" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="W206" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="X206" s="3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="Y206" s="3"/>
+      <c r="Z206" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA206" s="3"/>
+      <c r="AB206" s="3"/>
+      <c r="AC206" s="10" t="s">
+        <v>1376</v>
+      </c>
+      <c r="AD206" s="3"/>
+      <c r="AE206" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF206" s="3"/>
+      <c r="AG206" s="3"/>
+      <c r="AH206" s="3"/>
+      <c r="AI206" s="3"/>
+      <c r="AJ206" s="3"/>
+      <c r="AK206" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="207" spans="1:37">
+      <c r="A207" s="7">
+        <v>205</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C207" s="7">
+        <v>2026013499</v>
+      </c>
+      <c r="D207" s="7"/>
+      <c r="E207" s="7"/>
+      <c r="F207" s="7">
+        <v>4155</v>
+      </c>
+      <c r="G207" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="H207" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I207" s="7"/>
+      <c r="J207" s="7"/>
+      <c r="K207" s="7"/>
+      <c r="L207" s="7"/>
+      <c r="M207" s="8"/>
+      <c r="N207" s="7"/>
+      <c r="O207" s="8"/>
+      <c r="P207" s="8"/>
+      <c r="Q207" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="R207" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S207" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T207" s="7">
+        <v>1</v>
+      </c>
+      <c r="U207" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V207" s="7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="W207" s="7" t="s">
+        <v>1378</v>
+      </c>
+      <c r="X207" s="7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="Y207" s="7"/>
+      <c r="Z207" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA207" s="7"/>
+      <c r="AB207" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC207" s="8" t="s">
+        <v>1380</v>
+      </c>
+      <c r="AD207" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE207" s="7"/>
+      <c r="AF207" s="7"/>
+      <c r="AG207" s="7"/>
+      <c r="AH207" s="7"/>
+      <c r="AI207" s="7"/>
+      <c r="AJ207" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK207" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01270957
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$207</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$208</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1381">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-26  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1389">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-27  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -4222,6 +4222,30 @@
   </si>
   <si>
     <t xml:space="preserve">重新插拔電源. </t>
+  </si>
+  <si>
+    <t>13785115012601</t>
+  </si>
+  <si>
+    <t>2026-01-26 10:50:55</t>
+  </si>
+  <si>
+    <t>TM2(TCX800)錢匣彈簧斷3個(抽屜顏色:白、鑰匙孔:右、鑰匙孔編號:702)..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-26 10:56:43</t>
+  </si>
+  <si>
+    <t>2026-01-27 09:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 14:56:00</t>
+  </si>
+  <si>
+    <t>重裝彈簧</t>
   </si>
   <si>
     <t>三重重新橋</t>
@@ -4674,10 +4698,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK207"/>
+  <dimension ref="A1:AK208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A207" sqref="A207"/>
+      <selection activeCell="AC205" sqref="AC205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22184,38 +22208,58 @@
         <v>203</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C205" s="7">
-        <v>2026013468</v>
-      </c>
-      <c r="D205" s="7"/>
-      <c r="E205" s="7"/>
+        <v>2026013439</v>
+      </c>
+      <c r="D205" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E205" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F205" s="7">
-        <v>3627</v>
+        <v>3785</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>1368</v>
+        <v>191</v>
       </c>
       <c r="H205" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I205" s="7"/>
-      <c r="J205" s="7"/>
-      <c r="K205" s="7"/>
-      <c r="L205" s="7"/>
-      <c r="M205" s="8"/>
-      <c r="N205" s="7"/>
-      <c r="O205" s="8"/>
-      <c r="P205" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="I205" s="7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="J205" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="K205" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L205" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M205" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N205" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O205" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="P205" s="9" t="s">
+        <v>1370</v>
+      </c>
       <c r="Q205" s="7" t="s">
-        <v>1369</v>
+        <v>198</v>
       </c>
       <c r="R205" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S205" s="7" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="T205" s="7">
         <v>1</v>
@@ -22224,29 +22268,29 @@
         <v>53</v>
       </c>
       <c r="V205" s="7" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="W205" s="7" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="X205" s="7" t="s">
-        <v>1372</v>
-      </c>
-      <c r="Y205" s="7"/>
+        <v>1373</v>
+      </c>
+      <c r="Y205" s="7" t="s">
+        <v>1374</v>
+      </c>
       <c r="Z205" s="7">
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="AA205" s="7"/>
       <c r="AB205" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC205" s="9" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="AD205" s="7"/>
-      <c r="AE205" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE205" s="7"/>
       <c r="AF205" s="7"/>
       <c r="AG205" s="7"/>
       <c r="AH205" s="7"/>
@@ -22264,7 +22308,7 @@
         <v>118</v>
       </c>
       <c r="C206" s="3">
-        <v>2026013473</v>
+        <v>2026013468</v>
       </c>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
@@ -22272,7 +22316,7 @@
         <v>3627</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>1368</v>
+        <v>1376</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>92</v>
@@ -22286,13 +22330,13 @@
       <c r="O206" s="4"/>
       <c r="P206" s="10"/>
       <c r="Q206" s="3" t="s">
-        <v>1369</v>
+        <v>1377</v>
       </c>
       <c r="R206" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S206" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T206" s="3">
         <v>1</v>
@@ -22301,22 +22345,24 @@
         <v>53</v>
       </c>
       <c r="V206" s="3" t="s">
-        <v>1374</v>
+        <v>1378</v>
       </c>
       <c r="W206" s="3" t="s">
-        <v>1371</v>
+        <v>1379</v>
       </c>
       <c r="X206" s="3" t="s">
-        <v>1375</v>
+        <v>1380</v>
       </c>
       <c r="Y206" s="3"/>
       <c r="Z206" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="AA206" s="3"/>
-      <c r="AB206" s="3"/>
+      <c r="AB206" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="AC206" s="10" t="s">
-        <v>1376</v>
+        <v>1381</v>
       </c>
       <c r="AD206" s="3"/>
       <c r="AE206" s="3" t="s">
@@ -22339,15 +22385,15 @@
         <v>118</v>
       </c>
       <c r="C207" s="7">
-        <v>2026013499</v>
+        <v>2026013473</v>
       </c>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
       <c r="F207" s="7">
-        <v>4155</v>
+        <v>3627</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>732</v>
+        <v>1376</v>
       </c>
       <c r="H207" s="7" t="s">
         <v>92</v>
@@ -22359,9 +22405,9 @@
       <c r="M207" s="8"/>
       <c r="N207" s="7"/>
       <c r="O207" s="8"/>
-      <c r="P207" s="8"/>
+      <c r="P207" s="9"/>
       <c r="Q207" s="7" t="s">
-        <v>735</v>
+        <v>1377</v>
       </c>
       <c r="R207" s="7" t="s">
         <v>51</v>
@@ -22376,37 +22422,112 @@
         <v>53</v>
       </c>
       <c r="V207" s="7" t="s">
-        <v>1377</v>
+        <v>1382</v>
       </c>
       <c r="W207" s="7" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="X207" s="7" t="s">
-        <v>1379</v>
+        <v>1383</v>
       </c>
       <c r="Y207" s="7"/>
       <c r="Z207" s="7">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="AA207" s="7"/>
-      <c r="AB207" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC207" s="8" t="s">
-        <v>1380</v>
-      </c>
-      <c r="AD207" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE207" s="7"/>
+      <c r="AB207" s="7"/>
+      <c r="AC207" s="9" t="s">
+        <v>1384</v>
+      </c>
+      <c r="AD207" s="7"/>
+      <c r="AE207" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AF207" s="7"/>
       <c r="AG207" s="7"/>
       <c r="AH207" s="7"/>
       <c r="AI207" s="7"/>
-      <c r="AJ207" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ207" s="7"/>
       <c r="AK207" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="208" spans="1:37">
+      <c r="A208" s="3">
+        <v>206</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C208" s="3">
+        <v>2026013499</v>
+      </c>
+      <c r="D208" s="3"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="3">
+        <v>4155</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="H208" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I208" s="3"/>
+      <c r="J208" s="3"/>
+      <c r="K208" s="3"/>
+      <c r="L208" s="3"/>
+      <c r="M208" s="4"/>
+      <c r="N208" s="3"/>
+      <c r="O208" s="4"/>
+      <c r="P208" s="4"/>
+      <c r="Q208" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="R208" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S208" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T208" s="3">
+        <v>1</v>
+      </c>
+      <c r="U208" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V208" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="W208" s="3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="X208" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="Y208" s="3"/>
+      <c r="Z208" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA208" s="3"/>
+      <c r="AB208" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC208" s="4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="AD208" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE208" s="3"/>
+      <c r="AF208" s="3"/>
+      <c r="AG208" s="3"/>
+      <c r="AH208" s="3"/>
+      <c r="AI208" s="3"/>
+      <c r="AJ208" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK208" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01271718
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$208</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$213</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1424">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-27  )</t>
   </si>
@@ -4248,6 +4248,33 @@
     <t>重裝彈簧</t>
   </si>
   <si>
+    <t>E2201115012601</t>
+  </si>
+  <si>
+    <t>2026-01-26 10:52:04</t>
+  </si>
+  <si>
+    <t>性質轉換門市反應TM1 CCD掃描器(HC56IITR)刷讀所有條碼都無反應，無亮燈無嗶聲，要求協助更換......請台芝到店協助(刷槍無法刷)</t>
+  </si>
+  <si>
+    <t>未完工</t>
+  </si>
+  <si>
+    <t>2026-01-26 11:09:50</t>
+  </si>
+  <si>
+    <t>2026-01-27 14:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:09:00</t>
+  </si>
+  <si>
+    <t>因特殊線材損壞，須再更換線材</t>
+  </si>
+  <si>
     <t>三重重新橋</t>
   </si>
   <si>
@@ -4285,6 +4312,85 @@
   </si>
   <si>
     <t>PMQ1+7210002791</t>
+  </si>
+  <si>
+    <t>1F777115012701</t>
+  </si>
+  <si>
+    <t>F777</t>
+  </si>
+  <si>
+    <t>蘆竹南華店</t>
+  </si>
+  <si>
+    <t>2026-01-27 09:40:48</t>
+  </si>
+  <si>
+    <t>1/27 10:18 與總公司明翰確認啟動緊急叫修:SC(SHUTTLE6S)-門市反應從元旦開始，頻繁發生SC接收不到總部主檔異狀，都需門市自行手動接收並主檔轉入後才正常，或頻繁發生銷售沒有回傳成功的紅字提示，門市告知今天SC再度出現需請門市接收總部主檔的紅色提示視窗，門市依提示說明操作後，僅TM1更新後主檔為1/27，TM2仍顯示1/26，客服欲執行NEWOPEN&gt;主檔轉入作業時出現您的應用程式發生未處理的例外狀況，經總公司功評檢視相關紀錄後發現SC主機第二顆硬碟(ST1000LM048-2E7172  \\\\.\\PHYSICALDRIVE1  1000202273280 )裝置 \\Device\\Harddisk1\\DR1 有損壞區塊，請協助派工到店更換一二顆硬碟不備份還原。..請台芝到店協助 PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認帳務做到01/26，與功評確認有收到01/26的銷售</t>
+  </si>
+  <si>
+    <t>THILF0F777</t>
+  </si>
+  <si>
+    <t>2026-01-27 10:19:12</t>
+  </si>
+  <si>
+    <t>2026-01-27 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 16:19:00</t>
+  </si>
+  <si>
+    <t>更換第一顆及第二顆硬碟不備份
+更換Sata線一條</t>
+  </si>
+  <si>
+    <t>14748115012701</t>
+  </si>
+  <si>
+    <t>中和霸氣店</t>
+  </si>
+  <si>
+    <t>2026-01-27 10:54:04</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)抽屜無法關閉完全，抽屜外觀米白/鑰匙孔中/鑰匙孔編號:5001，已拿出重放以及無異物仍異常....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04748</t>
+  </si>
+  <si>
+    <t>2026-01-27 10:55:31</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:20:00</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 14:55:00</t>
+  </si>
+  <si>
+    <t>後方鐵架歪掉.已僑正</t>
+  </si>
+  <si>
+    <t>2026-01-27 13:41:52</t>
+  </si>
+  <si>
+    <t>2026-01-27 13:41:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002745+L90</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:52:20</t>
+  </si>
+  <si>
+    <t>2026-01-27 15:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002974</t>
   </si>
 </sst>
 </file>
@@ -4698,10 +4804,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK208"/>
+  <dimension ref="A1:AK213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC205" sqref="AC205"/>
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22305,32 +22411,52 @@
         <v>204</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C206" s="3">
-        <v>2026013468</v>
-      </c>
-      <c r="D206" s="3"/>
-      <c r="E206" s="3"/>
+        <v>2026013442</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F206" s="3">
-        <v>3627</v>
+        <v>2201</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>1376</v>
+        <v>671</v>
       </c>
       <c r="H206" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I206" s="3"/>
-      <c r="J206" s="3"/>
-      <c r="K206" s="3"/>
-      <c r="L206" s="3"/>
-      <c r="M206" s="4"/>
-      <c r="N206" s="3"/>
-      <c r="O206" s="4"/>
-      <c r="P206" s="10"/>
+        <v>106</v>
+      </c>
+      <c r="I206" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J206" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L206" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M206" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N206" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O206" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P206" s="10" t="s">
+        <v>1378</v>
+      </c>
       <c r="Q206" s="3" t="s">
-        <v>1377</v>
+        <v>674</v>
       </c>
       <c r="R206" s="3" t="s">
         <v>51</v>
@@ -22342,32 +22468,32 @@
         <v>1</v>
       </c>
       <c r="U206" s="3" t="s">
-        <v>53</v>
+        <v>1379</v>
       </c>
       <c r="V206" s="3" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="W206" s="3" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="X206" s="3" t="s">
-        <v>1380</v>
-      </c>
-      <c r="Y206" s="3"/>
+        <v>1382</v>
+      </c>
+      <c r="Y206" s="3" t="s">
+        <v>1383</v>
+      </c>
       <c r="Z206" s="3">
-        <v>3.2</v>
+        <v>0.5</v>
       </c>
       <c r="AA206" s="3"/>
       <c r="AB206" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC206" s="10" t="s">
-        <v>1381</v>
+        <v>1384</v>
       </c>
       <c r="AD206" s="3"/>
-      <c r="AE206" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE206" s="3"/>
       <c r="AF206" s="3"/>
       <c r="AG206" s="3"/>
       <c r="AH206" s="3"/>
@@ -22385,7 +22511,7 @@
         <v>118</v>
       </c>
       <c r="C207" s="7">
-        <v>2026013473</v>
+        <v>2026013468</v>
       </c>
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
@@ -22393,7 +22519,7 @@
         <v>3627</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>1376</v>
+        <v>1385</v>
       </c>
       <c r="H207" s="7" t="s">
         <v>92</v>
@@ -22407,13 +22533,13 @@
       <c r="O207" s="8"/>
       <c r="P207" s="9"/>
       <c r="Q207" s="7" t="s">
-        <v>1377</v>
+        <v>1386</v>
       </c>
       <c r="R207" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S207" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T207" s="7">
         <v>1</v>
@@ -22422,22 +22548,24 @@
         <v>53</v>
       </c>
       <c r="V207" s="7" t="s">
-        <v>1382</v>
+        <v>1387</v>
       </c>
       <c r="W207" s="7" t="s">
-        <v>1379</v>
+        <v>1388</v>
       </c>
       <c r="X207" s="7" t="s">
-        <v>1383</v>
+        <v>1389</v>
       </c>
       <c r="Y207" s="7"/>
       <c r="Z207" s="7">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="AA207" s="7"/>
-      <c r="AB207" s="7"/>
+      <c r="AB207" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="AC207" s="9" t="s">
-        <v>1384</v>
+        <v>1390</v>
       </c>
       <c r="AD207" s="7"/>
       <c r="AE207" s="7" t="s">
@@ -22460,15 +22588,15 @@
         <v>118</v>
       </c>
       <c r="C208" s="3">
-        <v>2026013499</v>
+        <v>2026013473</v>
       </c>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
       <c r="F208" s="3">
-        <v>4155</v>
+        <v>3627</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>732</v>
+        <v>1385</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>92</v>
@@ -22480,9 +22608,9 @@
       <c r="M208" s="4"/>
       <c r="N208" s="3"/>
       <c r="O208" s="4"/>
-      <c r="P208" s="4"/>
+      <c r="P208" s="10"/>
       <c r="Q208" s="3" t="s">
-        <v>735</v>
+        <v>1386</v>
       </c>
       <c r="R208" s="3" t="s">
         <v>51</v>
@@ -22497,37 +22625,462 @@
         <v>53</v>
       </c>
       <c r="V208" s="3" t="s">
-        <v>1385</v>
+        <v>1391</v>
       </c>
       <c r="W208" s="3" t="s">
-        <v>1386</v>
+        <v>1388</v>
       </c>
       <c r="X208" s="3" t="s">
-        <v>1387</v>
+        <v>1392</v>
       </c>
       <c r="Y208" s="3"/>
       <c r="Z208" s="3">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="AA208" s="3"/>
-      <c r="AB208" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC208" s="4" t="s">
-        <v>1388</v>
-      </c>
-      <c r="AD208" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE208" s="3"/>
+      <c r="AB208" s="3"/>
+      <c r="AC208" s="10" t="s">
+        <v>1393</v>
+      </c>
+      <c r="AD208" s="3"/>
+      <c r="AE208" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AF208" s="3"/>
       <c r="AG208" s="3"/>
       <c r="AH208" s="3"/>
       <c r="AI208" s="3"/>
-      <c r="AJ208" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ208" s="3"/>
       <c r="AK208" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="209" spans="1:37">
+      <c r="A209" s="7">
+        <v>207</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C209" s="7">
+        <v>2026013499</v>
+      </c>
+      <c r="D209" s="7"/>
+      <c r="E209" s="7"/>
+      <c r="F209" s="7">
+        <v>4155</v>
+      </c>
+      <c r="G209" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="H209" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I209" s="7"/>
+      <c r="J209" s="7"/>
+      <c r="K209" s="7"/>
+      <c r="L209" s="7"/>
+      <c r="M209" s="8"/>
+      <c r="N209" s="7"/>
+      <c r="O209" s="8"/>
+      <c r="P209" s="9"/>
+      <c r="Q209" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="R209" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S209" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T209" s="7">
+        <v>1</v>
+      </c>
+      <c r="U209" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V209" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="W209" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="X209" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="Y209" s="7"/>
+      <c r="Z209" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA209" s="7"/>
+      <c r="AB209" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC209" s="9" t="s">
+        <v>1397</v>
+      </c>
+      <c r="AD209" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE209" s="7"/>
+      <c r="AF209" s="7"/>
+      <c r="AG209" s="7"/>
+      <c r="AH209" s="7"/>
+      <c r="AI209" s="7"/>
+      <c r="AJ209" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK209" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="210" spans="1:37">
+      <c r="A210" s="3">
+        <v>208</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C210" s="3">
+        <v>2026013525</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H210" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="J210" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K210" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L210" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M210" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="N210" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O210" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P210" s="10" t="s">
+        <v>1402</v>
+      </c>
+      <c r="Q210" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="R210" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S210" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T210" s="3">
+        <v>1</v>
+      </c>
+      <c r="U210" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V210" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="W210" s="3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="X210" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="Y210" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="Z210" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA210" s="3"/>
+      <c r="AB210" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC210" s="10" t="s">
+        <v>1407</v>
+      </c>
+      <c r="AD210" s="3"/>
+      <c r="AE210" s="3"/>
+      <c r="AF210" s="3"/>
+      <c r="AG210" s="3"/>
+      <c r="AH210" s="3"/>
+      <c r="AI210" s="3"/>
+      <c r="AJ210" s="3"/>
+      <c r="AK210" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="211" spans="1:37">
+      <c r="A211" s="7">
+        <v>209</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C211" s="7">
+        <v>2026013542</v>
+      </c>
+      <c r="D211" s="7" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E211" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F211" s="7">
+        <v>4748</v>
+      </c>
+      <c r="G211" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="H211" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I211" s="7" t="s">
+        <v>1410</v>
+      </c>
+      <c r="J211" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K211" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L211" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M211" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N211" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O211" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="P211" s="9" t="s">
+        <v>1411</v>
+      </c>
+      <c r="Q211" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="R211" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S211" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T211" s="7">
+        <v>1</v>
+      </c>
+      <c r="U211" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V211" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="W211" s="7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="X211" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="Y211" s="7" t="s">
+        <v>1416</v>
+      </c>
+      <c r="Z211" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA211" s="7"/>
+      <c r="AB211" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC211" s="9" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AD211" s="7"/>
+      <c r="AE211" s="7"/>
+      <c r="AF211" s="7"/>
+      <c r="AG211" s="7"/>
+      <c r="AH211" s="7"/>
+      <c r="AI211" s="7"/>
+      <c r="AJ211" s="7"/>
+      <c r="AK211" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="212" spans="1:37">
+      <c r="A212" s="3">
+        <v>210</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C212" s="3">
+        <v>2026013586</v>
+      </c>
+      <c r="D212" s="3"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I212" s="3"/>
+      <c r="J212" s="3"/>
+      <c r="K212" s="3"/>
+      <c r="L212" s="3"/>
+      <c r="M212" s="4"/>
+      <c r="N212" s="3"/>
+      <c r="O212" s="4"/>
+      <c r="P212" s="10"/>
+      <c r="Q212" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="R212" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S212" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T212" s="3">
+        <v>1</v>
+      </c>
+      <c r="U212" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V212" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="W212" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="X212" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="Y212" s="3"/>
+      <c r="Z212" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA212" s="3"/>
+      <c r="AB212" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC212" s="10" t="s">
+        <v>1420</v>
+      </c>
+      <c r="AD212" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE212" s="3"/>
+      <c r="AF212" s="3"/>
+      <c r="AG212" s="3"/>
+      <c r="AH212" s="3"/>
+      <c r="AI212" s="3"/>
+      <c r="AJ212" s="3"/>
+      <c r="AK212" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="213" spans="1:37">
+      <c r="A213" s="7">
+        <v>211</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C213" s="7">
+        <v>2026013614</v>
+      </c>
+      <c r="D213" s="7"/>
+      <c r="E213" s="7"/>
+      <c r="F213" s="7">
+        <v>4748</v>
+      </c>
+      <c r="G213" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="H213" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I213" s="7"/>
+      <c r="J213" s="7"/>
+      <c r="K213" s="7"/>
+      <c r="L213" s="7"/>
+      <c r="M213" s="8"/>
+      <c r="N213" s="7"/>
+      <c r="O213" s="8"/>
+      <c r="P213" s="8"/>
+      <c r="Q213" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="R213" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S213" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T213" s="7">
+        <v>1</v>
+      </c>
+      <c r="U213" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V213" s="7" t="s">
+        <v>1421</v>
+      </c>
+      <c r="W213" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="X213" s="7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="Y213" s="7"/>
+      <c r="Z213" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA213" s="7"/>
+      <c r="AB213" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC213" s="8" t="s">
+        <v>1423</v>
+      </c>
+      <c r="AD213" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE213" s="7"/>
+      <c r="AF213" s="7"/>
+      <c r="AG213" s="7"/>
+      <c r="AH213" s="7"/>
+      <c r="AI213" s="7"/>
+      <c r="AJ213" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK213" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01291358
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$213</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$225</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1424">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-27  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1495">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-29  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -4257,9 +4257,6 @@
     <t>性質轉換門市反應TM1 CCD掃描器(HC56IITR)刷讀所有條碼都無反應，無亮燈無嗶聲，要求協助更換......請台芝到店協助(刷槍無法刷)</t>
   </si>
   <si>
-    <t>未完工</t>
-  </si>
-  <si>
     <t>2026-01-26 11:09:50</t>
   </si>
   <si>
@@ -4273,6 +4270,17 @@
   </si>
   <si>
     <t>因特殊線材損壞，須再更換線材</t>
+  </si>
+  <si>
+    <t>2026-01-27 16:00:00</t>
+  </si>
+  <si>
+    <t>0小時51分鐘</t>
+  </si>
+  <si>
+    <t>更換掃描槍及轉接頭
+換下8119006248
+換上8119013691</t>
   </si>
   <si>
     <t>三重重新橋</t>
@@ -4384,6 +4392,29 @@
     <t>PMQ1+7210002745+L90</t>
   </si>
   <si>
+    <t>E2201115012701</t>
+  </si>
+  <si>
+    <t>2026-01-27 14:50:10</t>
+  </si>
+  <si>
+    <t>門市反應TM2掃描槍(HC56II TR)所有商品與條碼都感應不良很難刷讀，確認有亮燈有逼聲、鼠標有在輸入的位置，先前已執行過掃槍校正仍異常...需請台芝到店協助(機2刷槍無法刷)</t>
+  </si>
+  <si>
+    <t>2026-01-27 14:55:15</t>
+  </si>
+  <si>
+    <t>2026-01-27 17:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 18:55:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119006249
+換上8119013215</t>
+  </si>
+  <si>
     <t>2026-01-27 15:52:20</t>
   </si>
   <si>
@@ -4391,6 +4422,192 @@
   </si>
   <si>
     <t>PMQ1+7210002974</t>
+  </si>
+  <si>
+    <t>2026-01-27 19:28:57</t>
+  </si>
+  <si>
+    <t>2026-01-27 17:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002721+L90</t>
+  </si>
+  <si>
+    <t>1D070115012802</t>
+  </si>
+  <si>
+    <t>2026-01-28 09:03:58</t>
+  </si>
+  <si>
+    <t>門市反應票券機L90燈號僅亮綠燈，但刷讀LIFEET小白單TM顯示印票機異常，點選偵測印票機也顯示異常，已有關機紙捲重裝仍無法排除異狀...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-01-28 09:06:41</t>
+  </si>
+  <si>
+    <t>2026-01-28 13:03:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 13:24:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 13:06:00</t>
+  </si>
+  <si>
+    <t>90印票機網路線脫落插回即可列印</t>
+  </si>
+  <si>
+    <t>新莊雙鳳店</t>
+  </si>
+  <si>
+    <t>THILF04005</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:16:22</t>
+  </si>
+  <si>
+    <t>2026-01-28 10:30:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003059</t>
+  </si>
+  <si>
+    <t>L562</t>
+  </si>
+  <si>
+    <t>田倉民安店</t>
+  </si>
+  <si>
+    <t>THILF0L562</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:27:48</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:30:00</t>
+  </si>
+  <si>
+    <t>C742</t>
+  </si>
+  <si>
+    <t>中和景安站</t>
+  </si>
+  <si>
+    <t>THILF0C742</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:44:57</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:18:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002983</t>
+  </si>
+  <si>
+    <t>C660</t>
+  </si>
+  <si>
+    <t>中和永安市場</t>
+  </si>
+  <si>
+    <t>THILF0C660</t>
+  </si>
+  <si>
+    <t>2026-01-28 12:20:06</t>
+  </si>
+  <si>
+    <t>2026-01-28 11:50:00</t>
+  </si>
+  <si>
+    <t>2026-01-28 12:16:00</t>
+  </si>
+  <si>
+    <t>D191</t>
+  </si>
+  <si>
+    <t>三重興德店</t>
+  </si>
+  <si>
+    <t>THILF0D191</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:22:37</t>
+  </si>
+  <si>
+    <t>2026-01-29 10:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:08:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002820</t>
+  </si>
+  <si>
+    <t>三重初戀店</t>
+  </si>
+  <si>
+    <t>THILF04977</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:43:26</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:15:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:37:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002809</t>
+  </si>
+  <si>
+    <t>D087</t>
+  </si>
+  <si>
+    <t>三重中興北</t>
+  </si>
+  <si>
+    <t>THILF0D087</t>
+  </si>
+  <si>
+    <t>2026-01-29 12:34:17</t>
+  </si>
+  <si>
+    <t>2026-01-29 11:45:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 12:09:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002818</t>
+  </si>
+  <si>
+    <t>L535</t>
+  </si>
+  <si>
+    <t>田倉新樹店</t>
+  </si>
+  <si>
+    <t>THILF0L535</t>
+  </si>
+  <si>
+    <t>2026-01-29 13:41:06</t>
+  </si>
+  <si>
+    <t>2026-01-29 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 13:30:00</t>
   </si>
 </sst>
 </file>
@@ -4804,10 +5021,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK213"/>
+  <dimension ref="A1:AK225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A213" sqref="A213"/>
+      <selection activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22468,19 +22685,19 @@
         <v>1</v>
       </c>
       <c r="U206" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V206" s="3" t="s">
         <v>1379</v>
       </c>
-      <c r="V206" s="3" t="s">
+      <c r="W206" s="3" t="s">
         <v>1380</v>
       </c>
-      <c r="W206" s="3" t="s">
+      <c r="X206" s="3" t="s">
         <v>1381</v>
       </c>
-      <c r="X206" s="3" t="s">
+      <c r="Y206" s="3" t="s">
         <v>1382</v>
-      </c>
-      <c r="Y206" s="3" t="s">
-        <v>1383</v>
       </c>
       <c r="Z206" s="3">
         <v>0.5</v>
@@ -22490,7 +22707,7 @@
         <v>58</v>
       </c>
       <c r="AC206" s="10" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="AD206" s="3"/>
       <c r="AE206" s="3"/>
@@ -22508,32 +22725,52 @@
         <v>205</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C207" s="7">
-        <v>2026013468</v>
-      </c>
-      <c r="D207" s="7"/>
-      <c r="E207" s="7"/>
+        <v>2026013442</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E207" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F207" s="7">
-        <v>3627</v>
+        <v>2201</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>1385</v>
+        <v>671</v>
       </c>
       <c r="H207" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I207" s="7"/>
-      <c r="J207" s="7"/>
-      <c r="K207" s="7"/>
-      <c r="L207" s="7"/>
-      <c r="M207" s="8"/>
-      <c r="N207" s="7"/>
-      <c r="O207" s="8"/>
-      <c r="P207" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="I207" s="7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J207" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="K207" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L207" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M207" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="N207" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O207" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="P207" s="9" t="s">
+        <v>1378</v>
+      </c>
       <c r="Q207" s="7" t="s">
-        <v>1386</v>
+        <v>674</v>
       </c>
       <c r="R207" s="7" t="s">
         <v>51</v>
@@ -22542,35 +22779,37 @@
         <v>113</v>
       </c>
       <c r="T207" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U207" s="7" t="s">
         <v>53</v>
       </c>
       <c r="V207" s="7" t="s">
-        <v>1387</v>
+        <v>1379</v>
       </c>
       <c r="W207" s="7" t="s">
-        <v>1388</v>
+        <v>1381</v>
       </c>
       <c r="X207" s="7" t="s">
-        <v>1389</v>
-      </c>
-      <c r="Y207" s="7"/>
+        <v>1384</v>
+      </c>
+      <c r="Y207" s="7" t="s">
+        <v>1382</v>
+      </c>
       <c r="Z207" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="AA207" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA207" s="7" t="s">
+        <v>1385</v>
+      </c>
       <c r="AB207" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC207" s="9" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="AD207" s="7"/>
-      <c r="AE207" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE207" s="7"/>
       <c r="AF207" s="7"/>
       <c r="AG207" s="7"/>
       <c r="AH207" s="7"/>
@@ -22588,7 +22827,7 @@
         <v>118</v>
       </c>
       <c r="C208" s="3">
-        <v>2026013473</v>
+        <v>2026013468</v>
       </c>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
@@ -22596,7 +22835,7 @@
         <v>3627</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>92</v>
@@ -22610,13 +22849,13 @@
       <c r="O208" s="4"/>
       <c r="P208" s="10"/>
       <c r="Q208" s="3" t="s">
-        <v>1386</v>
+        <v>1388</v>
       </c>
       <c r="R208" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S208" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T208" s="3">
         <v>1</v>
@@ -22625,22 +22864,24 @@
         <v>53</v>
       </c>
       <c r="V208" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="W208" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="X208" s="3" t="s">
         <v>1391</v>
-      </c>
-      <c r="W208" s="3" t="s">
-        <v>1388</v>
-      </c>
-      <c r="X208" s="3" t="s">
-        <v>1392</v>
       </c>
       <c r="Y208" s="3"/>
       <c r="Z208" s="3">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="AA208" s="3"/>
-      <c r="AB208" s="3"/>
+      <c r="AB208" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="AC208" s="10" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="AD208" s="3"/>
       <c r="AE208" s="3" t="s">
@@ -22663,15 +22904,15 @@
         <v>118</v>
       </c>
       <c r="C209" s="7">
-        <v>2026013499</v>
+        <v>2026013473</v>
       </c>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
       <c r="F209" s="7">
-        <v>4155</v>
+        <v>3627</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>732</v>
+        <v>1387</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>92</v>
@@ -22685,7 +22926,7 @@
       <c r="O209" s="8"/>
       <c r="P209" s="9"/>
       <c r="Q209" s="7" t="s">
-        <v>735</v>
+        <v>1388</v>
       </c>
       <c r="R209" s="7" t="s">
         <v>51</v>
@@ -22700,36 +22941,32 @@
         <v>53</v>
       </c>
       <c r="V209" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="W209" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="X209" s="7" t="s">
         <v>1394</v>
-      </c>
-      <c r="W209" s="7" t="s">
-        <v>1395</v>
-      </c>
-      <c r="X209" s="7" t="s">
-        <v>1396</v>
       </c>
       <c r="Y209" s="7"/>
       <c r="Z209" s="7">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="AA209" s="7"/>
-      <c r="AB209" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="AB209" s="7"/>
       <c r="AC209" s="9" t="s">
-        <v>1397</v>
-      </c>
-      <c r="AD209" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE209" s="7"/>
+        <v>1395</v>
+      </c>
+      <c r="AD209" s="7"/>
+      <c r="AE209" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AF209" s="7"/>
       <c r="AG209" s="7"/>
       <c r="AH209" s="7"/>
       <c r="AI209" s="7"/>
-      <c r="AJ209" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ209" s="7"/>
       <c r="AK209" s="7" t="s">
         <v>60</v>
       </c>
@@ -22739,58 +22976,38 @@
         <v>208</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
       <c r="C210" s="3">
-        <v>2026013525</v>
-      </c>
-      <c r="D210" s="3" t="s">
-        <v>1398</v>
-      </c>
-      <c r="E210" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F210" s="3" t="s">
-        <v>1399</v>
+        <v>2026013499</v>
+      </c>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="3">
+        <v>4155</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>1400</v>
+        <v>732</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I210" s="3" t="s">
-        <v>1401</v>
-      </c>
-      <c r="J210" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="K210" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L210" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="M210" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="N210" s="3">
-        <v>2405</v>
-      </c>
-      <c r="O210" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="P210" s="10" t="s">
-        <v>1402</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="I210" s="3"/>
+      <c r="J210" s="3"/>
+      <c r="K210" s="3"/>
+      <c r="L210" s="3"/>
+      <c r="M210" s="4"/>
+      <c r="N210" s="3"/>
+      <c r="O210" s="4"/>
+      <c r="P210" s="10"/>
       <c r="Q210" s="3" t="s">
-        <v>1403</v>
+        <v>735</v>
       </c>
       <c r="R210" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S210" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T210" s="3">
         <v>1</v>
@@ -22799,34 +23016,36 @@
         <v>53</v>
       </c>
       <c r="V210" s="3" t="s">
-        <v>1404</v>
+        <v>1396</v>
       </c>
       <c r="W210" s="3" t="s">
-        <v>1405</v>
+        <v>1397</v>
       </c>
       <c r="X210" s="3" t="s">
-        <v>1366</v>
-      </c>
-      <c r="Y210" s="3" t="s">
-        <v>1406</v>
-      </c>
+        <v>1398</v>
+      </c>
+      <c r="Y210" s="3"/>
       <c r="Z210" s="3">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="AA210" s="3"/>
       <c r="AB210" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC210" s="10" t="s">
-        <v>1407</v>
-      </c>
-      <c r="AD210" s="3"/>
+        <v>1399</v>
+      </c>
+      <c r="AD210" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AE210" s="3"/>
       <c r="AF210" s="3"/>
       <c r="AG210" s="3"/>
       <c r="AH210" s="3"/>
       <c r="AI210" s="3"/>
-      <c r="AJ210" s="3"/>
+      <c r="AJ210" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="AK210" s="3" t="s">
         <v>60</v>
       </c>
@@ -22839,25 +23058,25 @@
         <v>38</v>
       </c>
       <c r="C211" s="7">
-        <v>2026013542</v>
+        <v>2026013525</v>
       </c>
       <c r="D211" s="7" t="s">
-        <v>1408</v>
+        <v>1400</v>
       </c>
       <c r="E211" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F211" s="7">
-        <v>4748</v>
+        <v>40</v>
+      </c>
+      <c r="F211" s="7" t="s">
+        <v>1401</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>1409</v>
+        <v>1402</v>
       </c>
       <c r="H211" s="7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="I211" s="7" t="s">
-        <v>1410</v>
+        <v>1403</v>
       </c>
       <c r="J211" s="7" t="s">
         <v>398</v>
@@ -22866,28 +23085,28 @@
         <v>45</v>
       </c>
       <c r="L211" s="7" t="s">
-        <v>46</v>
+        <v>285</v>
       </c>
       <c r="M211" s="8" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="N211" s="7">
-        <v>2305</v>
+        <v>2405</v>
       </c>
       <c r="O211" s="8" t="s">
-        <v>888</v>
+        <v>287</v>
       </c>
       <c r="P211" s="9" t="s">
-        <v>1411</v>
+        <v>1404</v>
       </c>
       <c r="Q211" s="7" t="s">
-        <v>1412</v>
+        <v>1405</v>
       </c>
       <c r="R211" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S211" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T211" s="7">
         <v>1</v>
@@ -22896,26 +23115,26 @@
         <v>53</v>
       </c>
       <c r="V211" s="7" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="W211" s="7" t="s">
-        <v>1414</v>
+        <v>1407</v>
       </c>
       <c r="X211" s="7" t="s">
-        <v>1415</v>
+        <v>1366</v>
       </c>
       <c r="Y211" s="7" t="s">
-        <v>1416</v>
+        <v>1408</v>
       </c>
       <c r="Z211" s="7">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="AA211" s="7"/>
       <c r="AB211" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC211" s="9" t="s">
-        <v>1417</v>
+        <v>1409</v>
       </c>
       <c r="AD211" s="7"/>
       <c r="AE211" s="7"/>
@@ -22933,38 +23152,58 @@
         <v>210</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C212" s="3">
-        <v>2026013586</v>
-      </c>
-      <c r="D212" s="3"/>
-      <c r="E212" s="3"/>
-      <c r="F212" s="3" t="s">
-        <v>1399</v>
+        <v>2026013542</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F212" s="3">
+        <v>4748</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>1400</v>
+        <v>1411</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I212" s="3"/>
-      <c r="J212" s="3"/>
-      <c r="K212" s="3"/>
-      <c r="L212" s="3"/>
-      <c r="M212" s="4"/>
-      <c r="N212" s="3"/>
-      <c r="O212" s="4"/>
-      <c r="P212" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="J212" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K212" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L212" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M212" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N212" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O212" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="P212" s="10" t="s">
+        <v>1413</v>
+      </c>
       <c r="Q212" s="3" t="s">
-        <v>1403</v>
+        <v>1414</v>
       </c>
       <c r="R212" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S212" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="T212" s="3">
         <v>1</v>
@@ -22973,28 +23212,28 @@
         <v>53</v>
       </c>
       <c r="V212" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="W212" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="X212" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="Y212" s="3" t="s">
         <v>1418</v>
       </c>
-      <c r="W212" s="3" t="s">
-        <v>1366</v>
-      </c>
-      <c r="X212" s="3" t="s">
-        <v>1419</v>
-      </c>
-      <c r="Y212" s="3"/>
       <c r="Z212" s="3">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="AA212" s="3"/>
       <c r="AB212" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC212" s="10" t="s">
-        <v>1420</v>
-      </c>
-      <c r="AD212" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>1419</v>
+      </c>
+      <c r="AD212" s="3"/>
       <c r="AE212" s="3"/>
       <c r="AF212" s="3"/>
       <c r="AG212" s="3"/>
@@ -23013,18 +23252,18 @@
         <v>118</v>
       </c>
       <c r="C213" s="7">
-        <v>2026013614</v>
+        <v>2026013586</v>
       </c>
       <c r="D213" s="7"/>
       <c r="E213" s="7"/>
-      <c r="F213" s="7">
-        <v>4748</v>
+      <c r="F213" s="7" t="s">
+        <v>1401</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>1409</v>
+        <v>1402</v>
       </c>
       <c r="H213" s="7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
@@ -23033,15 +23272,15 @@
       <c r="M213" s="8"/>
       <c r="N213" s="7"/>
       <c r="O213" s="8"/>
-      <c r="P213" s="8"/>
+      <c r="P213" s="9"/>
       <c r="Q213" s="7" t="s">
-        <v>1412</v>
+        <v>1405</v>
       </c>
       <c r="R213" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S213" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T213" s="7">
         <v>1</v>
@@ -23050,24 +23289,24 @@
         <v>53</v>
       </c>
       <c r="V213" s="7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="W213" s="7" t="s">
+        <v>1366</v>
+      </c>
+      <c r="X213" s="7" t="s">
         <v>1421</v>
-      </c>
-      <c r="W213" s="7" t="s">
-        <v>1415</v>
-      </c>
-      <c r="X213" s="7" t="s">
-        <v>1422</v>
       </c>
       <c r="Y213" s="7"/>
       <c r="Z213" s="7">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AA213" s="7"/>
       <c r="AB213" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC213" s="8" t="s">
-        <v>1423</v>
+      <c r="AC213" s="9" t="s">
+        <v>1422</v>
       </c>
       <c r="AD213" s="7" t="s">
         <v>60</v>
@@ -23077,10 +23316,990 @@
       <c r="AG213" s="7"/>
       <c r="AH213" s="7"/>
       <c r="AI213" s="7"/>
-      <c r="AJ213" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ213" s="7"/>
       <c r="AK213" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="214" spans="1:37">
+      <c r="A214" s="3">
+        <v>212</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C214" s="3">
+        <v>2026013601</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F214" s="3">
+        <v>2201</v>
+      </c>
+      <c r="G214" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H214" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I214" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="J214" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="K214" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L214" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M214" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="N214" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O214" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="P214" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="Q214" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="R214" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S214" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T214" s="3">
+        <v>1</v>
+      </c>
+      <c r="U214" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V214" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="W214" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="X214" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="Y214" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="Z214" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA214" s="3"/>
+      <c r="AB214" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC214" s="10" t="s">
+        <v>1429</v>
+      </c>
+      <c r="AD214" s="3"/>
+      <c r="AE214" s="3"/>
+      <c r="AF214" s="3"/>
+      <c r="AG214" s="3"/>
+      <c r="AH214" s="3"/>
+      <c r="AI214" s="3"/>
+      <c r="AJ214" s="3"/>
+      <c r="AK214" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="215" spans="1:37">
+      <c r="A215" s="7">
+        <v>213</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C215" s="7">
+        <v>2026013614</v>
+      </c>
+      <c r="D215" s="7"/>
+      <c r="E215" s="7"/>
+      <c r="F215" s="7">
+        <v>4748</v>
+      </c>
+      <c r="G215" s="7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="H215" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I215" s="7"/>
+      <c r="J215" s="7"/>
+      <c r="K215" s="7"/>
+      <c r="L215" s="7"/>
+      <c r="M215" s="8"/>
+      <c r="N215" s="7"/>
+      <c r="O215" s="8"/>
+      <c r="P215" s="9"/>
+      <c r="Q215" s="7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="R215" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S215" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T215" s="7">
+        <v>1</v>
+      </c>
+      <c r="U215" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V215" s="7" t="s">
+        <v>1430</v>
+      </c>
+      <c r="W215" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="X215" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="Y215" s="7"/>
+      <c r="Z215" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA215" s="7"/>
+      <c r="AB215" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC215" s="9" t="s">
+        <v>1432</v>
+      </c>
+      <c r="AD215" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE215" s="7"/>
+      <c r="AF215" s="7"/>
+      <c r="AG215" s="7"/>
+      <c r="AH215" s="7"/>
+      <c r="AI215" s="7"/>
+      <c r="AJ215" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK215" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="216" spans="1:37">
+      <c r="A216" s="3">
+        <v>214</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C216" s="3">
+        <v>2026013673</v>
+      </c>
+      <c r="D216" s="3"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="3">
+        <v>2201</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H216" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I216" s="3"/>
+      <c r="J216" s="3"/>
+      <c r="K216" s="3"/>
+      <c r="L216" s="3"/>
+      <c r="M216" s="4"/>
+      <c r="N216" s="3"/>
+      <c r="O216" s="4"/>
+      <c r="P216" s="10"/>
+      <c r="Q216" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="R216" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S216" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T216" s="3">
+        <v>1</v>
+      </c>
+      <c r="U216" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V216" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="W216" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="X216" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="Y216" s="3"/>
+      <c r="Z216" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA216" s="3"/>
+      <c r="AB216" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC216" s="10" t="s">
+        <v>1435</v>
+      </c>
+      <c r="AD216" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE216" s="3"/>
+      <c r="AF216" s="3"/>
+      <c r="AG216" s="3"/>
+      <c r="AH216" s="3"/>
+      <c r="AI216" s="3"/>
+      <c r="AJ216" s="3"/>
+      <c r="AK216" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="217" spans="1:37">
+      <c r="A217" s="7">
+        <v>215</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C217" s="7">
+        <v>2026013675</v>
+      </c>
+      <c r="D217" s="7" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E217" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F217" s="7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G217" s="7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H217" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I217" s="7" t="s">
+        <v>1437</v>
+      </c>
+      <c r="J217" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="K217" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L217" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="M217" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="N217" s="7">
+        <v>6003</v>
+      </c>
+      <c r="O217" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="P217" s="9" t="s">
+        <v>1438</v>
+      </c>
+      <c r="Q217" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="R217" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S217" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T217" s="7">
+        <v>1</v>
+      </c>
+      <c r="U217" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V217" s="7" t="s">
+        <v>1439</v>
+      </c>
+      <c r="W217" s="7" t="s">
+        <v>1440</v>
+      </c>
+      <c r="X217" s="7" t="s">
+        <v>1441</v>
+      </c>
+      <c r="Y217" s="7" t="s">
+        <v>1442</v>
+      </c>
+      <c r="Z217" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA217" s="7"/>
+      <c r="AB217" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC217" s="9" t="s">
+        <v>1443</v>
+      </c>
+      <c r="AD217" s="7"/>
+      <c r="AE217" s="7"/>
+      <c r="AF217" s="7"/>
+      <c r="AG217" s="7"/>
+      <c r="AH217" s="7"/>
+      <c r="AI217" s="7"/>
+      <c r="AJ217" s="7"/>
+      <c r="AK217" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="218" spans="1:37">
+      <c r="A218" s="3">
+        <v>216</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C218" s="3">
+        <v>2026013699</v>
+      </c>
+      <c r="D218" s="3"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3">
+        <v>4005</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="H218" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I218" s="3"/>
+      <c r="J218" s="3"/>
+      <c r="K218" s="3"/>
+      <c r="L218" s="3"/>
+      <c r="M218" s="4"/>
+      <c r="N218" s="3"/>
+      <c r="O218" s="4"/>
+      <c r="P218" s="10"/>
+      <c r="Q218" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="R218" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S218" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T218" s="3">
+        <v>1</v>
+      </c>
+      <c r="U218" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V218" s="3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="W218" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="X218" s="3" t="s">
+        <v>1448</v>
+      </c>
+      <c r="Y218" s="3"/>
+      <c r="Z218" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA218" s="3"/>
+      <c r="AB218" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC218" s="10" t="s">
+        <v>1449</v>
+      </c>
+      <c r="AD218" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE218" s="3"/>
+      <c r="AF218" s="3"/>
+      <c r="AG218" s="3"/>
+      <c r="AH218" s="3"/>
+      <c r="AI218" s="3"/>
+      <c r="AJ218" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK218" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="219" spans="1:37">
+      <c r="A219" s="7">
+        <v>217</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C219" s="7">
+        <v>2026013703</v>
+      </c>
+      <c r="D219" s="7"/>
+      <c r="E219" s="7"/>
+      <c r="F219" s="7" t="s">
+        <v>1450</v>
+      </c>
+      <c r="G219" s="7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="H219" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I219" s="7"/>
+      <c r="J219" s="7"/>
+      <c r="K219" s="7"/>
+      <c r="L219" s="7"/>
+      <c r="M219" s="8"/>
+      <c r="N219" s="7"/>
+      <c r="O219" s="8"/>
+      <c r="P219" s="9"/>
+      <c r="Q219" s="7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="R219" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S219" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T219" s="7">
+        <v>1</v>
+      </c>
+      <c r="U219" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V219" s="7" t="s">
+        <v>1453</v>
+      </c>
+      <c r="W219" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="X219" s="7" t="s">
+        <v>1455</v>
+      </c>
+      <c r="Y219" s="7"/>
+      <c r="Z219" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA219" s="7"/>
+      <c r="AB219" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC219" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD219" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE219" s="7"/>
+      <c r="AF219" s="7"/>
+      <c r="AG219" s="7"/>
+      <c r="AH219" s="7"/>
+      <c r="AI219" s="7"/>
+      <c r="AJ219" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK219" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="220" spans="1:37">
+      <c r="A220" s="3">
+        <v>218</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C220" s="3">
+        <v>2026013708</v>
+      </c>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H220" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I220" s="3"/>
+      <c r="J220" s="3"/>
+      <c r="K220" s="3"/>
+      <c r="L220" s="3"/>
+      <c r="M220" s="4"/>
+      <c r="N220" s="3"/>
+      <c r="O220" s="4"/>
+      <c r="P220" s="10"/>
+      <c r="Q220" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="R220" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S220" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T220" s="3">
+        <v>1</v>
+      </c>
+      <c r="U220" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V220" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="W220" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="X220" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="Y220" s="3"/>
+      <c r="Z220" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA220" s="3"/>
+      <c r="AB220" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC220" s="10" t="s">
+        <v>1462</v>
+      </c>
+      <c r="AD220" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE220" s="3"/>
+      <c r="AF220" s="3"/>
+      <c r="AG220" s="3"/>
+      <c r="AH220" s="3"/>
+      <c r="AI220" s="3"/>
+      <c r="AJ220" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK220" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="221" spans="1:37">
+      <c r="A221" s="7">
+        <v>219</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C221" s="7">
+        <v>2026013712</v>
+      </c>
+      <c r="D221" s="7"/>
+      <c r="E221" s="7"/>
+      <c r="F221" s="7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G221" s="7" t="s">
+        <v>1464</v>
+      </c>
+      <c r="H221" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I221" s="7"/>
+      <c r="J221" s="7"/>
+      <c r="K221" s="7"/>
+      <c r="L221" s="7"/>
+      <c r="M221" s="8"/>
+      <c r="N221" s="7"/>
+      <c r="O221" s="8"/>
+      <c r="P221" s="9"/>
+      <c r="Q221" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="R221" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S221" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T221" s="7">
+        <v>1</v>
+      </c>
+      <c r="U221" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V221" s="7" t="s">
+        <v>1466</v>
+      </c>
+      <c r="W221" s="7" t="s">
+        <v>1467</v>
+      </c>
+      <c r="X221" s="7" t="s">
+        <v>1468</v>
+      </c>
+      <c r="Y221" s="7"/>
+      <c r="Z221" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA221" s="7"/>
+      <c r="AB221" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC221" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD221" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE221" s="7"/>
+      <c r="AF221" s="7"/>
+      <c r="AG221" s="7"/>
+      <c r="AH221" s="7"/>
+      <c r="AI221" s="7"/>
+      <c r="AJ221" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK221" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="222" spans="1:37">
+      <c r="A222" s="3">
+        <v>220</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C222" s="3">
+        <v>2026013807</v>
+      </c>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H222" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I222" s="3"/>
+      <c r="J222" s="3"/>
+      <c r="K222" s="3"/>
+      <c r="L222" s="3"/>
+      <c r="M222" s="4"/>
+      <c r="N222" s="3"/>
+      <c r="O222" s="4"/>
+      <c r="P222" s="10"/>
+      <c r="Q222" s="3" t="s">
+        <v>1471</v>
+      </c>
+      <c r="R222" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S222" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T222" s="3">
+        <v>1</v>
+      </c>
+      <c r="U222" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V222" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="W222" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="X222" s="3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="Y222" s="3"/>
+      <c r="Z222" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA222" s="3"/>
+      <c r="AB222" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC222" s="10" t="s">
+        <v>1475</v>
+      </c>
+      <c r="AD222" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE222" s="3"/>
+      <c r="AF222" s="3"/>
+      <c r="AG222" s="3"/>
+      <c r="AH222" s="3"/>
+      <c r="AI222" s="3"/>
+      <c r="AJ222" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK222" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="223" spans="1:37">
+      <c r="A223" s="7">
+        <v>221</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C223" s="7">
+        <v>2026013810</v>
+      </c>
+      <c r="D223" s="7"/>
+      <c r="E223" s="7"/>
+      <c r="F223" s="7">
+        <v>4977</v>
+      </c>
+      <c r="G223" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="H223" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I223" s="7"/>
+      <c r="J223" s="7"/>
+      <c r="K223" s="7"/>
+      <c r="L223" s="7"/>
+      <c r="M223" s="8"/>
+      <c r="N223" s="7"/>
+      <c r="O223" s="8"/>
+      <c r="P223" s="9"/>
+      <c r="Q223" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="R223" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S223" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T223" s="7">
+        <v>1</v>
+      </c>
+      <c r="U223" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V223" s="7" t="s">
+        <v>1478</v>
+      </c>
+      <c r="W223" s="7" t="s">
+        <v>1479</v>
+      </c>
+      <c r="X223" s="7" t="s">
+        <v>1480</v>
+      </c>
+      <c r="Y223" s="7"/>
+      <c r="Z223" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA223" s="7"/>
+      <c r="AB223" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC223" s="9" t="s">
+        <v>1481</v>
+      </c>
+      <c r="AD223" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE223" s="7"/>
+      <c r="AF223" s="7"/>
+      <c r="AG223" s="7"/>
+      <c r="AH223" s="7"/>
+      <c r="AI223" s="7"/>
+      <c r="AJ223" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK223" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="224" spans="1:37">
+      <c r="A224" s="3">
+        <v>222</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C224" s="3">
+        <v>2026013821</v>
+      </c>
+      <c r="D224" s="3"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="3" t="s">
+        <v>1482</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="H224" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I224" s="3"/>
+      <c r="J224" s="3"/>
+      <c r="K224" s="3"/>
+      <c r="L224" s="3"/>
+      <c r="M224" s="4"/>
+      <c r="N224" s="3"/>
+      <c r="O224" s="4"/>
+      <c r="P224" s="10"/>
+      <c r="Q224" s="3" t="s">
+        <v>1484</v>
+      </c>
+      <c r="R224" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S224" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T224" s="3">
+        <v>1</v>
+      </c>
+      <c r="U224" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V224" s="3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="W224" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="X224" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="Y224" s="3"/>
+      <c r="Z224" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA224" s="3"/>
+      <c r="AB224" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC224" s="10" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AD224" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE224" s="3"/>
+      <c r="AF224" s="3"/>
+      <c r="AG224" s="3"/>
+      <c r="AH224" s="3"/>
+      <c r="AI224" s="3"/>
+      <c r="AJ224" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK224" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="225" spans="1:37">
+      <c r="A225" s="7">
+        <v>223</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C225" s="7">
+        <v>2026013851</v>
+      </c>
+      <c r="D225" s="7"/>
+      <c r="E225" s="7"/>
+      <c r="F225" s="7" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G225" s="7" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H225" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I225" s="7"/>
+      <c r="J225" s="7"/>
+      <c r="K225" s="7"/>
+      <c r="L225" s="7"/>
+      <c r="M225" s="8"/>
+      <c r="N225" s="7"/>
+      <c r="O225" s="8"/>
+      <c r="P225" s="8"/>
+      <c r="Q225" s="7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="R225" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S225" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T225" s="7">
+        <v>1</v>
+      </c>
+      <c r="U225" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V225" s="7" t="s">
+        <v>1492</v>
+      </c>
+      <c r="W225" s="7" t="s">
+        <v>1493</v>
+      </c>
+      <c r="X225" s="7" t="s">
+        <v>1494</v>
+      </c>
+      <c r="Y225" s="7"/>
+      <c r="Z225" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA225" s="7"/>
+      <c r="AB225" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC225" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD225" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE225" s="7"/>
+      <c r="AF225" s="7"/>
+      <c r="AG225" s="7"/>
+      <c r="AH225" s="7"/>
+      <c r="AI225" s="7"/>
+      <c r="AJ225" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK225" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 01291846
</commit_message>
<xml_diff>
--- a/IM/202601_HL_Maintain_Report.xlsx
+++ b/IM/202601_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$225</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$229</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1521">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202601   (  製表日期:2026-01-29  )</t>
   </si>
@@ -4532,6 +4532,32 @@
     <t>2026-01-28 12:16:00</t>
   </si>
   <si>
+    <t>E4715115012901</t>
+  </si>
+  <si>
+    <t>2026-01-29 10:20:38</t>
+  </si>
+  <si>
+    <t>門市反應mmk熱感機(T70II)無反應無法出紙查看ERROR亮紅燈，門市已有重裝紙捲重開機仍異常....須請台芝到店協助(無法出紙)</t>
+  </si>
+  <si>
+    <t>2026-01-29 10:30:02</t>
+  </si>
+  <si>
+    <t>2026-01-29 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 15:55:00</t>
+  </si>
+  <si>
+    <t>2026-01-30 14:30:00</t>
+  </si>
+  <si>
+    <t>更換出單機
+換下8138002421
+換上8138001797</t>
+  </si>
+  <si>
     <t>D191</t>
   </si>
   <si>
@@ -4608,6 +4634,60 @@
   </si>
   <si>
     <t>2026-01-29 13:30:00</t>
+  </si>
+  <si>
+    <t>新莊國家置地</t>
+  </si>
+  <si>
+    <t>THILF05291</t>
+  </si>
+  <si>
+    <t>2026-01-29 14:01:43</t>
+  </si>
+  <si>
+    <t>2026-01-29 14:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003070</t>
+  </si>
+  <si>
+    <t>三重頂崁店</t>
+  </si>
+  <si>
+    <t>THILF04698</t>
+  </si>
+  <si>
+    <t>2026-01-29 16:09:25</t>
+  </si>
+  <si>
+    <t>2026-01-29 15:40:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 16:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002806</t>
+  </si>
+  <si>
+    <t>D138</t>
+  </si>
+  <si>
+    <t>三重中興北二</t>
+  </si>
+  <si>
+    <t>THILF0D138</t>
+  </si>
+  <si>
+    <t>2026-01-29 16:46:18</t>
+  </si>
+  <si>
+    <t>2026-01-29 16:10:00</t>
+  </si>
+  <si>
+    <t>2026-01-29 16:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002819</t>
   </si>
 </sst>
 </file>
@@ -5021,10 +5101,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK225"/>
+  <dimension ref="A1:AK229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A225" sqref="A225"/>
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23992,38 +24072,58 @@
         <v>220</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C222" s="3">
-        <v>2026013807</v>
-      </c>
-      <c r="D222" s="3"/>
-      <c r="E222" s="3"/>
-      <c r="F222" s="3" t="s">
+        <v>2026013800</v>
+      </c>
+      <c r="D222" s="3" t="s">
         <v>1469</v>
       </c>
+      <c r="E222" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F222" s="3">
+        <v>4715</v>
+      </c>
       <c r="G222" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="H222" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="I222" s="3" t="s">
         <v>1470</v>
       </c>
-      <c r="H222" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I222" s="3"/>
-      <c r="J222" s="3"/>
-      <c r="K222" s="3"/>
-      <c r="L222" s="3"/>
-      <c r="M222" s="4"/>
-      <c r="N222" s="3"/>
-      <c r="O222" s="4"/>
-      <c r="P222" s="10"/>
+      <c r="J222" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K222" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L222" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M222" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="N222" s="3">
+        <v>5901</v>
+      </c>
+      <c r="O222" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P222" s="10" t="s">
+        <v>1471</v>
+      </c>
       <c r="Q222" s="3" t="s">
-        <v>1471</v>
+        <v>543</v>
       </c>
       <c r="R222" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S222" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="T222" s="3">
         <v>1</v>
@@ -24040,28 +24140,26 @@
       <c r="X222" s="3" t="s">
         <v>1474</v>
       </c>
-      <c r="Y222" s="3"/>
+      <c r="Y222" s="3" t="s">
+        <v>1475</v>
+      </c>
       <c r="Z222" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AA222" s="3"/>
       <c r="AB222" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC222" s="10" t="s">
-        <v>1475</v>
-      </c>
-      <c r="AD222" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>1476</v>
+      </c>
+      <c r="AD222" s="3"/>
       <c r="AE222" s="3"/>
       <c r="AF222" s="3"/>
       <c r="AG222" s="3"/>
       <c r="AH222" s="3"/>
       <c r="AI222" s="3"/>
-      <c r="AJ222" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ222" s="3"/>
       <c r="AK222" s="3" t="s">
         <v>60</v>
       </c>
@@ -24074,15 +24172,15 @@
         <v>118</v>
       </c>
       <c r="C223" s="7">
-        <v>2026013810</v>
+        <v>2026013807</v>
       </c>
       <c r="D223" s="7"/>
       <c r="E223" s="7"/>
-      <c r="F223" s="7">
-        <v>4977</v>
+      <c r="F223" s="7" t="s">
+        <v>1477</v>
       </c>
       <c r="G223" s="7" t="s">
-        <v>1476</v>
+        <v>1478</v>
       </c>
       <c r="H223" s="7" t="s">
         <v>92</v>
@@ -24096,7 +24194,7 @@
       <c r="O223" s="8"/>
       <c r="P223" s="9"/>
       <c r="Q223" s="7" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
       <c r="R223" s="7" t="s">
         <v>51</v>
@@ -24111,13 +24209,13 @@
         <v>53</v>
       </c>
       <c r="V223" s="7" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
       <c r="W223" s="7" t="s">
-        <v>1479</v>
+        <v>1481</v>
       </c>
       <c r="X223" s="7" t="s">
-        <v>1480</v>
+        <v>1482</v>
       </c>
       <c r="Y223" s="7"/>
       <c r="Z223" s="7">
@@ -24128,7 +24226,7 @@
         <v>58</v>
       </c>
       <c r="AC223" s="9" t="s">
-        <v>1481</v>
+        <v>1483</v>
       </c>
       <c r="AD223" s="7" t="s">
         <v>60</v>
@@ -24153,15 +24251,15 @@
         <v>118</v>
       </c>
       <c r="C224" s="3">
-        <v>2026013821</v>
+        <v>2026013810</v>
       </c>
       <c r="D224" s="3"/>
       <c r="E224" s="3"/>
-      <c r="F224" s="3" t="s">
-        <v>1482</v>
+      <c r="F224" s="3">
+        <v>4977</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="H224" s="3" t="s">
         <v>92</v>
@@ -24175,7 +24273,7 @@
       <c r="O224" s="4"/>
       <c r="P224" s="10"/>
       <c r="Q224" s="3" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="R224" s="3" t="s">
         <v>51</v>
@@ -24190,13 +24288,13 @@
         <v>53</v>
       </c>
       <c r="V224" s="3" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="W224" s="3" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="X224" s="3" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="Y224" s="3"/>
       <c r="Z224" s="3">
@@ -24207,7 +24305,7 @@
         <v>58</v>
       </c>
       <c r="AC224" s="10" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="AD224" s="3" t="s">
         <v>60</v>
@@ -24232,18 +24330,18 @@
         <v>118</v>
       </c>
       <c r="C225" s="7">
-        <v>2026013851</v>
+        <v>2026013821</v>
       </c>
       <c r="D225" s="7"/>
       <c r="E225" s="7"/>
       <c r="F225" s="7" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="H225" s="7" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="I225" s="7"/>
       <c r="J225" s="7"/>
@@ -24252,15 +24350,15 @@
       <c r="M225" s="8"/>
       <c r="N225" s="7"/>
       <c r="O225" s="8"/>
-      <c r="P225" s="8"/>
+      <c r="P225" s="9"/>
       <c r="Q225" s="7" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="R225" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S225" s="7" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="T225" s="7">
         <v>1</v>
@@ -24269,24 +24367,24 @@
         <v>53</v>
       </c>
       <c r="V225" s="7" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="W225" s="7" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="X225" s="7" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="Y225" s="7"/>
       <c r="Z225" s="7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA225" s="7"/>
       <c r="AB225" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC225" s="8" t="s">
-        <v>510</v>
+      <c r="AC225" s="9" t="s">
+        <v>1496</v>
       </c>
       <c r="AD225" s="7" t="s">
         <v>60</v>
@@ -24300,6 +24398,322 @@
         <v>60</v>
       </c>
       <c r="AK225" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="226" spans="1:37">
+      <c r="A226" s="3">
+        <v>224</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C226" s="3">
+        <v>2026013851</v>
+      </c>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>1498</v>
+      </c>
+      <c r="H226" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I226" s="3"/>
+      <c r="J226" s="3"/>
+      <c r="K226" s="3"/>
+      <c r="L226" s="3"/>
+      <c r="M226" s="4"/>
+      <c r="N226" s="3"/>
+      <c r="O226" s="4"/>
+      <c r="P226" s="10"/>
+      <c r="Q226" s="3" t="s">
+        <v>1499</v>
+      </c>
+      <c r="R226" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S226" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T226" s="3">
+        <v>1</v>
+      </c>
+      <c r="U226" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V226" s="3" t="s">
+        <v>1500</v>
+      </c>
+      <c r="W226" s="3" t="s">
+        <v>1501</v>
+      </c>
+      <c r="X226" s="3" t="s">
+        <v>1502</v>
+      </c>
+      <c r="Y226" s="3"/>
+      <c r="Z226" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA226" s="3"/>
+      <c r="AB226" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC226" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD226" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE226" s="3"/>
+      <c r="AF226" s="3"/>
+      <c r="AG226" s="3"/>
+      <c r="AH226" s="3"/>
+      <c r="AI226" s="3"/>
+      <c r="AJ226" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK226" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="227" spans="1:37">
+      <c r="A227" s="7">
+        <v>225</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C227" s="7">
+        <v>2026013863</v>
+      </c>
+      <c r="D227" s="7"/>
+      <c r="E227" s="7"/>
+      <c r="F227" s="7">
+        <v>5291</v>
+      </c>
+      <c r="G227" s="7" t="s">
+        <v>1503</v>
+      </c>
+      <c r="H227" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I227" s="7"/>
+      <c r="J227" s="7"/>
+      <c r="K227" s="7"/>
+      <c r="L227" s="7"/>
+      <c r="M227" s="8"/>
+      <c r="N227" s="7"/>
+      <c r="O227" s="8"/>
+      <c r="P227" s="9"/>
+      <c r="Q227" s="7" t="s">
+        <v>1504</v>
+      </c>
+      <c r="R227" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S227" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T227" s="7">
+        <v>1</v>
+      </c>
+      <c r="U227" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V227" s="7" t="s">
+        <v>1505</v>
+      </c>
+      <c r="W227" s="7" t="s">
+        <v>1502</v>
+      </c>
+      <c r="X227" s="7" t="s">
+        <v>1506</v>
+      </c>
+      <c r="Y227" s="7"/>
+      <c r="Z227" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA227" s="7"/>
+      <c r="AB227" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC227" s="9" t="s">
+        <v>1507</v>
+      </c>
+      <c r="AD227" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE227" s="7"/>
+      <c r="AF227" s="7"/>
+      <c r="AG227" s="7"/>
+      <c r="AH227" s="7"/>
+      <c r="AI227" s="7"/>
+      <c r="AJ227" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK227" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="228" spans="1:37">
+      <c r="A228" s="3">
+        <v>226</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C228" s="3">
+        <v>2026013887</v>
+      </c>
+      <c r="D228" s="3"/>
+      <c r="E228" s="3"/>
+      <c r="F228" s="3">
+        <v>4698</v>
+      </c>
+      <c r="G228" s="3" t="s">
+        <v>1508</v>
+      </c>
+      <c r="H228" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I228" s="3"/>
+      <c r="J228" s="3"/>
+      <c r="K228" s="3"/>
+      <c r="L228" s="3"/>
+      <c r="M228" s="4"/>
+      <c r="N228" s="3"/>
+      <c r="O228" s="4"/>
+      <c r="P228" s="10"/>
+      <c r="Q228" s="3" t="s">
+        <v>1509</v>
+      </c>
+      <c r="R228" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S228" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="T228" s="3">
+        <v>1</v>
+      </c>
+      <c r="U228" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V228" s="3" t="s">
+        <v>1510</v>
+      </c>
+      <c r="W228" s="3" t="s">
+        <v>1511</v>
+      </c>
+      <c r="X228" s="3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="Y228" s="3"/>
+      <c r="Z228" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA228" s="3"/>
+      <c r="AB228" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC228" s="10" t="s">
+        <v>1513</v>
+      </c>
+      <c r="AD228" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE228" s="3"/>
+      <c r="AF228" s="3"/>
+      <c r="AG228" s="3"/>
+      <c r="AH228" s="3"/>
+      <c r="AI228" s="3"/>
+      <c r="AJ228" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK228" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="229" spans="1:37">
+      <c r="A229" s="7">
+        <v>227</v>
+      </c>
+      <c r="B229" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C229" s="7">
+        <v>2026013929</v>
+      </c>
+      <c r="D229" s="7"/>
+      <c r="E229" s="7"/>
+      <c r="F229" s="7" t="s">
+        <v>1514</v>
+      </c>
+      <c r="G229" s="7" t="s">
+        <v>1515</v>
+      </c>
+      <c r="H229" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I229" s="7"/>
+      <c r="J229" s="7"/>
+      <c r="K229" s="7"/>
+      <c r="L229" s="7"/>
+      <c r="M229" s="8"/>
+      <c r="N229" s="7"/>
+      <c r="O229" s="8"/>
+      <c r="P229" s="8"/>
+      <c r="Q229" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="R229" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S229" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T229" s="7">
+        <v>1</v>
+      </c>
+      <c r="U229" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V229" s="7" t="s">
+        <v>1517</v>
+      </c>
+      <c r="W229" s="7" t="s">
+        <v>1518</v>
+      </c>
+      <c r="X229" s="7" t="s">
+        <v>1519</v>
+      </c>
+      <c r="Y229" s="7"/>
+      <c r="Z229" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA229" s="7"/>
+      <c r="AB229" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC229" s="8" t="s">
+        <v>1520</v>
+      </c>
+      <c r="AD229" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE229" s="7"/>
+      <c r="AF229" s="7"/>
+      <c r="AG229" s="7"/>
+      <c r="AH229" s="7"/>
+      <c r="AI229" s="7"/>
+      <c r="AJ229" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK229" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>